<commit_message>
Create genetic algorithm for all functions
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="10">
   <si>
     <t>Rastrigin</t>
   </si>
@@ -46,12 +46,21 @@
   <si>
     <t>AVG</t>
   </si>
+  <si>
+    <t>Generations = 200</t>
+  </si>
+  <si>
+    <t>Algoritm Genetic [pop_size=50,crossover_pbb=0.4,mutation_pbb=0.1]</t>
+  </si>
+  <si>
+    <t>12.258187238.352997533613895908</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -62,6 +71,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -201,8 +217,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -215,15 +241,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -538,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N34"/>
+  <dimension ref="A1:N72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="N74" sqref="N74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -550,75 +567,75 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="1" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="1" t="s">
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="3" t="s">
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="4"/>
+      <c r="N1" s="14"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="1">
         <v>5</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="1">
         <v>10</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="2">
         <v>30</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="1">
         <v>5</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="1">
         <v>10</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="2">
         <v>30</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="5">
+      <c r="J2" s="1">
         <v>5</v>
       </c>
-      <c r="K2" s="5">
+      <c r="K2" s="1">
         <v>10</v>
       </c>
-      <c r="L2" s="6">
+      <c r="L2" s="2">
         <v>30</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N2" s="6">
+      <c r="N2" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="7">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
       <c r="B3">
@@ -627,10 +644,10 @@
       <c r="C3">
         <v>41.625392539811898</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="4">
         <v>72.694345070178201</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="3">
         <v>1</v>
       </c>
       <c r="F3">
@@ -639,10 +656,10 @@
       <c r="G3">
         <v>0.73338771056778695</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="4">
         <v>12.3015506785339</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="3">
         <v>1</v>
       </c>
       <c r="J3">
@@ -651,18 +668,18 @@
       <c r="K3">
         <v>9.7693796323807103</v>
       </c>
-      <c r="L3" s="8">
+      <c r="L3" s="4">
         <v>223.878376888921</v>
       </c>
-      <c r="M3" s="7">
+      <c r="M3" s="3">
         <v>1</v>
       </c>
-      <c r="N3" s="8">
+      <c r="N3" s="4">
         <v>-0.97056248757917196</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="9">
+      <c r="A4" s="5">
         <v>2</v>
       </c>
       <c r="B4">
@@ -671,10 +688,10 @@
       <c r="C4">
         <v>37.379163799111403</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="4">
         <v>80.3988262137878</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="5">
         <v>2</v>
       </c>
       <c r="F4">
@@ -683,10 +700,10 @@
       <c r="G4">
         <v>0.236008203306348</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="4">
         <v>29.48536102764</v>
       </c>
-      <c r="I4" s="9">
+      <c r="I4" s="5">
         <v>2</v>
       </c>
       <c r="J4">
@@ -695,18 +712,18 @@
       <c r="K4">
         <v>43.988991884964904</v>
       </c>
-      <c r="L4" s="8">
+      <c r="L4" s="4">
         <v>120.90520157828701</v>
       </c>
-      <c r="M4" s="9">
+      <c r="M4" s="5">
         <v>2</v>
       </c>
-      <c r="N4" s="8">
+      <c r="N4" s="4">
         <v>-0.74784721613453697</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="9">
+      <c r="A5" s="5">
         <v>3</v>
       </c>
       <c r="B5">
@@ -715,10 +732,10 @@
       <c r="C5">
         <v>37.955841317153897</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="4">
         <v>99.548387608353906</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="5">
         <v>3</v>
       </c>
       <c r="F5">
@@ -727,10 +744,10 @@
       <c r="G5">
         <v>0.12753554718855301</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="4">
         <v>69.129377946871799</v>
       </c>
-      <c r="I5" s="9">
+      <c r="I5" s="5">
         <v>3</v>
       </c>
       <c r="J5">
@@ -739,18 +756,18 @@
       <c r="K5">
         <v>9.2695646244667795</v>
       </c>
-      <c r="L5" s="8">
+      <c r="L5" s="4">
         <v>30.5991367402554</v>
       </c>
-      <c r="M5" s="9">
+      <c r="M5" s="5">
         <v>3</v>
       </c>
-      <c r="N5" s="8">
+      <c r="N5" s="4">
         <v>-0.982009523598117</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="9">
+      <c r="A6" s="5">
         <v>4</v>
       </c>
       <c r="B6">
@@ -759,10 +776,10 @@
       <c r="C6">
         <v>30.907246552514401</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="4">
         <v>95.460653679338094</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="5">
         <v>4</v>
       </c>
       <c r="F6">
@@ -771,10 +788,10 @@
       <c r="G6">
         <v>0.124014529256199</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="4">
         <v>42.582997751472398</v>
       </c>
-      <c r="I6" s="9">
+      <c r="I6" s="5">
         <v>4</v>
       </c>
       <c r="J6">
@@ -783,18 +800,18 @@
       <c r="K6">
         <v>80.186822877134503</v>
       </c>
-      <c r="L6" s="8">
+      <c r="L6" s="4">
         <v>334.07149291160403</v>
       </c>
-      <c r="M6" s="9">
+      <c r="M6" s="5">
         <v>4</v>
       </c>
-      <c r="N6" s="8">
+      <c r="N6" s="4">
         <v>-0.99367355496180698</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="9">
+      <c r="A7" s="5">
         <v>5</v>
       </c>
       <c r="B7">
@@ -803,10 +820,10 @@
       <c r="C7">
         <v>38.642829298938203</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="4">
         <v>92.630272820748203</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="5">
         <v>5</v>
       </c>
       <c r="F7">
@@ -815,10 +832,10 @@
       <c r="G7">
         <v>0.61589754975288502</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="4">
         <v>89.624175910353998</v>
       </c>
-      <c r="I7" s="9">
+      <c r="I7" s="5">
         <v>5</v>
       </c>
       <c r="J7">
@@ -827,18 +844,18 @@
       <c r="K7">
         <v>9.5565332445514901</v>
       </c>
-      <c r="L7" s="8">
+      <c r="L7" s="4">
         <v>147.02434859809699</v>
       </c>
-      <c r="M7" s="9">
+      <c r="M7" s="5">
         <v>5</v>
       </c>
-      <c r="N7" s="8">
+      <c r="N7" s="4">
         <v>-1.02992784328481</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="9">
+      <c r="A8" s="5">
         <v>6</v>
       </c>
       <c r="B8">
@@ -847,10 +864,10 @@
       <c r="C8">
         <v>19.425474887182901</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="4">
         <v>86.803435407027493</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="5">
         <v>6</v>
       </c>
       <c r="F8">
@@ -859,10 +876,10 @@
       <c r="G8">
         <v>8.4329768999114693E-2</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="4">
         <v>20.427679638213299</v>
       </c>
-      <c r="I8" s="9">
+      <c r="I8" s="5">
         <v>6</v>
       </c>
       <c r="J8">
@@ -871,18 +888,18 @@
       <c r="K8">
         <v>9.4997117710254706</v>
       </c>
-      <c r="L8" s="8">
+      <c r="L8" s="4">
         <v>107.66187868150099</v>
       </c>
-      <c r="M8" s="9">
+      <c r="M8" s="5">
         <v>6</v>
       </c>
-      <c r="N8" s="8">
+      <c r="N8" s="4">
         <v>-0.97056248757917196</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="9">
+      <c r="A9" s="5">
         <v>7</v>
       </c>
       <c r="B9">
@@ -891,10 +908,10 @@
       <c r="C9">
         <v>32.710594415949103</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="4">
         <v>73.196189587359797</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="5">
         <v>7</v>
       </c>
       <c r="F9">
@@ -903,10 +920,10 @@
       <c r="G9">
         <v>0.43252233722050398</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="4">
         <v>79.625706689441898</v>
       </c>
-      <c r="I9" s="9">
+      <c r="I9" s="5">
         <v>7</v>
       </c>
       <c r="J9">
@@ -915,18 +932,18 @@
       <c r="K9">
         <v>9.3179258260962392</v>
       </c>
-      <c r="L9" s="8">
+      <c r="L9" s="4">
         <v>174.35203380866699</v>
       </c>
-      <c r="M9" s="9">
+      <c r="M9" s="5">
         <v>7</v>
       </c>
-      <c r="N9" s="8">
+      <c r="N9" s="4">
         <v>-0.99550048954989001</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="9">
+      <c r="A10" s="5">
         <v>8</v>
       </c>
       <c r="B10">
@@ -935,10 +952,10 @@
       <c r="C10">
         <v>39.085974533368201</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="4">
         <v>116.31154846523999</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="5">
         <v>8</v>
       </c>
       <c r="F10">
@@ -947,10 +964,10 @@
       <c r="G10">
         <v>3.4586741408044602E-2</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="4">
         <v>76.218367758141198</v>
       </c>
-      <c r="I10" s="9">
+      <c r="I10" s="5">
         <v>8</v>
       </c>
       <c r="J10">
@@ -959,18 +976,18 @@
       <c r="K10">
         <v>12.476467959612499</v>
       </c>
-      <c r="L10" s="8">
+      <c r="L10" s="4">
         <v>128.579936587433</v>
       </c>
-      <c r="M10" s="9">
+      <c r="M10" s="5">
         <v>8</v>
       </c>
-      <c r="N10" s="8">
+      <c r="N10" s="4">
         <v>-0.94272473854657801</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="9">
+      <c r="A11" s="5">
         <v>9</v>
       </c>
       <c r="B11">
@@ -979,10 +996,10 @@
       <c r="C11">
         <v>18.884953936332199</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="4">
         <v>82.833886758419993</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="5">
         <v>9</v>
       </c>
       <c r="F11">
@@ -991,10 +1008,10 @@
       <c r="G11">
         <v>0.14445298711957699</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H11" s="4">
         <v>9.2560933733062694</v>
       </c>
-      <c r="I11" s="9">
+      <c r="I11" s="5">
         <v>9</v>
       </c>
       <c r="J11">
@@ -1003,18 +1020,18 @@
       <c r="K11">
         <v>88.243817799357004</v>
       </c>
-      <c r="L11" s="8">
+      <c r="L11" s="4">
         <v>177.914156779222</v>
       </c>
-      <c r="M11" s="9">
+      <c r="M11" s="5">
         <v>9</v>
       </c>
-      <c r="N11" s="8">
+      <c r="N11" s="4">
         <v>-0.99511469963927401</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="9">
+      <c r="A12" s="5">
         <v>10</v>
       </c>
       <c r="B12">
@@ -1023,10 +1040,10 @@
       <c r="C12">
         <v>33.836703767683801</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="4">
         <v>88.569592716591401</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="5">
         <v>10</v>
       </c>
       <c r="F12">
@@ -1035,10 +1052,10 @@
       <c r="G12">
         <v>0.115608343352923</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H12" s="4">
         <v>14.9191715020589</v>
       </c>
-      <c r="I12" s="9">
+      <c r="I12" s="5">
         <v>10</v>
       </c>
       <c r="J12">
@@ -1047,18 +1064,18 @@
       <c r="K12">
         <v>9.8642539026375999</v>
       </c>
-      <c r="L12" s="8">
+      <c r="L12" s="4">
         <v>221.96364507235501</v>
       </c>
-      <c r="M12" s="9">
+      <c r="M12" s="5">
         <v>10</v>
       </c>
-      <c r="N12" s="8">
+      <c r="N12" s="4">
         <v>-1.0241175434207299</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="9">
+      <c r="A13" s="5">
         <v>11</v>
       </c>
       <c r="B13">
@@ -1067,10 +1084,10 @@
       <c r="C13">
         <v>18.895847896212398</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="4">
         <v>110.688413536537</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="5">
         <v>11</v>
       </c>
       <c r="F13">
@@ -1079,10 +1096,10 @@
       <c r="G13">
         <v>0.11830958392309</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H13" s="4">
         <v>53.437324963723299</v>
       </c>
-      <c r="I13" s="9">
+      <c r="I13" s="5">
         <v>11</v>
       </c>
       <c r="J13">
@@ -1091,18 +1108,18 @@
       <c r="K13">
         <v>79.259030786125294</v>
       </c>
-      <c r="L13" s="8">
+      <c r="L13" s="4">
         <v>347.89857906466602</v>
       </c>
-      <c r="M13" s="9">
+      <c r="M13" s="5">
         <v>11</v>
       </c>
-      <c r="N13" s="8">
+      <c r="N13" s="4">
         <v>-0.99550048954989001</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="9">
+      <c r="A14" s="5">
         <v>12</v>
       </c>
       <c r="B14">
@@ -1111,10 +1128,10 @@
       <c r="C14">
         <v>25.130932109210502</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D14" s="4">
         <v>56.295292336114699</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="5">
         <v>12</v>
       </c>
       <c r="F14">
@@ -1123,10 +1140,10 @@
       <c r="G14">
         <v>1.28144909575108</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H14" s="4">
         <v>39.9937309002121</v>
       </c>
-      <c r="I14" s="9">
+      <c r="I14" s="5">
         <v>12</v>
       </c>
       <c r="J14">
@@ -1135,18 +1152,18 @@
       <c r="K14">
         <v>46.814297746629499</v>
       </c>
-      <c r="L14" s="8">
+      <c r="L14" s="4">
         <v>115.79932057927201</v>
       </c>
-      <c r="M14" s="9">
+      <c r="M14" s="5">
         <v>12</v>
       </c>
-      <c r="N14" s="8">
+      <c r="N14" s="4">
         <v>-0.74784721613453697</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="9">
+      <c r="A15" s="5">
         <v>13</v>
       </c>
       <c r="B15">
@@ -1155,10 +1172,10 @@
       <c r="C15">
         <v>35.710991647556099</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="4">
         <v>81.907979974636206</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="5">
         <v>13</v>
       </c>
       <c r="F15">
@@ -1167,10 +1184,10 @@
       <c r="G15">
         <v>0.10867671624939899</v>
       </c>
-      <c r="H15" s="8">
+      <c r="H15" s="4">
         <v>110.405246808702</v>
       </c>
-      <c r="I15" s="9">
+      <c r="I15" s="5">
         <v>13</v>
       </c>
       <c r="J15">
@@ -1179,18 +1196,18 @@
       <c r="K15">
         <v>7.3290581148114304</v>
       </c>
-      <c r="L15" s="8">
+      <c r="L15" s="4">
         <v>111.638759283106</v>
       </c>
-      <c r="M15" s="9">
+      <c r="M15" s="5">
         <v>13</v>
       </c>
-      <c r="N15" s="8">
+      <c r="N15" s="4">
         <v>0.75128030984111505</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="9">
+      <c r="A16" s="5">
         <v>14</v>
       </c>
       <c r="B16">
@@ -1199,10 +1216,10 @@
       <c r="C16">
         <v>30.452438596381601</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16" s="4">
         <v>65.463331652410602</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="5">
         <v>14</v>
       </c>
       <c r="F16">
@@ -1211,10 +1228,10 @@
       <c r="G16">
         <v>0.36886214368782</v>
       </c>
-      <c r="H16" s="8">
+      <c r="H16" s="4">
         <v>48.727230315465398</v>
       </c>
-      <c r="I16" s="9">
+      <c r="I16" s="5">
         <v>14</v>
       </c>
       <c r="J16">
@@ -1223,18 +1240,18 @@
       <c r="K16">
         <v>9.6190154802530898</v>
       </c>
-      <c r="L16" s="8">
+      <c r="L16" s="4">
         <v>126.85083786675401</v>
       </c>
-      <c r="M16" s="9">
+      <c r="M16" s="5">
         <v>14</v>
       </c>
-      <c r="N16" s="8">
+      <c r="N16" s="4">
         <v>-0.99511469963927401</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="9">
+      <c r="A17" s="5">
         <v>15</v>
       </c>
       <c r="B17">
@@ -1243,10 +1260,10 @@
       <c r="C17">
         <v>34.507141513801002</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D17" s="4">
         <v>86.784058493584098</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E17" s="5">
         <v>15</v>
       </c>
       <c r="F17">
@@ -1255,10 +1272,10 @@
       <c r="G17">
         <v>0.27256702654278298</v>
       </c>
-      <c r="H17" s="8">
+      <c r="H17" s="4">
         <v>45.670098761440499</v>
       </c>
-      <c r="I17" s="9">
+      <c r="I17" s="5">
         <v>15</v>
       </c>
       <c r="J17">
@@ -1267,18 +1284,18 @@
       <c r="K17">
         <v>8.8793848825599895</v>
       </c>
-      <c r="L17" s="8">
+      <c r="L17" s="4">
         <v>166.508864424942</v>
       </c>
-      <c r="M17" s="9">
+      <c r="M17" s="5">
         <v>15</v>
       </c>
-      <c r="N17" s="8">
+      <c r="N17" s="4">
         <v>-0.99550048954989001</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="9">
+      <c r="A18" s="5">
         <v>16</v>
       </c>
       <c r="B18">
@@ -1287,22 +1304,22 @@
       <c r="C18">
         <v>21.784641474364498</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D18" s="4">
         <v>85.467320888299298</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E18" s="5">
         <v>16</v>
       </c>
-      <c r="F18" s="13">
+      <c r="F18" s="9">
         <v>2.91686656605616E-4</v>
       </c>
       <c r="G18">
         <v>8.14867063883052E-2</v>
       </c>
-      <c r="H18" s="8">
+      <c r="H18" s="4">
         <v>29.922660112209201</v>
       </c>
-      <c r="I18" s="9">
+      <c r="I18" s="5">
         <v>16</v>
       </c>
       <c r="J18">
@@ -1311,18 +1328,18 @@
       <c r="K18">
         <v>9.3870390657270999</v>
       </c>
-      <c r="L18" s="8">
+      <c r="L18" s="4">
         <v>292.93360241125401</v>
       </c>
-      <c r="M18" s="9">
+      <c r="M18" s="5">
         <v>16</v>
       </c>
-      <c r="N18" s="8">
+      <c r="N18" s="4">
         <v>-0.99511469963927401</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="9">
+      <c r="A19" s="5">
         <v>17</v>
       </c>
       <c r="B19">
@@ -1331,10 +1348,10 @@
       <c r="C19">
         <v>62.562770208980098</v>
       </c>
-      <c r="D19" s="8">
+      <c r="D19" s="4">
         <v>119.960047284954</v>
       </c>
-      <c r="E19" s="9">
+      <c r="E19" s="5">
         <v>17</v>
       </c>
       <c r="F19">
@@ -1343,10 +1360,10 @@
       <c r="G19">
         <v>0.36933129703637402</v>
       </c>
-      <c r="H19" s="8">
+      <c r="H19" s="4">
         <v>20.586228872654399</v>
       </c>
-      <c r="I19" s="9">
+      <c r="I19" s="5">
         <v>17</v>
       </c>
       <c r="J19">
@@ -1355,18 +1372,18 @@
       <c r="K19">
         <v>8.8925814730305408</v>
       </c>
-      <c r="L19" s="8">
+      <c r="L19" s="4">
         <v>230.68397917264701</v>
       </c>
-      <c r="M19" s="9">
+      <c r="M19" s="5">
         <v>17</v>
       </c>
-      <c r="N19" s="8">
+      <c r="N19" s="4">
         <v>-0.75312481486496696</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="9">
+      <c r="A20" s="5">
         <v>18</v>
       </c>
       <c r="B20">
@@ -1375,10 +1392,10 @@
       <c r="C20">
         <v>17.8405712632313</v>
       </c>
-      <c r="D20" s="8">
+      <c r="D20" s="4">
         <v>83.8782514781809</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="5">
         <v>18</v>
       </c>
       <c r="F20">
@@ -1387,10 +1404,10 @@
       <c r="G20">
         <v>0.27758277674121401</v>
       </c>
-      <c r="H20" s="8">
+      <c r="H20" s="4">
         <v>93.038833792654202</v>
       </c>
-      <c r="I20" s="9">
+      <c r="I20" s="5">
         <v>18</v>
       </c>
       <c r="J20">
@@ -1399,18 +1416,18 @@
       <c r="K20">
         <v>88.909396765737597</v>
       </c>
-      <c r="L20" s="8">
+      <c r="L20" s="4">
         <v>183.632539302087</v>
       </c>
-      <c r="M20" s="9">
+      <c r="M20" s="5">
         <v>18</v>
       </c>
-      <c r="N20" s="8">
+      <c r="N20" s="4">
         <v>-1.02992784328481</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="9">
+      <c r="A21" s="5">
         <v>19</v>
       </c>
       <c r="B21">
@@ -1419,10 +1436,10 @@
       <c r="C21">
         <v>25.790971041042901</v>
       </c>
-      <c r="D21" s="8">
+      <c r="D21" s="4">
         <v>69.512919910212602</v>
       </c>
-      <c r="E21" s="9">
+      <c r="E21" s="5">
         <v>19</v>
       </c>
       <c r="F21">
@@ -1431,10 +1448,10 @@
       <c r="G21">
         <v>0.23831761675317201</v>
       </c>
-      <c r="H21" s="8">
+      <c r="H21" s="4">
         <v>66.266355684375498</v>
       </c>
-      <c r="I21" s="9">
+      <c r="I21" s="5">
         <v>19</v>
       </c>
       <c r="J21">
@@ -1443,18 +1460,18 @@
       <c r="K21">
         <v>17.1988556038723</v>
       </c>
-      <c r="L21" s="8">
+      <c r="L21" s="4">
         <v>325.13987506502599</v>
       </c>
-      <c r="M21" s="9">
+      <c r="M21" s="5">
         <v>19</v>
       </c>
-      <c r="N21" s="8">
+      <c r="N21" s="4">
         <v>-0.70306507946305796</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="9">
+      <c r="A22" s="5">
         <v>20</v>
       </c>
       <c r="B22">
@@ -1463,10 +1480,10 @@
       <c r="C22">
         <v>23.683215955667599</v>
       </c>
-      <c r="D22" s="8">
+      <c r="D22" s="4">
         <v>62.371718134112101</v>
       </c>
-      <c r="E22" s="9">
+      <c r="E22" s="5">
         <v>20</v>
       </c>
       <c r="F22">
@@ -1475,10 +1492,10 @@
       <c r="G22">
         <v>0.12557351981510501</v>
       </c>
-      <c r="H22" s="8">
+      <c r="H22" s="4">
         <v>10.6316113543679</v>
       </c>
-      <c r="I22" s="9">
+      <c r="I22" s="5">
         <v>20</v>
       </c>
       <c r="J22">
@@ -1487,18 +1504,18 @@
       <c r="K22">
         <v>9.4476949772629695</v>
       </c>
-      <c r="L22" s="8">
+      <c r="L22" s="4">
         <v>427.310523383077</v>
       </c>
-      <c r="M22" s="9">
+      <c r="M22" s="5">
         <v>20</v>
       </c>
-      <c r="N22" s="8">
+      <c r="N22" s="4">
         <v>-0.99550048954989001</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="9">
+      <c r="A23" s="5">
         <v>21</v>
       </c>
       <c r="B23">
@@ -1507,10 +1524,10 @@
       <c r="C23">
         <v>35.144610977549597</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="4">
         <v>73.101321153497906</v>
       </c>
-      <c r="E23" s="9">
+      <c r="E23" s="5">
         <v>21</v>
       </c>
       <c r="F23">
@@ -1519,10 +1536,10 @@
       <c r="G23">
         <v>0.31453626071093699</v>
       </c>
-      <c r="H23" s="8">
+      <c r="H23" s="4">
         <v>65.633092219618305</v>
       </c>
-      <c r="I23" s="9">
+      <c r="I23" s="5">
         <v>21</v>
       </c>
       <c r="J23">
@@ -1531,18 +1548,18 @@
       <c r="K23">
         <v>28.441953073350501</v>
       </c>
-      <c r="L23" s="8">
+      <c r="L23" s="4">
         <v>233.62059116647299</v>
       </c>
-      <c r="M23" s="9">
+      <c r="M23" s="5">
         <v>21</v>
       </c>
-      <c r="N23" s="8">
+      <c r="N23" s="4">
         <v>-0.982009523598117</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="9">
+      <c r="A24" s="5">
         <v>22</v>
       </c>
       <c r="B24">
@@ -1551,10 +1568,10 @@
       <c r="C24">
         <v>24.652882720892698</v>
       </c>
-      <c r="D24" s="8">
+      <c r="D24" s="4">
         <v>114.534027663988</v>
       </c>
-      <c r="E24" s="9">
+      <c r="E24" s="5">
         <v>22</v>
       </c>
       <c r="F24">
@@ -1563,10 +1580,10 @@
       <c r="G24">
         <v>0.14406548903586899</v>
       </c>
-      <c r="H24" s="8">
+      <c r="H24" s="4">
         <v>64.317129493876095</v>
       </c>
-      <c r="I24" s="9">
+      <c r="I24" s="5">
         <v>22</v>
       </c>
       <c r="J24">
@@ -1575,18 +1592,18 @@
       <c r="K24">
         <v>71.6313906002528</v>
       </c>
-      <c r="L24" s="8">
+      <c r="L24" s="4">
         <v>136.26338796413401</v>
       </c>
-      <c r="M24" s="9">
+      <c r="M24" s="5">
         <v>22</v>
       </c>
-      <c r="N24" s="8">
+      <c r="N24" s="4">
         <v>-0.99550048954989001</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="9">
+      <c r="A25" s="5">
         <v>23</v>
       </c>
       <c r="B25">
@@ -1595,10 +1612,10 @@
       <c r="C25">
         <v>38.8762381954243</v>
       </c>
-      <c r="D25" s="8">
+      <c r="D25" s="4">
         <v>97.577500674346297</v>
       </c>
-      <c r="E25" s="9">
+      <c r="E25" s="5">
         <v>23</v>
       </c>
       <c r="F25">
@@ -1607,10 +1624,10 @@
       <c r="G25">
         <v>1.3762495697455099</v>
       </c>
-      <c r="H25" s="8">
+      <c r="H25" s="4">
         <v>6.9961653712795799</v>
       </c>
-      <c r="I25" s="9">
+      <c r="I25" s="5">
         <v>23</v>
       </c>
       <c r="J25">
@@ -1619,18 +1636,18 @@
       <c r="K25">
         <v>10.5528071505423</v>
       </c>
-      <c r="L25" s="8">
+      <c r="L25" s="4">
         <v>110.453944952854</v>
       </c>
-      <c r="M25" s="9">
+      <c r="M25" s="5">
         <v>23</v>
       </c>
-      <c r="N25" s="8">
+      <c r="N25" s="4">
         <v>-1.03124356431136</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="9">
+      <c r="A26" s="5">
         <v>24</v>
       </c>
       <c r="B26">
@@ -1639,10 +1656,10 @@
       <c r="C26">
         <v>9.1244973146300303</v>
       </c>
-      <c r="D26" s="8">
+      <c r="D26" s="4">
         <v>97.382049268628805</v>
       </c>
-      <c r="E26" s="9">
+      <c r="E26" s="5">
         <v>24</v>
       </c>
       <c r="F26">
@@ -1651,10 +1668,10 @@
       <c r="G26">
         <v>0.144133886284289</v>
       </c>
-      <c r="H26" s="8">
+      <c r="H26" s="4">
         <v>20.2039494390607</v>
       </c>
-      <c r="I26" s="9">
+      <c r="I26" s="5">
         <v>24</v>
       </c>
       <c r="J26">
@@ -1663,18 +1680,18 @@
       <c r="K26">
         <v>8.6999441433450198</v>
       </c>
-      <c r="L26" s="8">
+      <c r="L26" s="4">
         <v>109.87188062957399</v>
       </c>
-      <c r="M26" s="9">
+      <c r="M26" s="5">
         <v>24</v>
       </c>
-      <c r="N26" s="8">
+      <c r="N26" s="4">
         <v>-0.94272473854657801</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="9">
+      <c r="A27" s="5">
         <v>25</v>
       </c>
       <c r="B27">
@@ -1683,10 +1700,10 @@
       <c r="C27">
         <v>42.021038850694502</v>
       </c>
-      <c r="D27" s="8">
+      <c r="D27" s="4">
         <v>83.055674987426002</v>
       </c>
-      <c r="E27" s="9">
+      <c r="E27" s="5">
         <v>25</v>
       </c>
       <c r="F27">
@@ -1695,10 +1712,10 @@
       <c r="G27">
         <v>0.217462801853266</v>
       </c>
-      <c r="H27" s="8">
+      <c r="H27" s="4">
         <v>51.857927962785801</v>
       </c>
-      <c r="I27" s="9">
+      <c r="I27" s="5">
         <v>25</v>
       </c>
       <c r="J27">
@@ -1707,18 +1724,18 @@
       <c r="K27">
         <v>8.99537308982298</v>
       </c>
-      <c r="L27" s="8">
+      <c r="L27" s="4">
         <v>169.36733078178801</v>
       </c>
-      <c r="M27" s="9">
+      <c r="M27" s="5">
         <v>25</v>
       </c>
-      <c r="N27" s="8">
+      <c r="N27" s="4">
         <v>-1.0308900958220399</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="9">
+      <c r="A28" s="5">
         <v>26</v>
       </c>
       <c r="B28">
@@ -1727,10 +1744,10 @@
       <c r="C28">
         <v>31.249847540655701</v>
       </c>
-      <c r="D28" s="8">
+      <c r="D28" s="4">
         <v>68.436469295800805</v>
       </c>
-      <c r="E28" s="9">
+      <c r="E28" s="5">
         <v>26</v>
       </c>
       <c r="F28">
@@ -1739,10 +1756,10 @@
       <c r="G28">
         <v>0.21366268831530799</v>
       </c>
-      <c r="H28" s="8">
+      <c r="H28" s="4">
         <v>40.615171157462598</v>
       </c>
-      <c r="I28" s="9">
+      <c r="I28" s="5">
         <v>26</v>
       </c>
       <c r="J28">
@@ -1751,18 +1768,18 @@
       <c r="K28">
         <v>9.1432898211414901</v>
       </c>
-      <c r="L28" s="8">
+      <c r="L28" s="4">
         <v>167.60681249338401</v>
       </c>
-      <c r="M28" s="9">
+      <c r="M28" s="5">
         <v>26</v>
       </c>
-      <c r="N28" s="8">
+      <c r="N28" s="4">
         <v>-0.99511469963927401</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="9">
+      <c r="A29" s="5">
         <v>27</v>
       </c>
       <c r="B29">
@@ -1771,10 +1788,10 @@
       <c r="C29">
         <v>25.205025272469701</v>
       </c>
-      <c r="D29" s="8">
+      <c r="D29" s="4">
         <v>81.7685404570597</v>
       </c>
-      <c r="E29" s="9">
+      <c r="E29" s="5">
         <v>27</v>
       </c>
       <c r="F29">
@@ -1783,10 +1800,10 @@
       <c r="G29">
         <v>0.20623530910212301</v>
       </c>
-      <c r="H29" s="8">
+      <c r="H29" s="4">
         <v>85.684202132585</v>
       </c>
-      <c r="I29" s="9">
+      <c r="I29" s="5">
         <v>27</v>
       </c>
       <c r="J29">
@@ -1795,18 +1812,18 @@
       <c r="K29">
         <v>43.930988519916497</v>
       </c>
-      <c r="L29" s="8">
+      <c r="L29" s="4">
         <v>161.528126926331</v>
       </c>
-      <c r="M29" s="9">
+      <c r="M29" s="5">
         <v>27</v>
       </c>
-      <c r="N29" s="8">
+      <c r="N29" s="4">
         <v>-1.02781076098617</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="9">
+      <c r="A30" s="5">
         <v>28</v>
       </c>
       <c r="B30">
@@ -1815,10 +1832,10 @@
       <c r="C30">
         <v>46.166631415250002</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D30" s="4">
         <v>77.941893445837593</v>
       </c>
-      <c r="E30" s="9">
+      <c r="E30" s="5">
         <v>28</v>
       </c>
       <c r="F30">
@@ -1827,10 +1844,10 @@
       <c r="G30">
         <v>0.33068915365534202</v>
       </c>
-      <c r="H30" s="8">
+      <c r="H30" s="4">
         <v>18.967912048909401</v>
       </c>
-      <c r="I30" s="9">
+      <c r="I30" s="5">
         <v>28</v>
       </c>
       <c r="J30">
@@ -1839,18 +1856,18 @@
       <c r="K30">
         <v>184.68138340528699</v>
       </c>
-      <c r="L30" s="8">
+      <c r="L30" s="4">
         <v>143.85129883231201</v>
       </c>
-      <c r="M30" s="9">
+      <c r="M30" s="5">
         <v>28</v>
       </c>
-      <c r="N30" s="8">
+      <c r="N30" s="4">
         <v>-0.72822445235351096</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="9">
+      <c r="A31" s="5">
         <v>29</v>
       </c>
       <c r="B31">
@@ -1859,10 +1876,10 @@
       <c r="C31">
         <v>30.127081627550101</v>
       </c>
-      <c r="D31" s="8">
+      <c r="D31" s="4">
         <v>87.3445097157839</v>
       </c>
-      <c r="E31" s="9">
+      <c r="E31" s="5">
         <v>29</v>
       </c>
       <c r="F31">
@@ -1871,10 +1888,10 @@
       <c r="G31">
         <v>0.13611485500824799</v>
       </c>
-      <c r="H31" s="8">
+      <c r="H31" s="4">
         <v>117.696298936275</v>
       </c>
-      <c r="I31" s="9">
+      <c r="I31" s="5">
         <v>29</v>
       </c>
       <c r="J31">
@@ -1883,18 +1900,18 @@
       <c r="K31">
         <v>75.2152174734331</v>
       </c>
-      <c r="L31" s="8">
+      <c r="L31" s="4">
         <v>116.707802811424</v>
       </c>
-      <c r="M31" s="9">
+      <c r="M31" s="5">
         <v>29</v>
       </c>
-      <c r="N31" s="8">
+      <c r="N31" s="4">
         <v>-0.70306507946305796</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="10">
+      <c r="A32" s="6">
         <v>30</v>
       </c>
       <c r="B32">
@@ -1903,10 +1920,10 @@
       <c r="C32">
         <v>40.292177299527701</v>
       </c>
-      <c r="D32" s="8">
+      <c r="D32" s="4">
         <v>59.610493138636599</v>
       </c>
-      <c r="E32" s="10">
+      <c r="E32" s="6">
         <v>30</v>
       </c>
       <c r="F32">
@@ -1915,10 +1932,10 @@
       <c r="G32">
         <v>2.4346126943899201E-2</v>
       </c>
-      <c r="H32" s="8">
+      <c r="H32" s="4">
         <v>19.712821252457701</v>
       </c>
-      <c r="I32" s="10">
+      <c r="I32" s="6">
         <v>30</v>
       </c>
       <c r="J32">
@@ -1927,118 +1944,1621 @@
       <c r="K32">
         <v>9.5048565409574</v>
       </c>
-      <c r="L32" s="8">
+      <c r="L32" s="4">
         <v>246.34339012516801</v>
       </c>
-      <c r="M32" s="10">
+      <c r="M32" s="6">
         <v>30</v>
       </c>
-      <c r="N32" s="8">
+      <c r="N32" s="4">
         <v>-0.70306507946305796</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="11" t="s">
+      <c r="A33" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B33" s="11">
+      <c r="B33" s="7">
         <f>_xlfn.STDEV.S(B3:B32)</f>
         <v>7.2960459092425749</v>
       </c>
-      <c r="C33" s="11">
+      <c r="C33" s="7">
         <f>_xlfn.STDEV.S(C3:C32)</f>
         <v>10.546439309618179</v>
       </c>
-      <c r="D33" s="11">
+      <c r="D33" s="7">
         <f>_xlfn.STDEV.S(D3:D32)</f>
         <v>16.463086623683175</v>
       </c>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11">
+      <c r="E33" s="7"/>
+      <c r="F33" s="7">
         <f>_xlfn.STDEV.S(F3:F32)</f>
         <v>0.4649220186419139</v>
       </c>
-      <c r="G33" s="11">
+      <c r="G33" s="7">
         <f>_xlfn.STDEV.S(G3:G32)</f>
         <v>0.32188874060886874</v>
       </c>
-      <c r="H33" s="11">
+      <c r="H33" s="7">
         <f>_xlfn.STDEV.S(H3:H32)</f>
         <v>31.526297058439841</v>
       </c>
-      <c r="I33" s="11"/>
-      <c r="J33" s="11">
+      <c r="I33" s="7"/>
+      <c r="J33" s="7">
         <f>_xlfn.STDEV.S(J3:J32)</f>
         <v>25.666776363732431</v>
       </c>
-      <c r="K33" s="11">
+      <c r="K33" s="7">
         <f>_xlfn.STDEV.S(K3:K32)</f>
         <v>40.469102080193572</v>
       </c>
-      <c r="L33" s="11">
+      <c r="L33" s="7">
         <f>_xlfn.STDEV.S(L3:L32)</f>
         <v>87.77764255420955</v>
       </c>
-      <c r="M33" s="12"/>
-      <c r="N33" s="11">
+      <c r="M33" s="8"/>
+      <c r="N33" s="7">
         <f>_xlfn.STDEV.S(N3:N32)</f>
         <v>0.32901347356754185</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="11" t="s">
+      <c r="A34" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B34" s="11">
+      <c r="B34" s="7">
         <f>AVERAGE(B3:B32)</f>
         <v>12.46627977627489</v>
       </c>
-      <c r="C34" s="11">
+      <c r="C34" s="7">
         <f>AVERAGE(C3:C32)</f>
         <v>31.655790932304605</v>
       </c>
-      <c r="D34" s="11">
+      <c r="D34" s="7">
         <f t="shared" ref="D34:N34" si="0">AVERAGE(D3:D32)</f>
         <v>85.050965060569709</v>
       </c>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11">
+      <c r="E34" s="7"/>
+      <c r="F34" s="7">
         <f t="shared" si="0"/>
         <v>0.6512982229542621</v>
       </c>
-      <c r="G34" s="11">
+      <c r="G34" s="7">
         <f t="shared" si="0"/>
         <v>0.29993321139050227</v>
       </c>
-      <c r="H34" s="11">
+      <c r="H34" s="7">
         <f t="shared" si="0"/>
         <v>48.464482461871619</v>
       </c>
-      <c r="I34" s="11"/>
-      <c r="J34" s="11">
+      <c r="I34" s="7"/>
+      <c r="J34" s="7">
         <f t="shared" si="0"/>
         <v>12.385858259561877</v>
       </c>
-      <c r="K34" s="11">
+      <c r="K34" s="7">
         <f t="shared" si="0"/>
         <v>33.956900941209526</v>
       </c>
-      <c r="L34" s="11">
+      <c r="L34" s="7">
         <f t="shared" si="0"/>
         <v>186.36538849608718</v>
       </c>
-      <c r="M34" s="11"/>
-      <c r="N34" s="11">
+      <c r="M34" s="7"/>
+      <c r="N34" s="7">
         <f t="shared" si="0"/>
         <v>-0.87503681932872057</v>
       </c>
     </row>
+    <row r="37" spans="1:14" ht="20.399999999999999" x14ac:dyDescent="0.75">
+      <c r="A37" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="10"/>
+      <c r="J37" s="10"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="12"/>
+      <c r="I39" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="J39" s="11"/>
+      <c r="K39" s="11"/>
+      <c r="L39" s="12"/>
+      <c r="M39" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="N39" s="14"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40" s="1">
+        <v>5</v>
+      </c>
+      <c r="C40" s="1">
+        <v>10</v>
+      </c>
+      <c r="D40" s="2">
+        <v>30</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F40" s="1">
+        <v>5</v>
+      </c>
+      <c r="G40" s="1">
+        <v>10</v>
+      </c>
+      <c r="H40" s="2">
+        <v>30</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J40" s="1">
+        <v>5</v>
+      </c>
+      <c r="K40" s="1">
+        <v>10</v>
+      </c>
+      <c r="L40" s="2">
+        <v>30</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N40" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="3">
+        <v>1</v>
+      </c>
+      <c r="B41">
+        <v>28.2758676276001</v>
+      </c>
+      <c r="C41">
+        <v>106.27582968890501</v>
+      </c>
+      <c r="D41" s="4">
+        <v>377.17587677000802</v>
+      </c>
+      <c r="E41" s="3">
+        <v>1</v>
+      </c>
+      <c r="F41">
+        <v>17.312161788346302</v>
+      </c>
+      <c r="G41">
+        <v>116.318401546345</v>
+      </c>
+      <c r="H41" s="4">
+        <v>529.29139347668797</v>
+      </c>
+      <c r="I41" s="3">
+        <v>1</v>
+      </c>
+      <c r="J41">
+        <v>72.937694924152396</v>
+      </c>
+      <c r="K41">
+        <v>669.48974729520705</v>
+      </c>
+      <c r="L41" s="4">
+        <v>2212.6555720992701</v>
+      </c>
+      <c r="M41" s="3">
+        <v>1</v>
+      </c>
+      <c r="N41" s="4">
+        <v>-1.02732441138881</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="5">
+        <v>2</v>
+      </c>
+      <c r="B42">
+        <v>28.330123480707801</v>
+      </c>
+      <c r="C42">
+        <v>104.054330503274</v>
+      </c>
+      <c r="D42" s="4">
+        <v>388.84387136343798</v>
+      </c>
+      <c r="E42" s="5">
+        <v>2</v>
+      </c>
+      <c r="F42">
+        <v>11.184149897808</v>
+      </c>
+      <c r="G42">
+        <v>112.165842824301</v>
+      </c>
+      <c r="H42" s="4">
+        <v>453.42186877921398</v>
+      </c>
+      <c r="I42" s="5">
+        <v>2</v>
+      </c>
+      <c r="J42">
+        <v>75.2110443973489</v>
+      </c>
+      <c r="K42">
+        <v>354.41347430441198</v>
+      </c>
+      <c r="L42" s="4">
+        <v>6976.07308023522</v>
+      </c>
+      <c r="M42" s="5">
+        <v>2</v>
+      </c>
+      <c r="N42" s="4">
+        <v>-1.0104042726026301</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="5">
+        <v>3</v>
+      </c>
+      <c r="B43">
+        <v>32.877104628543101</v>
+      </c>
+      <c r="C43">
+        <v>81.9422336847705</v>
+      </c>
+      <c r="D43" s="4">
+        <v>426.20721782317702</v>
+      </c>
+      <c r="E43" s="5">
+        <v>3</v>
+      </c>
+      <c r="F43">
+        <v>21.404673696270699</v>
+      </c>
+      <c r="G43">
+        <v>98.832905458991405</v>
+      </c>
+      <c r="H43" s="4">
+        <v>563.85688737868895</v>
+      </c>
+      <c r="I43" s="5">
+        <v>3</v>
+      </c>
+      <c r="J43">
+        <v>25.375713229956499</v>
+      </c>
+      <c r="K43">
+        <v>148.070279249485</v>
+      </c>
+      <c r="L43" s="4">
+        <v>4665.0600506268502</v>
+      </c>
+      <c r="M43" s="5">
+        <v>3</v>
+      </c>
+      <c r="N43" s="4">
+        <v>-1.0062512475861001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="5">
+        <v>4</v>
+      </c>
+      <c r="B44">
+        <v>38.315546725854297</v>
+      </c>
+      <c r="C44">
+        <v>106.99753195034</v>
+      </c>
+      <c r="D44" s="4">
+        <v>403.41887172396599</v>
+      </c>
+      <c r="E44" s="5">
+        <v>4</v>
+      </c>
+      <c r="F44">
+        <v>6.5342951567957597</v>
+      </c>
+      <c r="G44">
+        <v>124.915205944278</v>
+      </c>
+      <c r="H44" s="4">
+        <v>432.83473177965499</v>
+      </c>
+      <c r="I44" s="5">
+        <v>4</v>
+      </c>
+      <c r="J44">
+        <v>32.415233346370599</v>
+      </c>
+      <c r="K44">
+        <v>425.62170464830501</v>
+      </c>
+      <c r="L44" s="4">
+        <v>4331.4797394126299</v>
+      </c>
+      <c r="M44" s="5">
+        <v>4</v>
+      </c>
+      <c r="N44" s="4">
+        <v>-0.970582905676593</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" s="5">
+        <v>5</v>
+      </c>
+      <c r="B45">
+        <v>28.943261062467698</v>
+      </c>
+      <c r="C45">
+        <v>87.326520679952395</v>
+      </c>
+      <c r="D45" s="4">
+        <v>402.61639336285202</v>
+      </c>
+      <c r="E45" s="5">
+        <v>5</v>
+      </c>
+      <c r="F45">
+        <v>9.6308251690420903</v>
+      </c>
+      <c r="G45">
+        <v>87.867943923521693</v>
+      </c>
+      <c r="H45" s="4">
+        <v>562.83591439311499</v>
+      </c>
+      <c r="I45" s="5">
+        <v>5</v>
+      </c>
+      <c r="J45">
+        <v>97.484552948229194</v>
+      </c>
+      <c r="K45">
+        <v>285.01365462592003</v>
+      </c>
+      <c r="L45" s="4">
+        <v>5830.3522313526801</v>
+      </c>
+      <c r="M45" s="5">
+        <v>5</v>
+      </c>
+      <c r="N45" s="4">
+        <v>-1.0277685575066999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" s="5">
+        <v>6</v>
+      </c>
+      <c r="B46">
+        <v>21.9529677641621</v>
+      </c>
+      <c r="C46">
+        <v>90.752833926731995</v>
+      </c>
+      <c r="D46" s="4">
+        <v>419.96880452141198</v>
+      </c>
+      <c r="E46" s="5">
+        <v>6</v>
+      </c>
+      <c r="F46">
+        <v>23.6081928429392</v>
+      </c>
+      <c r="G46">
+        <v>128.53172354217</v>
+      </c>
+      <c r="H46" s="4">
+        <v>551.49775336644302</v>
+      </c>
+      <c r="I46" s="5">
+        <v>6</v>
+      </c>
+      <c r="J46">
+        <v>15.825501183584301</v>
+      </c>
+      <c r="K46">
+        <v>345.23058139567797</v>
+      </c>
+      <c r="L46" s="4">
+        <v>6246.4370987726497</v>
+      </c>
+      <c r="M46" s="5">
+        <v>6</v>
+      </c>
+      <c r="N46" s="4">
+        <v>-1.0292333137148999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" s="5">
+        <v>7</v>
+      </c>
+      <c r="B47">
+        <v>26.6141145947343</v>
+      </c>
+      <c r="C47">
+        <v>105.13358432462201</v>
+      </c>
+      <c r="D47" s="4">
+        <v>398.71386624283599</v>
+      </c>
+      <c r="E47" s="5">
+        <v>7</v>
+      </c>
+      <c r="F47">
+        <v>11.7458172073956</v>
+      </c>
+      <c r="G47">
+        <v>104.01113060407</v>
+      </c>
+      <c r="H47" s="4">
+        <v>503.999188867915</v>
+      </c>
+      <c r="I47" s="5">
+        <v>7</v>
+      </c>
+      <c r="J47">
+        <v>105.327897134154</v>
+      </c>
+      <c r="K47">
+        <v>507.99738037682198</v>
+      </c>
+      <c r="L47" s="4">
+        <v>5509.51522065473</v>
+      </c>
+      <c r="M47" s="5">
+        <v>7</v>
+      </c>
+      <c r="N47" s="4">
+        <v>-1.0213708230949401</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" s="5">
+        <v>8</v>
+      </c>
+      <c r="B48">
+        <v>26.730492836003801</v>
+      </c>
+      <c r="C48">
+        <v>101.64449829116199</v>
+      </c>
+      <c r="D48" s="4">
+        <v>419.22964548702902</v>
+      </c>
+      <c r="E48" s="5">
+        <v>8</v>
+      </c>
+      <c r="F48">
+        <v>23.877329501301201</v>
+      </c>
+      <c r="G48">
+        <v>75.989091984055605</v>
+      </c>
+      <c r="H48" s="4">
+        <v>550.36027457572095</v>
+      </c>
+      <c r="I48" s="5">
+        <v>8</v>
+      </c>
+      <c r="J48">
+        <v>103.77342321723</v>
+      </c>
+      <c r="K48">
+        <v>522.08640756144405</v>
+      </c>
+      <c r="L48" s="4">
+        <v>4843.4619039437102</v>
+      </c>
+      <c r="M48" s="5">
+        <v>8</v>
+      </c>
+      <c r="N48" s="4">
+        <v>-1.00749954388456</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" s="5">
+        <v>9</v>
+      </c>
+      <c r="B49">
+        <v>37.714205021931697</v>
+      </c>
+      <c r="C49">
+        <v>104.964256398449</v>
+      </c>
+      <c r="D49" s="4">
+        <v>437.70605320643199</v>
+      </c>
+      <c r="E49" s="5">
+        <v>9</v>
+      </c>
+      <c r="F49">
+        <v>18.778696754910399</v>
+      </c>
+      <c r="G49">
+        <v>86.454623551348305</v>
+      </c>
+      <c r="H49" s="4">
+        <v>493.88255114780497</v>
+      </c>
+      <c r="I49" s="5">
+        <v>9</v>
+      </c>
+      <c r="J49">
+        <v>61.5619960349945</v>
+      </c>
+      <c r="K49">
+        <v>646.70098319367196</v>
+      </c>
+      <c r="L49" s="4">
+        <v>6560.4127305603897</v>
+      </c>
+      <c r="M49" s="5">
+        <v>9</v>
+      </c>
+      <c r="N49" s="4">
+        <v>-0.96463973036932205</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" s="5">
+        <v>10</v>
+      </c>
+      <c r="B50">
+        <v>23.785737030828201</v>
+      </c>
+      <c r="C50">
+        <v>108.058001401232</v>
+      </c>
+      <c r="D50" s="4">
+        <v>430.48408182196698</v>
+      </c>
+      <c r="E50" s="5">
+        <v>10</v>
+      </c>
+      <c r="F50">
+        <v>16.943148202582101</v>
+      </c>
+      <c r="G50">
+        <v>103.972981456529</v>
+      </c>
+      <c r="H50" s="4">
+        <v>494.21839219545097</v>
+      </c>
+      <c r="I50" s="5">
+        <v>10</v>
+      </c>
+      <c r="J50">
+        <v>94.656161794902999</v>
+      </c>
+      <c r="K50">
+        <v>599.53590355543201</v>
+      </c>
+      <c r="L50" s="4">
+        <v>5762.1672675712698</v>
+      </c>
+      <c r="M50" s="5">
+        <v>10</v>
+      </c>
+      <c r="N50" s="4">
+        <v>-1.022553030481</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" s="5">
+        <v>11</v>
+      </c>
+      <c r="B51">
+        <v>32.301881728792601</v>
+      </c>
+      <c r="C51">
+        <v>95.211113747550101</v>
+      </c>
+      <c r="D51" s="4">
+        <v>372.44187508965098</v>
+      </c>
+      <c r="E51" s="5">
+        <v>11</v>
+      </c>
+      <c r="F51">
+        <v>22.288174912886198</v>
+      </c>
+      <c r="G51">
+        <v>72.085358218364902</v>
+      </c>
+      <c r="H51" s="4">
+        <v>504.93329714921401</v>
+      </c>
+      <c r="I51" s="5">
+        <v>11</v>
+      </c>
+      <c r="J51">
+        <v>31.678909337258201</v>
+      </c>
+      <c r="K51">
+        <v>918.05689089370799</v>
+      </c>
+      <c r="L51" s="4">
+        <v>7032.68117280755</v>
+      </c>
+      <c r="M51" s="5">
+        <v>11</v>
+      </c>
+      <c r="N51" s="4">
+        <v>-1.0171519805646101</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" s="5">
+        <v>12</v>
+      </c>
+      <c r="B52">
+        <v>17.932531006400001</v>
+      </c>
+      <c r="C52">
+        <v>74.246610334877701</v>
+      </c>
+      <c r="D52" s="4">
+        <v>421.52604045272898</v>
+      </c>
+      <c r="E52" s="5">
+        <v>12</v>
+      </c>
+      <c r="F52">
+        <v>9.3317266357990594</v>
+      </c>
+      <c r="G52">
+        <v>88.723988729692806</v>
+      </c>
+      <c r="H52" s="4">
+        <v>624.692565024239</v>
+      </c>
+      <c r="I52" s="5">
+        <v>12</v>
+      </c>
+      <c r="J52">
+        <v>35.034108306642501</v>
+      </c>
+      <c r="K52">
+        <v>308.97461418624601</v>
+      </c>
+      <c r="L52" s="4">
+        <v>5437.2740694412196</v>
+      </c>
+      <c r="M52" s="5">
+        <v>12</v>
+      </c>
+      <c r="N52" s="4">
+        <v>-0.98720849379143405</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" s="5">
+        <v>13</v>
+      </c>
+      <c r="B53">
+        <v>25.917707445762201</v>
+      </c>
+      <c r="C53">
+        <v>75.048460271215504</v>
+      </c>
+      <c r="D53" s="4">
+        <v>427.008736375019</v>
+      </c>
+      <c r="E53" s="5">
+        <v>13</v>
+      </c>
+      <c r="F53">
+        <v>19.337345179925901</v>
+      </c>
+      <c r="G53">
+        <v>69.884888087872895</v>
+      </c>
+      <c r="H53" s="4">
+        <v>514.389829811254</v>
+      </c>
+      <c r="I53" s="5">
+        <v>13</v>
+      </c>
+      <c r="J53">
+        <v>60.403410873275099</v>
+      </c>
+      <c r="K53">
+        <v>596.10020208640503</v>
+      </c>
+      <c r="L53" s="4">
+        <v>6251.0983815064701</v>
+      </c>
+      <c r="M53" s="5">
+        <v>13</v>
+      </c>
+      <c r="N53" s="4">
+        <v>-1.00697125889183</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" s="5">
+        <v>14</v>
+      </c>
+      <c r="B54">
+        <v>37.187680960567199</v>
+      </c>
+      <c r="C54">
+        <v>101.708545664122</v>
+      </c>
+      <c r="D54" s="4">
+        <v>411.03125408335097</v>
+      </c>
+      <c r="E54" s="5">
+        <v>14</v>
+      </c>
+      <c r="F54">
+        <v>27.818188535299999</v>
+      </c>
+      <c r="G54">
+        <v>127.65634069200399</v>
+      </c>
+      <c r="H54" s="4">
+        <v>465.509562633114</v>
+      </c>
+      <c r="I54" s="5">
+        <v>14</v>
+      </c>
+      <c r="J54">
+        <v>62.942534767280897</v>
+      </c>
+      <c r="K54">
+        <v>658.52161841009899</v>
+      </c>
+      <c r="L54" s="4">
+        <v>5308.1995455246197</v>
+      </c>
+      <c r="M54" s="5">
+        <v>14</v>
+      </c>
+      <c r="N54" s="4">
+        <v>-0.99072545193717199</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" s="5">
+        <v>15</v>
+      </c>
+      <c r="B55">
+        <v>20.5440863493805</v>
+      </c>
+      <c r="C55">
+        <v>78.629480210276498</v>
+      </c>
+      <c r="D55" s="4">
+        <v>385.339869418288</v>
+      </c>
+      <c r="E55" s="5">
+        <v>15</v>
+      </c>
+      <c r="F55">
+        <v>32.570681720028198</v>
+      </c>
+      <c r="G55">
+        <v>102.927511166801</v>
+      </c>
+      <c r="H55" s="4">
+        <v>467.22580163694602</v>
+      </c>
+      <c r="I55" s="5">
+        <v>15</v>
+      </c>
+      <c r="J55">
+        <v>13.634399999999999</v>
+      </c>
+      <c r="K55">
+        <v>580.17634245676004</v>
+      </c>
+      <c r="L55" s="4">
+        <v>5035.1028968135497</v>
+      </c>
+      <c r="M55" s="5">
+        <v>15</v>
+      </c>
+      <c r="N55" s="4">
+        <v>-1.0112694956197901</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" s="5">
+        <v>16</v>
+      </c>
+      <c r="B56">
+        <v>25.484631991383502</v>
+      </c>
+      <c r="C56">
+        <v>103.41336767995</v>
+      </c>
+      <c r="D56" s="4">
+        <v>359.71101665336101</v>
+      </c>
+      <c r="E56" s="5">
+        <v>16</v>
+      </c>
+      <c r="F56">
+        <v>29.629850828580999</v>
+      </c>
+      <c r="G56">
+        <v>56.839365004756303</v>
+      </c>
+      <c r="H56" s="4">
+        <v>534.01484870908598</v>
+      </c>
+      <c r="I56" s="5">
+        <v>16</v>
+      </c>
+      <c r="J56">
+        <v>12.571863552210401</v>
+      </c>
+      <c r="K56">
+        <v>646.24431810439603</v>
+      </c>
+      <c r="L56" s="4">
+        <v>5612.21748862811</v>
+      </c>
+      <c r="M56" s="5">
+        <v>16</v>
+      </c>
+      <c r="N56" s="4">
+        <v>-0.99147323787182495</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" s="5">
+        <v>17</v>
+      </c>
+      <c r="B57">
+        <v>21.0908222962038</v>
+      </c>
+      <c r="C57">
+        <v>102.04499829890899</v>
+      </c>
+      <c r="D57" s="4">
+        <v>451.63229410391898</v>
+      </c>
+      <c r="E57" s="5">
+        <v>17</v>
+      </c>
+      <c r="F57">
+        <v>11.943917521008901</v>
+      </c>
+      <c r="G57">
+        <v>18.4346515834333</v>
+      </c>
+      <c r="H57" s="4">
+        <v>565.87320194357096</v>
+      </c>
+      <c r="I57" s="5">
+        <v>17</v>
+      </c>
+      <c r="J57">
+        <v>78.071857412048104</v>
+      </c>
+      <c r="K57">
+        <v>546.55146522913299</v>
+      </c>
+      <c r="L57" s="4">
+        <v>4857.1153969383404</v>
+      </c>
+      <c r="M57" s="5">
+        <v>17</v>
+      </c>
+      <c r="N57" s="4">
+        <v>-0.94526708873528698</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" s="5">
+        <v>18</v>
+      </c>
+      <c r="B58">
+        <v>33.414928361052297</v>
+      </c>
+      <c r="C58">
+        <v>99.403121983206802</v>
+      </c>
+      <c r="D58" s="4">
+        <v>447.81542617535598</v>
+      </c>
+      <c r="E58" s="5">
+        <v>18</v>
+      </c>
+      <c r="F58">
+        <v>17.423861072420902</v>
+      </c>
+      <c r="G58">
+        <v>88.902775038860398</v>
+      </c>
+      <c r="H58" s="4">
+        <v>452.57357283358698</v>
+      </c>
+      <c r="I58" s="5">
+        <v>18</v>
+      </c>
+      <c r="J58">
+        <v>14.8611755757192</v>
+      </c>
+      <c r="K58">
+        <v>499.694213289966</v>
+      </c>
+      <c r="L58" s="4">
+        <v>5957.31542094631</v>
+      </c>
+      <c r="M58" s="5">
+        <v>18</v>
+      </c>
+      <c r="N58" s="4">
+        <v>-0.97564858242666697</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" s="5">
+        <v>19</v>
+      </c>
+      <c r="B59" t="s">
+        <v>9</v>
+      </c>
+      <c r="C59">
+        <v>87.516831133333</v>
+      </c>
+      <c r="D59" s="4">
+        <v>439.09812535128998</v>
+      </c>
+      <c r="E59" s="5">
+        <v>19</v>
+      </c>
+      <c r="F59">
+        <v>22.485545037943002</v>
+      </c>
+      <c r="G59">
+        <v>103.98620817910999</v>
+      </c>
+      <c r="H59" s="4">
+        <v>679.62581263844902</v>
+      </c>
+      <c r="I59" s="5">
+        <v>19</v>
+      </c>
+      <c r="J59">
+        <v>43.596796325038902</v>
+      </c>
+      <c r="K59">
+        <v>716.04206530578597</v>
+      </c>
+      <c r="L59" s="4">
+        <v>8059.5269095233498</v>
+      </c>
+      <c r="M59" s="5">
+        <v>19</v>
+      </c>
+      <c r="N59" s="4">
+        <v>-1.0277685575066999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" s="5">
+        <v>20</v>
+      </c>
+      <c r="B60">
+        <v>28.192105425703701</v>
+      </c>
+      <c r="C60">
+        <v>81.213582899568095</v>
+      </c>
+      <c r="D60" s="4">
+        <v>340.887415680044</v>
+      </c>
+      <c r="E60" s="5">
+        <v>20</v>
+      </c>
+      <c r="F60">
+        <v>22.9286279811067</v>
+      </c>
+      <c r="G60">
+        <v>103.98620817910999</v>
+      </c>
+      <c r="H60" s="4">
+        <v>514.23270238552004</v>
+      </c>
+      <c r="I60" s="5">
+        <v>20</v>
+      </c>
+      <c r="J60">
+        <v>17.253717903090902</v>
+      </c>
+      <c r="K60">
+        <v>475.18916246549298</v>
+      </c>
+      <c r="L60" s="4">
+        <v>5280.9767876147898</v>
+      </c>
+      <c r="M60" s="5">
+        <v>20</v>
+      </c>
+      <c r="N60" s="4">
+        <v>-1.00369855806081</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61" s="5">
+        <v>21</v>
+      </c>
+      <c r="B61">
+        <v>30.682257425345199</v>
+      </c>
+      <c r="C61">
+        <v>96.371058530286604</v>
+      </c>
+      <c r="D61" s="4">
+        <v>408.89669054667002</v>
+      </c>
+      <c r="E61" s="5">
+        <v>21</v>
+      </c>
+      <c r="F61">
+        <v>15.738618658428701</v>
+      </c>
+      <c r="G61">
+        <v>131.688062034106</v>
+      </c>
+      <c r="H61" s="4">
+        <v>536.10495539951205</v>
+      </c>
+      <c r="I61" s="5">
+        <v>21</v>
+      </c>
+      <c r="J61">
+        <v>41.833581285098603</v>
+      </c>
+      <c r="K61">
+        <v>922.01157910316101</v>
+      </c>
+      <c r="L61" s="4">
+        <v>8263.5346912516707</v>
+      </c>
+      <c r="M61" s="5">
+        <v>21</v>
+      </c>
+      <c r="N61" s="4">
+        <v>-1.0241175434207299</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62" s="5">
+        <v>22</v>
+      </c>
+      <c r="B62">
+        <v>36.790098976324799</v>
+      </c>
+      <c r="C62">
+        <v>95.910942468157501</v>
+      </c>
+      <c r="D62" s="4">
+        <v>432.19845930873902</v>
+      </c>
+      <c r="E62" s="5">
+        <v>22</v>
+      </c>
+      <c r="F62">
+        <v>4.7165869436461003</v>
+      </c>
+      <c r="G62">
+        <v>76.882605720737999</v>
+      </c>
+      <c r="H62" s="4">
+        <v>525.25493313738605</v>
+      </c>
+      <c r="I62" s="5">
+        <v>22</v>
+      </c>
+      <c r="J62">
+        <v>50.126597912776802</v>
+      </c>
+      <c r="K62">
+        <v>480.59157895171199</v>
+      </c>
+      <c r="L62" s="4">
+        <v>4822.3866998207804</v>
+      </c>
+      <c r="M62" s="5">
+        <v>22</v>
+      </c>
+      <c r="N62" s="4">
+        <v>-0.94783075637275505</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" s="5">
+        <v>23</v>
+      </c>
+      <c r="B63">
+        <v>21.332633254709599</v>
+      </c>
+      <c r="C63">
+        <v>104.60198409580499</v>
+      </c>
+      <c r="D63" s="4">
+        <v>379.40837041815399</v>
+      </c>
+      <c r="E63" s="5">
+        <v>23</v>
+      </c>
+      <c r="F63">
+        <v>19.6253152939911</v>
+      </c>
+      <c r="G63">
+        <v>77.595024699717996</v>
+      </c>
+      <c r="H63" s="4">
+        <v>451.69367547469699</v>
+      </c>
+      <c r="I63" s="5">
+        <v>23</v>
+      </c>
+      <c r="J63">
+        <v>135.13688873077299</v>
+      </c>
+      <c r="K63">
+        <v>352.17622053310998</v>
+      </c>
+      <c r="L63" s="4">
+        <v>5580.1891361500402</v>
+      </c>
+      <c r="M63" s="5">
+        <v>23</v>
+      </c>
+      <c r="N63" s="4">
+        <v>-0.98751689339140603</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64" s="5">
+        <v>24</v>
+      </c>
+      <c r="B64">
+        <v>43.922692069086999</v>
+      </c>
+      <c r="C64">
+        <v>100.475428335728</v>
+      </c>
+      <c r="D64" s="4">
+        <v>409.43381959573702</v>
+      </c>
+      <c r="E64" s="5">
+        <v>24</v>
+      </c>
+      <c r="F64">
+        <v>10.7919692268368</v>
+      </c>
+      <c r="G64">
+        <v>126.944436812695</v>
+      </c>
+      <c r="H64" s="4">
+        <v>494.80943838434598</v>
+      </c>
+      <c r="I64" s="5">
+        <v>24</v>
+      </c>
+      <c r="J64">
+        <v>51.159398171348798</v>
+      </c>
+      <c r="K64">
+        <v>400.69479606108399</v>
+      </c>
+      <c r="L64" s="4">
+        <v>5479.7259624528997</v>
+      </c>
+      <c r="M64" s="5">
+        <v>24</v>
+      </c>
+      <c r="N64" s="4">
+        <v>-1.02732441138881</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" s="5">
+        <v>25</v>
+      </c>
+      <c r="B65">
+        <v>41.965901219673199</v>
+      </c>
+      <c r="C65">
+        <v>88.744823953233194</v>
+      </c>
+      <c r="D65" s="4">
+        <v>401.53963264106602</v>
+      </c>
+      <c r="E65" s="5">
+        <v>25</v>
+      </c>
+      <c r="F65">
+        <v>31.389688354421398</v>
+      </c>
+      <c r="G65">
+        <v>93.815854418206996</v>
+      </c>
+      <c r="H65" s="4">
+        <v>571.30508604801105</v>
+      </c>
+      <c r="I65" s="5">
+        <v>25</v>
+      </c>
+      <c r="J65">
+        <v>30.225346088721601</v>
+      </c>
+      <c r="K65">
+        <v>504.71822962298802</v>
+      </c>
+      <c r="L65" s="4">
+        <v>5292.9924847784796</v>
+      </c>
+      <c r="M65" s="5">
+        <v>25</v>
+      </c>
+      <c r="N65" s="4">
+        <v>-1.01937061060783</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66" s="5">
+        <v>26</v>
+      </c>
+      <c r="B66">
+        <v>26.511517630990198</v>
+      </c>
+      <c r="C66">
+        <v>109.224375601945</v>
+      </c>
+      <c r="D66" s="4">
+        <v>342.54686226513701</v>
+      </c>
+      <c r="E66" s="5">
+        <v>26</v>
+      </c>
+      <c r="F66">
+        <v>27.4635819881989</v>
+      </c>
+      <c r="G66">
+        <v>106.536068311525</v>
+      </c>
+      <c r="H66" s="4">
+        <v>563.426133062487</v>
+      </c>
+      <c r="I66" s="5">
+        <v>26</v>
+      </c>
+      <c r="J66">
+        <v>31.6580172220295</v>
+      </c>
+      <c r="K66">
+        <v>568.239866511694</v>
+      </c>
+      <c r="L66" s="4">
+        <v>7874.2052998196004</v>
+      </c>
+      <c r="M66" s="5">
+        <v>26</v>
+      </c>
+      <c r="N66" s="4">
+        <v>-1.0083020806288301</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67" s="5">
+        <v>27</v>
+      </c>
+      <c r="B67">
+        <v>30.089815710804899</v>
+      </c>
+      <c r="C67">
+        <v>76.002221184457397</v>
+      </c>
+      <c r="D67" s="4">
+        <v>399.13115559890002</v>
+      </c>
+      <c r="E67" s="5">
+        <v>27</v>
+      </c>
+      <c r="F67">
+        <v>11.607498755232299</v>
+      </c>
+      <c r="G67">
+        <v>119.047942527988</v>
+      </c>
+      <c r="H67" s="4">
+        <v>593.84647268380695</v>
+      </c>
+      <c r="I67" s="5">
+        <v>27</v>
+      </c>
+      <c r="J67">
+        <v>22.6464839166226</v>
+      </c>
+      <c r="K67">
+        <v>451.41927329784397</v>
+      </c>
+      <c r="L67" s="4">
+        <v>7230.7701904964997</v>
+      </c>
+      <c r="M67" s="5">
+        <v>27</v>
+      </c>
+      <c r="N67" s="4">
+        <v>-1.022553030481</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68" s="5">
+        <v>28</v>
+      </c>
+      <c r="B68">
+        <v>31.472989307850899</v>
+      </c>
+      <c r="C68">
+        <v>103.487685324315</v>
+      </c>
+      <c r="D68" s="4">
+        <v>415.13695147632501</v>
+      </c>
+      <c r="E68" s="5">
+        <v>28</v>
+      </c>
+      <c r="F68">
+        <v>27.044057472130401</v>
+      </c>
+      <c r="G68">
+        <v>69.5116160529506</v>
+      </c>
+      <c r="H68" s="4">
+        <v>422.48130362500001</v>
+      </c>
+      <c r="I68" s="5">
+        <v>28</v>
+      </c>
+      <c r="J68">
+        <v>88.635029409864103</v>
+      </c>
+      <c r="K68">
+        <v>515.92907358319906</v>
+      </c>
+      <c r="L68" s="4">
+        <v>5773.3053952659702</v>
+      </c>
+      <c r="M68" s="5">
+        <v>28</v>
+      </c>
+      <c r="N68" s="4">
+        <v>-1.0062512475861001</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" s="5">
+        <v>29</v>
+      </c>
+      <c r="B69">
+        <v>31.227848439030701</v>
+      </c>
+      <c r="C69">
+        <v>97.278776876277604</v>
+      </c>
+      <c r="D69" s="4">
+        <v>388.53066835700002</v>
+      </c>
+      <c r="E69" s="5">
+        <v>29</v>
+      </c>
+      <c r="F69">
+        <v>19.675328543506801</v>
+      </c>
+      <c r="G69">
+        <v>138.011034607591</v>
+      </c>
+      <c r="H69" s="4">
+        <v>508.25962719985898</v>
+      </c>
+      <c r="I69" s="5">
+        <v>29</v>
+      </c>
+      <c r="J69">
+        <v>67.756951708970504</v>
+      </c>
+      <c r="K69">
+        <v>519.69214729786199</v>
+      </c>
+      <c r="L69" s="4">
+        <v>5957.31542094631</v>
+      </c>
+      <c r="M69" s="5">
+        <v>29</v>
+      </c>
+      <c r="N69" s="4">
+        <v>-0.99367355496180698</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70" s="6">
+        <v>30</v>
+      </c>
+      <c r="B70">
+        <v>30.782435355894599</v>
+      </c>
+      <c r="C70">
+        <v>98.234515319253902</v>
+      </c>
+      <c r="D70" s="4">
+        <v>418.07079611976297</v>
+      </c>
+      <c r="E70" s="6">
+        <v>30</v>
+      </c>
+      <c r="F70">
+        <v>44.544266787534497</v>
+      </c>
+      <c r="G70">
+        <v>49.236981701552999</v>
+      </c>
+      <c r="H70" s="4">
+        <v>485.08217709394802</v>
+      </c>
+      <c r="I70" s="6">
+        <v>30</v>
+      </c>
+      <c r="J70">
+        <v>41.7306679477255</v>
+      </c>
+      <c r="K70">
+        <v>659.54585645177394</v>
+      </c>
+      <c r="L70" s="4">
+        <v>133139.76639999999</v>
+      </c>
+      <c r="M70" s="6">
+        <v>30</v>
+      </c>
+      <c r="N70" s="4">
+        <v>-1.02620690035041</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B71" s="7">
+        <f>_xlfn.STDEV.S(B41:B70)</f>
+        <v>6.4495078121272664</v>
+      </c>
+      <c r="C71" s="7">
+        <f>_xlfn.STDEV.S(C41:C70)</f>
+        <v>10.750012097326463</v>
+      </c>
+      <c r="D71" s="7">
+        <f>_xlfn.STDEV.S(D41:D70)</f>
+        <v>28.26643704535763</v>
+      </c>
+      <c r="E71" s="7"/>
+      <c r="F71" s="7">
+        <f>_xlfn.STDEV.S(F41:F70)</f>
+        <v>8.7913687591226992</v>
+      </c>
+      <c r="G71" s="7">
+        <f>_xlfn.STDEV.S(G41:G70)</f>
+        <v>27.273523473747016</v>
+      </c>
+      <c r="H71" s="7">
+        <f>_xlfn.STDEV.S(H41:H70)</f>
+        <v>57.279436622865852</v>
+      </c>
+      <c r="I71" s="7"/>
+      <c r="J71" s="7">
+        <f>_xlfn.STDEV.S(J41:J70)</f>
+        <v>32.429704661406952</v>
+      </c>
+      <c r="K71" s="7">
+        <f>_xlfn.STDEV.S(K41:K70)</f>
+        <v>168.66695443607955</v>
+      </c>
+      <c r="L71" s="7">
+        <f>_xlfn.STDEV.S(L41:L70)</f>
+        <v>23281.277522041877</v>
+      </c>
+      <c r="M71" s="7"/>
+      <c r="N71" s="7">
+        <f>_xlfn.STDEV.S(N41:N70)</f>
+        <v>2.3750470205233524E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B72" s="7">
+        <f>AVERAGE(B41:B70)</f>
+        <v>29.668413300958274</v>
+      </c>
+      <c r="C72" s="7">
+        <f t="shared" ref="C72:N72" si="1">AVERAGE(C41:C70)</f>
+        <v>95.530584825396929</v>
+      </c>
+      <c r="D72" s="7">
+        <f t="shared" si="1"/>
+        <v>405.19167140112046</v>
+      </c>
+      <c r="E72" s="7"/>
+      <c r="F72" s="7">
+        <f t="shared" si="1"/>
+        <v>19.645804055543941</v>
+      </c>
+      <c r="G72" s="7">
+        <f t="shared" si="1"/>
+        <v>95.39189242008959</v>
+      </c>
+      <c r="H72" s="7">
+        <f t="shared" si="1"/>
+        <v>520.38446509449091</v>
+      </c>
+      <c r="I72" s="7"/>
+      <c r="J72" s="7">
+        <f t="shared" si="1"/>
+        <v>53.850898488580633</v>
+      </c>
+      <c r="K72" s="7">
+        <f t="shared" si="1"/>
+        <v>527.4909876682932</v>
+      </c>
+      <c r="L72" s="7">
+        <f t="shared" si="1"/>
+        <v>10039.443821531866</v>
+      </c>
+      <c r="M72" s="7"/>
+      <c r="N72" s="7">
+        <f t="shared" si="1"/>
+        <v>-1.003598585696712</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="8">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="I1:L1"/>
     <mergeCell ref="M1:N1"/>
+    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="E39:H39"/>
+    <mergeCell ref="I39:L39"/>
+    <mergeCell ref="M39:N39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Create hybrid algorithm for Rastrigin and Griewank functions
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="12">
   <si>
     <t>Rastrigin</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t>12.258187238.352997533613895908</t>
+  </si>
+  <si>
+    <t>Hibridizare [pop_size=50,crossover_pbb=0.4,mutation_pbb=0.1, hillcimbing_pbb=0.3]</t>
+  </si>
+  <si>
+    <t>Iterations = 200</t>
   </si>
 </sst>
 </file>
@@ -555,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N72"/>
+  <dimension ref="A1:N110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N74" sqref="N74"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="F109" sqref="F109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3549,8 +3555,1514 @@
         <v>-1.003598585696712</v>
       </c>
     </row>
+    <row r="75" spans="1:14" ht="20.399999999999999" x14ac:dyDescent="0.75">
+      <c r="A75" t="s">
+        <v>7</v>
+      </c>
+      <c r="C75" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D75" s="10"/>
+      <c r="E75" s="10"/>
+      <c r="F75" s="10"/>
+      <c r="G75" s="10"/>
+      <c r="H75" s="10"/>
+      <c r="I75" s="10"/>
+      <c r="J75" s="10"/>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A76" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A77" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B77" s="11"/>
+      <c r="C77" s="11"/>
+      <c r="D77" s="12"/>
+      <c r="E77" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="F77" s="11"/>
+      <c r="G77" s="11"/>
+      <c r="H77" s="12"/>
+      <c r="I77" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="J77" s="11"/>
+      <c r="K77" s="11"/>
+      <c r="L77" s="12"/>
+      <c r="M77" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="N77" s="14"/>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A78" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B78" s="1">
+        <v>5</v>
+      </c>
+      <c r="C78" s="1">
+        <v>10</v>
+      </c>
+      <c r="D78" s="2">
+        <v>30</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F78" s="1">
+        <v>5</v>
+      </c>
+      <c r="G78" s="1">
+        <v>10</v>
+      </c>
+      <c r="H78" s="2">
+        <v>30</v>
+      </c>
+      <c r="I78" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J78" s="1">
+        <v>5</v>
+      </c>
+      <c r="K78" s="1">
+        <v>10</v>
+      </c>
+      <c r="L78" s="2">
+        <v>30</v>
+      </c>
+      <c r="M78" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N78" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A79" s="3">
+        <v>1</v>
+      </c>
+      <c r="B79">
+        <v>0.104292362612405</v>
+      </c>
+      <c r="C79">
+        <v>1.17488415661039</v>
+      </c>
+      <c r="D79" s="4">
+        <v>30.132480990226298</v>
+      </c>
+      <c r="E79" s="3">
+        <v>1</v>
+      </c>
+      <c r="F79" s="9">
+        <v>5.1516244644644795E-4</v>
+      </c>
+      <c r="G79">
+        <v>2.2207401192999998</v>
+      </c>
+      <c r="H79" s="4">
+        <v>282.63097067500001</v>
+      </c>
+      <c r="I79" s="3">
+        <v>1</v>
+      </c>
+      <c r="J79">
+        <v>37.7864</v>
+      </c>
+      <c r="K79">
+        <v>7364.3796000000002</v>
+      </c>
+      <c r="L79" s="4">
+        <v>66663.710399999996</v>
+      </c>
+      <c r="M79" s="3">
+        <v>1</v>
+      </c>
+      <c r="N79" s="4">
+        <v>-0.84866200012699999</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A80" s="5">
+        <v>2</v>
+      </c>
+      <c r="B80">
+        <v>0.14401580372928499</v>
+      </c>
+      <c r="C80">
+        <v>0.20858472522480201</v>
+      </c>
+      <c r="D80" s="4">
+        <v>28.891567154662798</v>
+      </c>
+      <c r="E80" s="5">
+        <v>2</v>
+      </c>
+      <c r="F80" s="9">
+        <v>9.5797370065819898E-5</v>
+      </c>
+      <c r="G80">
+        <v>0.72534354114699995</v>
+      </c>
+      <c r="H80" s="4">
+        <v>178.39668370000001</v>
+      </c>
+      <c r="I80" s="5">
+        <v>2</v>
+      </c>
+      <c r="J80">
+        <v>5.03</v>
+      </c>
+      <c r="K80">
+        <v>8098.4543999999996</v>
+      </c>
+      <c r="L80" s="4">
+        <v>45218.058400000002</v>
+      </c>
+      <c r="M80" s="5">
+        <v>2</v>
+      </c>
+      <c r="N80" s="4">
+        <v>-0.94272473854700001</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A81" s="5">
+        <v>3</v>
+      </c>
+      <c r="B81">
+        <v>2.48454803786444E-2</v>
+      </c>
+      <c r="C81">
+        <v>3.69019557952761</v>
+      </c>
+      <c r="D81" s="4">
+        <v>25.0510166539806</v>
+      </c>
+      <c r="E81" s="5">
+        <v>3</v>
+      </c>
+      <c r="F81" s="9">
+        <v>3.3079669169944198E-4</v>
+      </c>
+      <c r="G81">
+        <v>1.4639979776200001</v>
+      </c>
+      <c r="H81" s="4">
+        <v>196.505368374</v>
+      </c>
+      <c r="I81" s="5">
+        <v>3</v>
+      </c>
+      <c r="J81">
+        <v>5.2552000000000003</v>
+      </c>
+      <c r="K81">
+        <v>5826.6927999999998</v>
+      </c>
+      <c r="L81" s="4">
+        <v>81736.441200000001</v>
+      </c>
+      <c r="M81" s="5">
+        <v>3</v>
+      </c>
+      <c r="N81" s="4">
+        <v>-0.94240306222500003</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A82" s="5">
+        <v>4</v>
+      </c>
+      <c r="B82">
+        <v>2.48454803786444E-2</v>
+      </c>
+      <c r="C82">
+        <v>3.55519623852669</v>
+      </c>
+      <c r="D82" s="4">
+        <v>23.5488119446787</v>
+      </c>
+      <c r="E82" s="5">
+        <v>4</v>
+      </c>
+      <c r="F82" s="9">
+        <v>9.5797370065819898E-5</v>
+      </c>
+      <c r="G82">
+        <v>1.2449799450400001</v>
+      </c>
+      <c r="H82" s="4">
+        <v>156.66681185900001</v>
+      </c>
+      <c r="I82" s="5">
+        <v>4</v>
+      </c>
+      <c r="J82">
+        <v>4.99</v>
+      </c>
+      <c r="K82">
+        <v>16.836400000000001</v>
+      </c>
+      <c r="L82" s="4">
+        <v>168229.92079999999</v>
+      </c>
+      <c r="M82" s="5">
+        <v>4</v>
+      </c>
+      <c r="N82" s="4">
+        <v>-0.95445181065600004</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A83" s="5">
+        <v>5</v>
+      </c>
+      <c r="B83">
+        <v>0.104292362612405</v>
+      </c>
+      <c r="C83">
+        <v>1.25433103884416</v>
+      </c>
+      <c r="D83" s="4">
+        <v>21.587819481901199</v>
+      </c>
+      <c r="E83" s="5">
+        <v>5</v>
+      </c>
+      <c r="F83" s="9">
+        <v>2.07715397280705E-4</v>
+      </c>
+      <c r="G83">
+        <v>1.7181403096700001</v>
+      </c>
+      <c r="H83" s="4">
+        <v>228.33418409999999</v>
+      </c>
+      <c r="I83" s="5">
+        <v>5</v>
+      </c>
+      <c r="J83">
+        <v>5.98</v>
+      </c>
+      <c r="K83">
+        <v>12630.362800000001</v>
+      </c>
+      <c r="L83" s="4">
+        <v>154232.0852</v>
+      </c>
+      <c r="M83" s="5">
+        <v>5</v>
+      </c>
+      <c r="N83" s="4">
+        <v>-0.86292977452800002</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A84" s="5">
+        <v>6</v>
+      </c>
+      <c r="B84">
+        <v>1.0547627763477301</v>
+      </c>
+      <c r="C84">
+        <v>3.6026764008828098</v>
+      </c>
+      <c r="D84" s="4">
+        <v>22.527166663907</v>
+      </c>
+      <c r="E84" s="5">
+        <v>6</v>
+      </c>
+      <c r="F84" s="9">
+        <v>4.3120992065681603E-4</v>
+      </c>
+      <c r="G84">
+        <v>7.5395192779400002</v>
+      </c>
+      <c r="H84" s="4">
+        <v>306.32736059699999</v>
+      </c>
+      <c r="I84" s="5">
+        <v>6</v>
+      </c>
+      <c r="J84">
+        <v>5.98</v>
+      </c>
+      <c r="K84">
+        <v>1780.9212</v>
+      </c>
+      <c r="L84" s="4">
+        <v>97579.87</v>
+      </c>
+      <c r="M84" s="5">
+        <v>6</v>
+      </c>
+      <c r="N84" s="4">
+        <v>-0.99323103716299999</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A85" s="5">
+        <v>7</v>
+      </c>
+      <c r="B85">
+        <v>2.48454803786444E-2</v>
+      </c>
+      <c r="C85">
+        <v>3.1949953074316801</v>
+      </c>
+      <c r="D85" s="4">
+        <v>27.8130334175043</v>
+      </c>
+      <c r="E85" s="5">
+        <v>7</v>
+      </c>
+      <c r="F85" s="9">
+        <v>4.3120992065681603E-4</v>
+      </c>
+      <c r="G85">
+        <v>2.3333538176199999</v>
+      </c>
+      <c r="H85" s="4">
+        <v>278.232622338</v>
+      </c>
+      <c r="I85" s="5">
+        <v>7</v>
+      </c>
+      <c r="J85">
+        <v>5.2839999999999998</v>
+      </c>
+      <c r="K85">
+        <v>5020.8504000000003</v>
+      </c>
+      <c r="L85" s="4">
+        <v>96681.039199999999</v>
+      </c>
+      <c r="M85" s="5">
+        <v>7</v>
+      </c>
+      <c r="N85" s="4">
+        <v>-0.97438735377200003</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A86" s="5">
+        <v>8</v>
+      </c>
+      <c r="B86">
+        <v>0.14401580372928799</v>
+      </c>
+      <c r="C86">
+        <v>1.15905513896014</v>
+      </c>
+      <c r="D86" s="4">
+        <v>29.1910841145273</v>
+      </c>
+      <c r="E86" s="5">
+        <v>8</v>
+      </c>
+      <c r="F86" s="9">
+        <v>1.63015493456653E-4</v>
+      </c>
+      <c r="G86">
+        <v>1.6911719247799999</v>
+      </c>
+      <c r="H86" s="4">
+        <v>165.50668202</v>
+      </c>
+      <c r="I86" s="5">
+        <v>8</v>
+      </c>
+      <c r="J86">
+        <v>5.0831999999999997</v>
+      </c>
+      <c r="K86">
+        <v>7020.2056000000002</v>
+      </c>
+      <c r="L86" s="4">
+        <v>139476.38039999999</v>
+      </c>
+      <c r="M86" s="5">
+        <v>8</v>
+      </c>
+      <c r="N86" s="4">
+        <v>-0.77016806463599996</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A87" s="5">
+        <v>9</v>
+      </c>
+      <c r="B87">
+        <v>6.4568921495524706E-2</v>
+      </c>
+      <c r="C87">
+        <v>1.15905513896012</v>
+      </c>
+      <c r="D87" s="4">
+        <v>26.029149723692701</v>
+      </c>
+      <c r="E87" s="5">
+        <v>9</v>
+      </c>
+      <c r="F87" s="9">
+        <v>1.63015493456653E-4</v>
+      </c>
+      <c r="G87">
+        <v>1.14973159789</v>
+      </c>
+      <c r="H87" s="4">
+        <v>210.48890007</v>
+      </c>
+      <c r="I87" s="5">
+        <v>9</v>
+      </c>
+      <c r="J87">
+        <v>49.932000000000002</v>
+      </c>
+      <c r="K87">
+        <v>789.70799999999997</v>
+      </c>
+      <c r="L87" s="4">
+        <v>216727.61559999999</v>
+      </c>
+      <c r="M87" s="5">
+        <v>9</v>
+      </c>
+      <c r="N87" s="4">
+        <v>-1.02781076099</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A88" s="5">
+        <v>10</v>
+      </c>
+      <c r="B88">
+        <v>2.48454803786444E-2</v>
+      </c>
+      <c r="C88">
+        <v>3.6901886889329698</v>
+      </c>
+      <c r="D88" s="4">
+        <v>29.258685703975502</v>
+      </c>
+      <c r="E88" s="5">
+        <v>10</v>
+      </c>
+      <c r="F88" s="9">
+        <v>9.5797370065819898E-5</v>
+      </c>
+      <c r="G88">
+        <v>3.8694480445999999</v>
+      </c>
+      <c r="H88" s="4">
+        <v>327.1224843</v>
+      </c>
+      <c r="I88" s="5">
+        <v>10</v>
+      </c>
+      <c r="J88">
+        <v>7.4572000000000003</v>
+      </c>
+      <c r="K88">
+        <v>74.568399999999997</v>
+      </c>
+      <c r="L88" s="4">
+        <v>52531.737999999998</v>
+      </c>
+      <c r="M88" s="5">
+        <v>10</v>
+      </c>
+      <c r="N88" s="4">
+        <v>-0.88534153985399999</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A89" s="5">
+        <v>11</v>
+      </c>
+      <c r="B89">
+        <v>0.14401580372928799</v>
+      </c>
+      <c r="C89">
+        <v>1.1193316978432399</v>
+      </c>
+      <c r="D89" s="4">
+        <v>30.4520980058332</v>
+      </c>
+      <c r="E89" s="5">
+        <v>11</v>
+      </c>
+      <c r="F89" s="9">
+        <v>9.5797370065819898E-5</v>
+      </c>
+      <c r="G89">
+        <v>0.84385574292900001</v>
+      </c>
+      <c r="H89" s="4">
+        <v>297.803499225</v>
+      </c>
+      <c r="I89" s="5">
+        <v>11</v>
+      </c>
+      <c r="J89">
+        <v>12.334</v>
+      </c>
+      <c r="K89">
+        <v>47.188400000000001</v>
+      </c>
+      <c r="L89" s="4">
+        <v>172630.90239999999</v>
+      </c>
+      <c r="M89" s="5">
+        <v>11</v>
+      </c>
+      <c r="N89" s="4">
+        <v>-1.0069712588899999</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A90" s="5">
+        <v>12</v>
+      </c>
+      <c r="B90">
+        <v>0.104292362612405</v>
+      </c>
+      <c r="C90">
+        <v>3.1633441627257901</v>
+      </c>
+      <c r="D90" s="4">
+        <v>35.122347898334802</v>
+      </c>
+      <c r="E90" s="5">
+        <v>12</v>
+      </c>
+      <c r="F90" s="9">
+        <v>4.1475764827880702E-4</v>
+      </c>
+      <c r="G90">
+        <v>11.3382949068</v>
+      </c>
+      <c r="H90" s="4">
+        <v>239.37654161500001</v>
+      </c>
+      <c r="I90" s="5">
+        <v>12</v>
+      </c>
+      <c r="J90">
+        <v>6.02</v>
+      </c>
+      <c r="K90">
+        <v>33.825200000000002</v>
+      </c>
+      <c r="L90" s="4">
+        <v>153608.72200000001</v>
+      </c>
+      <c r="M90" s="5">
+        <v>12</v>
+      </c>
+      <c r="N90" s="4">
+        <v>-1.0125727546600001</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A91" s="5">
+        <v>13</v>
+      </c>
+      <c r="B91">
+        <v>6.4568921495528203E-2</v>
+      </c>
+      <c r="C91">
+        <v>3.15527186631481</v>
+      </c>
+      <c r="D91" s="4">
+        <v>196.04570539299999</v>
+      </c>
+      <c r="E91" s="5">
+        <v>13</v>
+      </c>
+      <c r="F91" s="9">
+        <v>9.5797370065819898E-5</v>
+      </c>
+      <c r="G91">
+        <v>1.23123517662</v>
+      </c>
+      <c r="H91" s="4">
+        <v>216.11438264700001</v>
+      </c>
+      <c r="I91" s="5">
+        <v>13</v>
+      </c>
+      <c r="J91">
+        <v>6.06</v>
+      </c>
+      <c r="K91">
+        <v>21.0044</v>
+      </c>
+      <c r="L91" s="4">
+        <v>157324.15160000001</v>
+      </c>
+      <c r="M91" s="5">
+        <v>13</v>
+      </c>
+      <c r="N91" s="4">
+        <v>-0.97637484376399997</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A92" s="5">
+        <v>14</v>
+      </c>
+      <c r="B92">
+        <v>6.4568921495528203E-2</v>
+      </c>
+      <c r="C92">
+        <v>2.4487590630823499</v>
+      </c>
+      <c r="D92" s="4">
+        <v>266.37789383900002</v>
+      </c>
+      <c r="E92" s="5">
+        <v>14</v>
+      </c>
+      <c r="F92" s="9">
+        <v>1.63015493456653E-4</v>
+      </c>
+      <c r="G92">
+        <v>3.1863634045799998</v>
+      </c>
+      <c r="H92" s="4">
+        <v>131.384804124</v>
+      </c>
+      <c r="I92" s="5">
+        <v>14</v>
+      </c>
+      <c r="J92">
+        <v>5.98</v>
+      </c>
+      <c r="K92">
+        <v>4396.2543999999998</v>
+      </c>
+      <c r="L92" s="4">
+        <v>103798.1832</v>
+      </c>
+      <c r="M92" s="5">
+        <v>14</v>
+      </c>
+      <c r="N92" s="4">
+        <v>-0.94893320896300004</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A93" s="5">
+        <v>15</v>
+      </c>
+      <c r="B93">
+        <v>6.4568921495524706E-2</v>
+      </c>
+      <c r="C93">
+        <v>1.1987785800770001</v>
+      </c>
+      <c r="D93" s="4">
+        <v>221.73054757099999</v>
+      </c>
+      <c r="E93" s="5">
+        <v>15</v>
+      </c>
+      <c r="F93" s="9">
+        <v>9.5797370065819898E-5</v>
+      </c>
+      <c r="G93">
+        <v>1.69410600438</v>
+      </c>
+      <c r="H93" s="4">
+        <v>262.61299414299998</v>
+      </c>
+      <c r="I93" s="5">
+        <v>15</v>
+      </c>
+      <c r="J93">
+        <v>5.2952000000000004</v>
+      </c>
+      <c r="K93">
+        <v>22.751200000000001</v>
+      </c>
+      <c r="L93" s="4">
+        <v>121352.5212</v>
+      </c>
+      <c r="M93" s="5">
+        <v>15</v>
+      </c>
+      <c r="N93" s="4">
+        <v>-0.97698850750699995</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A94" s="5">
+        <v>16</v>
+      </c>
+      <c r="B94">
+        <v>1.01503933523085</v>
+      </c>
+      <c r="C94">
+        <v>4.61116104722855</v>
+      </c>
+      <c r="D94" s="4">
+        <v>276.13026026799997</v>
+      </c>
+      <c r="E94" s="5">
+        <v>16</v>
+      </c>
+      <c r="F94" s="9">
+        <v>3.5889166675207002E-4</v>
+      </c>
+      <c r="G94">
+        <v>3.2918434085900001</v>
+      </c>
+      <c r="H94" s="4">
+        <v>409.39163306099999</v>
+      </c>
+      <c r="I94" s="5">
+        <v>16</v>
+      </c>
+      <c r="J94">
+        <v>143.41720000000001</v>
+      </c>
+      <c r="K94">
+        <v>192.15719999999999</v>
+      </c>
+      <c r="L94" s="4">
+        <v>61270.782800000001</v>
+      </c>
+      <c r="M94" s="5">
+        <v>16</v>
+      </c>
+      <c r="N94" s="4">
+        <v>-0.87501799100400002</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A95" s="5">
+        <v>17</v>
+      </c>
+      <c r="B95">
+        <v>0.104292362612405</v>
+      </c>
+      <c r="C95">
+        <v>1.2146075977272801</v>
+      </c>
+      <c r="D95" s="4">
+        <v>193.62846848999999</v>
+      </c>
+      <c r="E95" s="5">
+        <v>17</v>
+      </c>
+      <c r="F95" s="9">
+        <v>3.5889166675207002E-4</v>
+      </c>
+      <c r="G95">
+        <v>15.295003940100001</v>
+      </c>
+      <c r="H95" s="4">
+        <v>207.27407116699999</v>
+      </c>
+      <c r="I95" s="5">
+        <v>17</v>
+      </c>
+      <c r="J95">
+        <v>41.946399999999997</v>
+      </c>
+      <c r="K95">
+        <v>366.12</v>
+      </c>
+      <c r="L95" s="4">
+        <v>83567.953999999998</v>
+      </c>
+      <c r="M95" s="5">
+        <v>17</v>
+      </c>
+      <c r="N95" s="4">
+        <v>-0.88373802487300002</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A96" s="5">
+        <v>18</v>
+      </c>
+      <c r="B96">
+        <v>6.4568921495528203E-2</v>
+      </c>
+      <c r="C96">
+        <v>1.5777355315807799</v>
+      </c>
+      <c r="D96" s="4">
+        <v>189.78622058400001</v>
+      </c>
+      <c r="E96" s="5">
+        <v>18</v>
+      </c>
+      <c r="F96" s="9">
+        <v>2.6358980870733097E-4</v>
+      </c>
+      <c r="G96">
+        <v>1.15449141197</v>
+      </c>
+      <c r="H96" s="4">
+        <v>185.70657385000001</v>
+      </c>
+      <c r="I96" s="5">
+        <v>18</v>
+      </c>
+      <c r="J96">
+        <v>5.03</v>
+      </c>
+      <c r="K96">
+        <v>4278.9040000000005</v>
+      </c>
+      <c r="L96" s="4">
+        <v>67863.719599999997</v>
+      </c>
+      <c r="M96" s="5">
+        <v>18</v>
+      </c>
+      <c r="N96" s="4">
+        <v>-1.0056594076300001</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A97" s="5">
+        <v>19</v>
+      </c>
+      <c r="B97">
+        <v>0.104292362612405</v>
+      </c>
+      <c r="C97">
+        <v>1.70980097922856</v>
+      </c>
+      <c r="D97" s="4">
+        <v>220.209084327</v>
+      </c>
+      <c r="E97" s="5">
+        <v>19</v>
+      </c>
+      <c r="F97" s="9">
+        <v>3.3079669169944198E-4</v>
+      </c>
+      <c r="G97">
+        <v>2.3480247470700002</v>
+      </c>
+      <c r="H97" s="4">
+        <v>216.687479225</v>
+      </c>
+      <c r="I97" s="5">
+        <v>19</v>
+      </c>
+      <c r="J97">
+        <v>6.02</v>
+      </c>
+      <c r="K97">
+        <v>13902.035599999999</v>
+      </c>
+      <c r="L97" s="4">
+        <v>136284.32680000001</v>
+      </c>
+      <c r="M97" s="5">
+        <v>19</v>
+      </c>
+      <c r="N97" s="4">
+        <v>-0.83682006877600001</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A98" s="5">
+        <v>20</v>
+      </c>
+      <c r="B98">
+        <v>0.14401580372928499</v>
+      </c>
+      <c r="C98">
+        <v>2.2445248936963602</v>
+      </c>
+      <c r="D98" s="4">
+        <v>198.62909922599999</v>
+      </c>
+      <c r="E98" s="5">
+        <v>20</v>
+      </c>
+      <c r="F98" s="9">
+        <v>2.6358980870733097E-4</v>
+      </c>
+      <c r="G98">
+        <v>4.0851619958500001</v>
+      </c>
+      <c r="H98" s="4">
+        <v>320.48983562000001</v>
+      </c>
+      <c r="I98" s="5">
+        <v>20</v>
+      </c>
+      <c r="J98">
+        <v>4.99</v>
+      </c>
+      <c r="K98">
+        <v>14.93</v>
+      </c>
+      <c r="L98" s="4">
+        <v>100089.1308</v>
+      </c>
+      <c r="M98" s="5">
+        <v>20</v>
+      </c>
+      <c r="N98" s="4">
+        <v>-0.86292977452800002</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A99" s="5">
+        <v>21</v>
+      </c>
+      <c r="B99">
+        <v>6.4568921495528203E-2</v>
+      </c>
+      <c r="C99">
+        <v>1.2385020211939</v>
+      </c>
+      <c r="D99" s="4">
+        <v>233.03996203599999</v>
+      </c>
+      <c r="E99" s="5">
+        <v>21</v>
+      </c>
+      <c r="F99" s="9">
+        <v>3.7548910199425301E-4</v>
+      </c>
+      <c r="G99">
+        <v>6.7698472062799997</v>
+      </c>
+      <c r="H99" s="4">
+        <v>195.74149853899999</v>
+      </c>
+      <c r="I99" s="5">
+        <v>21</v>
+      </c>
+      <c r="J99">
+        <v>3.7240000000000002</v>
+      </c>
+      <c r="K99">
+        <v>857.42079999999999</v>
+      </c>
+      <c r="L99" s="4">
+        <v>91337.357999999993</v>
+      </c>
+      <c r="M99" s="5">
+        <v>21</v>
+      </c>
+      <c r="N99" s="4">
+        <v>-0.98732552664100004</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A100" s="5">
+        <v>22</v>
+      </c>
+      <c r="B100">
+        <v>6.4568921495524706E-2</v>
+      </c>
+      <c r="C100">
+        <v>1.2940544799610301</v>
+      </c>
+      <c r="D100" s="4">
+        <v>272.57215725899999</v>
+      </c>
+      <c r="E100" s="5">
+        <v>22</v>
+      </c>
+      <c r="F100" s="9">
+        <v>2.07715397280705E-4</v>
+      </c>
+      <c r="G100">
+        <v>2.7996913273400001</v>
+      </c>
+      <c r="H100" s="4">
+        <v>210.49307276799999</v>
+      </c>
+      <c r="I100" s="5">
+        <v>22</v>
+      </c>
+      <c r="J100">
+        <v>5.98</v>
+      </c>
+      <c r="K100">
+        <v>49.857999999999997</v>
+      </c>
+      <c r="L100" s="4">
+        <v>105722.6532</v>
+      </c>
+      <c r="M100" s="5">
+        <v>22</v>
+      </c>
+      <c r="N100" s="4">
+        <v>-0.899438110736</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A101" s="5">
+        <v>23</v>
+      </c>
+      <c r="B101">
+        <v>6.4568921495524706E-2</v>
+      </c>
+      <c r="C101">
+        <v>2.2684193171629801</v>
+      </c>
+      <c r="D101" s="4">
+        <v>216.61610875900001</v>
+      </c>
+      <c r="E101" s="5">
+        <v>23</v>
+      </c>
+      <c r="F101" s="9">
+        <v>9.5797370065819898E-5</v>
+      </c>
+      <c r="G101">
+        <v>2.38401425161</v>
+      </c>
+      <c r="H101" s="4">
+        <v>156.24476667600001</v>
+      </c>
+      <c r="I101" s="5">
+        <v>23</v>
+      </c>
+      <c r="J101">
+        <v>55.049199999999999</v>
+      </c>
+      <c r="K101">
+        <v>14.341200000000001</v>
+      </c>
+      <c r="L101" s="4">
+        <v>59703.234400000001</v>
+      </c>
+      <c r="M101" s="5">
+        <v>23</v>
+      </c>
+      <c r="N101" s="4">
+        <v>-0.86691561270600004</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A102" s="5">
+        <v>24</v>
+      </c>
+      <c r="B102">
+        <v>6.4568921495528203E-2</v>
+      </c>
+      <c r="C102">
+        <v>3.1791731803760501</v>
+      </c>
+      <c r="D102" s="4">
+        <v>233.79029008200001</v>
+      </c>
+      <c r="E102" s="5">
+        <v>24</v>
+      </c>
+      <c r="F102" s="9">
+        <v>2.7492602703749203E-4</v>
+      </c>
+      <c r="G102">
+        <v>2.88915472474</v>
+      </c>
+      <c r="H102" s="4">
+        <v>204.79149471100001</v>
+      </c>
+      <c r="I102" s="5">
+        <v>24</v>
+      </c>
+      <c r="J102">
+        <v>4.0991999999999997</v>
+      </c>
+      <c r="K102">
+        <v>20.3964</v>
+      </c>
+      <c r="L102" s="4">
+        <v>99208.648000000001</v>
+      </c>
+      <c r="M102" s="5">
+        <v>24</v>
+      </c>
+      <c r="N102" s="4">
+        <v>-0.98280119735399996</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A103" s="5">
+        <v>25</v>
+      </c>
+      <c r="B103">
+        <v>6.4568921495524706E-2</v>
+      </c>
+      <c r="C103">
+        <v>1.2146075977272599</v>
+      </c>
+      <c r="D103" s="4">
+        <v>242.75501206199999</v>
+      </c>
+      <c r="E103" s="5">
+        <v>25</v>
+      </c>
+      <c r="F103" s="9">
+        <v>1.79777996420216E-4</v>
+      </c>
+      <c r="G103">
+        <v>2.24951647473</v>
+      </c>
+      <c r="H103" s="4">
+        <v>175.16593535000001</v>
+      </c>
+      <c r="I103" s="5">
+        <v>25</v>
+      </c>
+      <c r="J103">
+        <v>3.9523999999999999</v>
+      </c>
+      <c r="K103">
+        <v>2099.9176000000002</v>
+      </c>
+      <c r="L103" s="4">
+        <v>94613.171600000001</v>
+      </c>
+      <c r="M103" s="5">
+        <v>25</v>
+      </c>
+      <c r="N103" s="4">
+        <v>-1.02137082309</v>
+      </c>
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A104" s="5">
+        <v>26</v>
+      </c>
+      <c r="B104">
+        <v>0.104292362612405</v>
+      </c>
+      <c r="C104">
+        <v>3.2347256391432002</v>
+      </c>
+      <c r="D104" s="4">
+        <v>230.40819644300001</v>
+      </c>
+      <c r="E104" s="5">
+        <v>26</v>
+      </c>
+      <c r="F104" s="9">
+        <v>2.4699049957244102E-4</v>
+      </c>
+      <c r="G104">
+        <v>9.9386437934699998</v>
+      </c>
+      <c r="H104" s="4">
+        <v>207.63553039999999</v>
+      </c>
+      <c r="I104" s="5">
+        <v>26</v>
+      </c>
+      <c r="J104">
+        <v>5.98</v>
+      </c>
+      <c r="K104">
+        <v>33.345999999999997</v>
+      </c>
+      <c r="L104" s="4">
+        <v>128354.26760000001</v>
+      </c>
+      <c r="M104" s="5">
+        <v>26</v>
+      </c>
+      <c r="N104" s="4">
+        <v>-0.81220982957200005</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A105" s="5">
+        <v>27</v>
+      </c>
+      <c r="B105">
+        <v>6.4568921495528203E-2</v>
+      </c>
+      <c r="C105">
+        <v>1.26240333525515</v>
+      </c>
+      <c r="D105" s="4">
+        <v>212.4213417</v>
+      </c>
+      <c r="E105" s="5">
+        <v>27</v>
+      </c>
+      <c r="F105" s="9">
+        <v>1.79777996420216E-4</v>
+      </c>
+      <c r="G105">
+        <v>3.2318803639000002</v>
+      </c>
+      <c r="H105" s="4">
+        <v>130.97930439999999</v>
+      </c>
+      <c r="I105" s="5">
+        <v>27</v>
+      </c>
+      <c r="J105">
+        <v>133.03</v>
+      </c>
+      <c r="K105">
+        <v>243.7868</v>
+      </c>
+      <c r="L105" s="4">
+        <v>169759.12239999999</v>
+      </c>
+      <c r="M105" s="5">
+        <v>27</v>
+      </c>
+      <c r="N105" s="4">
+        <v>-1.02781076099</v>
+      </c>
+    </row>
+    <row r="106" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A106" s="5">
+        <v>28</v>
+      </c>
+      <c r="B106">
+        <v>0.14401580372928499</v>
+      </c>
+      <c r="C106">
+        <v>2.268419317163</v>
+      </c>
+      <c r="D106" s="4">
+        <v>151.03226055900001</v>
+      </c>
+      <c r="E106" s="5">
+        <v>28</v>
+      </c>
+      <c r="F106" s="9">
+        <v>9.5797370065819898E-5</v>
+      </c>
+      <c r="G106">
+        <v>3.8270356422799998</v>
+      </c>
+      <c r="H106" s="4">
+        <v>316.25570872499998</v>
+      </c>
+      <c r="I106" s="5">
+        <v>28</v>
+      </c>
+      <c r="J106">
+        <v>7.2972000000000001</v>
+      </c>
+      <c r="K106">
+        <v>41.002800000000001</v>
+      </c>
+      <c r="L106" s="4">
+        <v>79176.057199999996</v>
+      </c>
+      <c r="M106" s="5">
+        <v>28</v>
+      </c>
+      <c r="N106" s="4">
+        <v>-0.97056248757899999</v>
+      </c>
+    </row>
+    <row r="107" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A107" s="5">
+        <v>29</v>
+      </c>
+      <c r="B107">
+        <v>6.4568921495524706E-2</v>
+      </c>
+      <c r="C107">
+        <v>0.20858472522480201</v>
+      </c>
+      <c r="D107" s="4">
+        <v>260.72371644999998</v>
+      </c>
+      <c r="E107" s="5">
+        <v>29</v>
+      </c>
+      <c r="F107" s="9">
+        <v>1.63015493456653E-4</v>
+      </c>
+      <c r="G107">
+        <v>4.8651899684200002</v>
+      </c>
+      <c r="H107" s="4">
+        <v>245.64631846099999</v>
+      </c>
+      <c r="I107" s="5">
+        <v>29</v>
+      </c>
+      <c r="J107">
+        <v>3.9180000000000001</v>
+      </c>
+      <c r="K107">
+        <v>15.997199999999999</v>
+      </c>
+      <c r="L107" s="4">
+        <v>108322.7016</v>
+      </c>
+      <c r="M107" s="5">
+        <v>29</v>
+      </c>
+      <c r="N107" s="4">
+        <v>-1.0095307061500001</v>
+      </c>
+    </row>
+    <row r="108" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A108" s="6">
+        <v>30</v>
+      </c>
+      <c r="B108">
+        <v>6.4568921495524706E-2</v>
+      </c>
+      <c r="C108">
+        <v>3.47867635905145</v>
+      </c>
+      <c r="D108" s="4"/>
+      <c r="E108" s="6">
+        <v>30</v>
+      </c>
+      <c r="F108" s="9">
+        <v>3.7548910199425301E-4</v>
+      </c>
+      <c r="G108">
+        <v>2.4279092316500002</v>
+      </c>
+      <c r="H108" s="4">
+        <v>213.11110060199999</v>
+      </c>
+      <c r="I108" s="6">
+        <v>30</v>
+      </c>
+      <c r="J108">
+        <v>2.8403999999999998</v>
+      </c>
+      <c r="K108">
+        <v>8086.6124</v>
+      </c>
+      <c r="L108" s="4">
+        <v>123046.4964</v>
+      </c>
+      <c r="M108" s="6">
+        <v>30</v>
+      </c>
+      <c r="N108" s="4">
+        <v>-0.90651151904500005</v>
+      </c>
+    </row>
+    <row r="109" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A109" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B109" s="7">
+        <f>_xlfn.STDEV.S(B79:B108)</f>
+        <v>0.24469763973955411</v>
+      </c>
+      <c r="C109" s="7">
+        <f>_xlfn.STDEV.S(C79:C108)</f>
+        <v>1.1742291621182335</v>
+      </c>
+      <c r="D109" s="7">
+        <f>_xlfn.STDEV.S(D79:D107)</f>
+        <v>101.94497098980156</v>
+      </c>
+      <c r="E109" s="7"/>
+      <c r="F109" s="7">
+        <f>_xlfn.STDEV.S(F79:F108)</f>
+        <v>1.2629892665104732E-4</v>
+      </c>
+      <c r="G109" s="7">
+        <f>_xlfn.STDEV.S(G79:G108)</f>
+        <v>3.3729706288617907</v>
+      </c>
+      <c r="H109" s="7">
+        <f>_xlfn.STDEV.S(H79:H108)</f>
+        <v>64.764808395063142</v>
+      </c>
+      <c r="I109" s="7"/>
+      <c r="J109" s="7">
+        <f>_xlfn.STDEV.S(J79:J108)</f>
+        <v>35.220818472206716</v>
+      </c>
+      <c r="K109" s="7">
+        <f>_xlfn.STDEV.S(K79:K108)</f>
+        <v>3989.7994539180936</v>
+      </c>
+      <c r="L109" s="7">
+        <f>_xlfn.STDEV.S(L79:L108)</f>
+        <v>41614.380203941902</v>
+      </c>
+      <c r="M109" s="7"/>
+      <c r="N109" s="7">
+        <f>_xlfn.STDEV.S(N79:N108)</f>
+        <v>7.1181983391068654E-2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A110" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B110" s="7">
+        <f>AVERAGE(B79:B108)</f>
+        <v>0.14514710689519539</v>
+      </c>
+      <c r="C110" s="7">
+        <f t="shared" ref="C110:N110" si="2">AVERAGE(C79:C108)</f>
+        <v>2.1593347935221634</v>
+      </c>
+      <c r="D110" s="7">
+        <f t="shared" si="2"/>
+        <v>142.94833057935256</v>
+      </c>
+      <c r="E110" s="7"/>
+      <c r="F110" s="7">
+        <f t="shared" si="2"/>
+        <v>2.3884062409033416E-4</v>
+      </c>
+      <c r="G110" s="7">
+        <f t="shared" si="2"/>
+        <v>3.6602563426305332</v>
+      </c>
+      <c r="H110" s="7">
+        <f t="shared" si="2"/>
+        <v>229.10395377806665</v>
+      </c>
+      <c r="I110" s="7"/>
+      <c r="J110" s="7">
+        <f t="shared" si="2"/>
+        <v>19.858040000000003</v>
+      </c>
+      <c r="K110" s="7">
+        <f t="shared" si="2"/>
+        <v>2778.6943066666663</v>
+      </c>
+      <c r="L110" s="7">
+        <f t="shared" si="2"/>
+        <v>111203.6988</v>
+      </c>
+      <c r="M110" s="7"/>
+      <c r="N110" s="7">
+        <f t="shared" si="2"/>
+        <v>-0.93575308523186662</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="12">
+    <mergeCell ref="A77:D77"/>
+    <mergeCell ref="E77:H77"/>
+    <mergeCell ref="I77:L77"/>
+    <mergeCell ref="M77:N77"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="I1:L1"/>

</xml_diff>

<commit_message>
Create hybrid algorithm for Rosenbrock and Shcb functions
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -563,8 +563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="F109" sqref="F109"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="D111" sqref="D111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3662,8 +3662,8 @@
       <c r="F79" s="9">
         <v>5.1516244644644795E-4</v>
       </c>
-      <c r="G79">
-        <v>2.2207401192999998</v>
+      <c r="G79" s="9">
+        <v>5.0724415506575495E-4</v>
       </c>
       <c r="H79" s="4">
         <v>282.63097067500001</v>
@@ -3672,10 +3672,10 @@
         <v>1</v>
       </c>
       <c r="J79">
-        <v>37.7864</v>
+        <v>0.50915290804257696</v>
       </c>
       <c r="K79">
-        <v>7364.3796000000002</v>
+        <v>1.69148420809235</v>
       </c>
       <c r="L79" s="4">
         <v>66663.710399999996</v>
@@ -3706,8 +3706,8 @@
       <c r="F80" s="9">
         <v>9.5797370065819898E-5</v>
       </c>
-      <c r="G80">
-        <v>0.72534354114699995</v>
+      <c r="G80" s="9">
+        <v>4.9204262391100396E-4</v>
       </c>
       <c r="H80" s="4">
         <v>178.39668370000001</v>
@@ -3716,10 +3716,10 @@
         <v>2</v>
       </c>
       <c r="J80">
-        <v>5.03</v>
+        <v>6.2613365072224604E-3</v>
       </c>
       <c r="K80">
-        <v>8098.4543999999996</v>
+        <v>4.5024864087076404</v>
       </c>
       <c r="L80" s="4">
         <v>45218.058400000002</v>
@@ -3750,8 +3750,8 @@
       <c r="F81" s="9">
         <v>3.3079669169944198E-4</v>
       </c>
-      <c r="G81">
-        <v>1.4639979776200001</v>
+      <c r="G81" s="9">
+        <v>2.38231036261638E-4</v>
       </c>
       <c r="H81" s="4">
         <v>196.505368374</v>
@@ -3760,10 +3760,10 @@
         <v>3</v>
       </c>
       <c r="J81">
-        <v>5.2552000000000003</v>
+        <v>6.2613365072224604E-3</v>
       </c>
       <c r="K81">
-        <v>5826.6927999999998</v>
+        <v>6.3001922092448499</v>
       </c>
       <c r="L81" s="4">
         <v>81736.441200000001</v>
@@ -3794,8 +3794,8 @@
       <c r="F82" s="9">
         <v>9.5797370065819898E-5</v>
       </c>
-      <c r="G82">
-        <v>1.2449799450400001</v>
+      <c r="G82" s="9">
+        <v>7.4985130940941004E-4</v>
       </c>
       <c r="H82" s="4">
         <v>156.66681185900001</v>
@@ -3804,10 +3804,10 @@
         <v>4</v>
       </c>
       <c r="J82">
-        <v>4.99</v>
+        <v>8.4170775983744894E-2</v>
       </c>
       <c r="K82">
-        <v>16.836400000000001</v>
+        <v>1.55227442443659</v>
       </c>
       <c r="L82" s="4">
         <v>168229.92079999999</v>
@@ -3838,8 +3838,8 @@
       <c r="F83" s="9">
         <v>2.07715397280705E-4</v>
       </c>
-      <c r="G83">
-        <v>1.7181403096700001</v>
+      <c r="G83" s="9">
+        <v>6.0571838485390297E-4</v>
       </c>
       <c r="H83" s="4">
         <v>228.33418409999999</v>
@@ -3848,10 +3848,10 @@
         <v>5</v>
       </c>
       <c r="J83">
-        <v>5.98</v>
+        <v>6.2613365072224604E-3</v>
       </c>
       <c r="K83">
-        <v>12630.362800000001</v>
+        <v>1.1600154865385699</v>
       </c>
       <c r="L83" s="4">
         <v>154232.0852</v>
@@ -3882,8 +3882,8 @@
       <c r="F84" s="9">
         <v>4.3120992065681603E-4</v>
       </c>
-      <c r="G84">
-        <v>7.5395192779400002</v>
+      <c r="G84" s="9">
+        <v>1.65031461983544E-4</v>
       </c>
       <c r="H84" s="4">
         <v>306.32736059699999</v>
@@ -3892,10 +3892,10 @@
         <v>6</v>
       </c>
       <c r="J84">
-        <v>5.98</v>
+        <v>8.4170775983744894E-2</v>
       </c>
       <c r="K84">
-        <v>1780.9212</v>
+        <v>3.69685467612703</v>
       </c>
       <c r="L84" s="4">
         <v>97579.87</v>
@@ -3926,8 +3926,8 @@
       <c r="F85" s="9">
         <v>4.3120992065681603E-4</v>
       </c>
-      <c r="G85">
-        <v>2.3333538176199999</v>
+      <c r="G85" s="9">
+        <v>2.5848405569506202E-4</v>
       </c>
       <c r="H85" s="4">
         <v>278.232622338</v>
@@ -3936,10 +3936,10 @@
         <v>7</v>
       </c>
       <c r="J85">
-        <v>5.2839999999999998</v>
+        <v>6.2613365072224604E-3</v>
       </c>
       <c r="K85">
-        <v>5020.8504000000003</v>
+        <v>1.3951854161677499</v>
       </c>
       <c r="L85" s="4">
         <v>96681.039199999999</v>
@@ -3970,8 +3970,8 @@
       <c r="F86" s="9">
         <v>1.63015493456653E-4</v>
       </c>
-      <c r="G86">
-        <v>1.6911719247799999</v>
+      <c r="G86" s="9">
+        <v>3.5960935131029698E-4</v>
       </c>
       <c r="H86" s="4">
         <v>165.50668202</v>
@@ -3980,10 +3980,10 @@
         <v>8</v>
       </c>
       <c r="J86">
-        <v>5.0831999999999997</v>
+        <v>8.4170775983744894E-2</v>
       </c>
       <c r="K86">
-        <v>7020.2056000000002</v>
+        <v>0.16411688241304501</v>
       </c>
       <c r="L86" s="4">
         <v>139476.38039999999</v>
@@ -4014,8 +4014,8 @@
       <c r="F87" s="9">
         <v>1.63015493456653E-4</v>
       </c>
-      <c r="G87">
-        <v>1.14973159789</v>
+      <c r="G87" s="9">
+        <v>2.1269009470259399E-4</v>
       </c>
       <c r="H87" s="4">
         <v>210.48890007</v>
@@ -4024,10 +4024,10 @@
         <v>9</v>
       </c>
       <c r="J87">
-        <v>49.932000000000002</v>
+        <v>0.56653986967125303</v>
       </c>
       <c r="K87">
-        <v>789.70799999999997</v>
+        <v>1.47436498496007</v>
       </c>
       <c r="L87" s="4">
         <v>216727.61559999999</v>
@@ -4058,8 +4058,8 @@
       <c r="F88" s="9">
         <v>9.5797370065819898E-5</v>
       </c>
-      <c r="G88">
-        <v>3.8694480445999999</v>
+      <c r="G88" s="9">
+        <v>3.1884230988832302E-4</v>
       </c>
       <c r="H88" s="4">
         <v>327.1224843</v>
@@ -4068,10 +4068,10 @@
         <v>10</v>
       </c>
       <c r="J88">
-        <v>7.4572000000000003</v>
+        <v>6.2613365072224604E-3</v>
       </c>
       <c r="K88">
-        <v>74.568399999999997</v>
+        <v>6.8006306533828003</v>
       </c>
       <c r="L88" s="4">
         <v>52531.737999999998</v>
@@ -4102,8 +4102,8 @@
       <c r="F89" s="9">
         <v>9.5797370065819898E-5</v>
       </c>
-      <c r="G89">
-        <v>0.84385574292900001</v>
+      <c r="G89" s="9">
+        <v>3.1435305250038199E-4</v>
       </c>
       <c r="H89" s="4">
         <v>297.803499225</v>
@@ -4112,10 +4112,10 @@
         <v>11</v>
       </c>
       <c r="J89">
-        <v>12.334</v>
+        <v>6.2613365072224604E-3</v>
       </c>
       <c r="K89">
-        <v>47.188400000000001</v>
+        <v>5.7276062855444803</v>
       </c>
       <c r="L89" s="4">
         <v>172630.90239999999</v>
@@ -4146,8 +4146,8 @@
       <c r="F90" s="9">
         <v>4.1475764827880702E-4</v>
       </c>
-      <c r="G90">
-        <v>11.3382949068</v>
+      <c r="G90" s="9">
+        <v>5.9035160652920395E-4</v>
       </c>
       <c r="H90" s="4">
         <v>239.37654161500001</v>
@@ -4156,10 +4156,10 @@
         <v>12</v>
       </c>
       <c r="J90">
-        <v>6.02</v>
+        <v>6.2613365072224604E-3</v>
       </c>
       <c r="K90">
-        <v>33.825200000000002</v>
+        <v>1.2738548571250701</v>
       </c>
       <c r="L90" s="4">
         <v>153608.72200000001</v>
@@ -4182,7 +4182,7 @@
         <v>3.15527186631481</v>
       </c>
       <c r="D91" s="4">
-        <v>196.04570539299999</v>
+        <v>30.043217175964202</v>
       </c>
       <c r="E91" s="5">
         <v>13</v>
@@ -4190,8 +4190,8 @@
       <c r="F91" s="9">
         <v>9.5797370065819898E-5</v>
       </c>
-      <c r="G91">
-        <v>1.23123517662</v>
+      <c r="G91" s="9">
+        <v>2.16414811278431E-4</v>
       </c>
       <c r="H91" s="4">
         <v>216.11438264700001</v>
@@ -4200,10 +4200,10 @@
         <v>13</v>
       </c>
       <c r="J91">
-        <v>6.06</v>
+        <v>6.2613365072224604E-3</v>
       </c>
       <c r="K91">
-        <v>21.0044</v>
+        <v>1.1135808078815801</v>
       </c>
       <c r="L91" s="4">
         <v>157324.15160000001</v>
@@ -4226,7 +4226,7 @@
         <v>2.4487590630823499</v>
       </c>
       <c r="D92" s="4">
-        <v>266.37789383900002</v>
+        <v>30.1918842256819</v>
       </c>
       <c r="E92" s="5">
         <v>14</v>
@@ -4234,8 +4234,8 @@
       <c r="F92" s="9">
         <v>1.63015493456653E-4</v>
       </c>
-      <c r="G92">
-        <v>3.1863634045799998</v>
+      <c r="G92" s="9">
+        <v>4.0616211098343198E-4</v>
       </c>
       <c r="H92" s="4">
         <v>131.384804124</v>
@@ -4244,10 +4244,10 @@
         <v>14</v>
       </c>
       <c r="J92">
-        <v>5.98</v>
+        <v>6.2613365072224604E-3</v>
       </c>
       <c r="K92">
-        <v>4396.2543999999998</v>
+        <v>0.93069554709332603</v>
       </c>
       <c r="L92" s="4">
         <v>103798.1832</v>
@@ -4270,7 +4270,7 @@
         <v>1.1987785800770001</v>
       </c>
       <c r="D93" s="4">
-        <v>221.73054757099999</v>
+        <v>24.340199721112</v>
       </c>
       <c r="E93" s="5">
         <v>15</v>
@@ -4278,8 +4278,8 @@
       <c r="F93" s="9">
         <v>9.5797370065819898E-5</v>
       </c>
-      <c r="G93">
-        <v>1.69410600438</v>
+      <c r="G93" s="9">
+        <v>3.38797812932223E-4</v>
       </c>
       <c r="H93" s="4">
         <v>262.61299414299998</v>
@@ -4288,10 +4288,10 @@
         <v>15</v>
       </c>
       <c r="J93">
-        <v>5.2952000000000004</v>
+        <v>8.4170775983744894E-2</v>
       </c>
       <c r="K93">
-        <v>22.751200000000001</v>
+        <v>4.3629473635155396</v>
       </c>
       <c r="L93" s="4">
         <v>121352.5212</v>
@@ -4314,7 +4314,7 @@
         <v>4.61116104722855</v>
       </c>
       <c r="D94" s="4">
-        <v>276.13026026799997</v>
+        <v>29.602187068574001</v>
       </c>
       <c r="E94" s="5">
         <v>16</v>
@@ -4322,8 +4322,8 @@
       <c r="F94" s="9">
         <v>3.5889166675207002E-4</v>
       </c>
-      <c r="G94">
-        <v>3.2918434085900001</v>
+      <c r="G94" s="9">
+        <v>5.1788309756573003E-4</v>
       </c>
       <c r="H94" s="4">
         <v>409.39163306099999</v>
@@ -4332,10 +4332,10 @@
         <v>16</v>
       </c>
       <c r="J94">
-        <v>143.41720000000001</v>
+        <v>6.2613365072224604E-3</v>
       </c>
       <c r="K94">
-        <v>192.15719999999999</v>
+        <v>0.943580494710764</v>
       </c>
       <c r="L94" s="4">
         <v>61270.782800000001</v>
@@ -4358,7 +4358,7 @@
         <v>1.2146075977272801</v>
       </c>
       <c r="D95" s="4">
-        <v>193.62846848999999</v>
+        <v>31.335187071088299</v>
       </c>
       <c r="E95" s="5">
         <v>17</v>
@@ -4366,8 +4366,8 @@
       <c r="F95" s="9">
         <v>3.5889166675207002E-4</v>
       </c>
-      <c r="G95">
-        <v>15.295003940100001</v>
+      <c r="G95" s="9">
+        <v>4.1005281472439298E-4</v>
       </c>
       <c r="H95" s="4">
         <v>207.27407116699999</v>
@@ -4376,10 +4376,10 @@
         <v>17</v>
       </c>
       <c r="J95">
-        <v>41.946399999999997</v>
+        <v>6.2613365072224604E-3</v>
       </c>
       <c r="K95">
-        <v>366.12</v>
+        <v>0.92490554341207498</v>
       </c>
       <c r="L95" s="4">
         <v>83567.953999999998</v>
@@ -4402,7 +4402,7 @@
         <v>1.5777355315807799</v>
       </c>
       <c r="D96" s="4">
-        <v>189.78622058400001</v>
+        <v>35.6787276554778</v>
       </c>
       <c r="E96" s="5">
         <v>18</v>
@@ -4410,8 +4410,8 @@
       <c r="F96" s="9">
         <v>2.6358980870733097E-4</v>
       </c>
-      <c r="G96">
-        <v>1.15449141197</v>
+      <c r="G96" s="9">
+        <v>4.6481871109338403E-4</v>
       </c>
       <c r="H96" s="4">
         <v>185.70657385000001</v>
@@ -4420,10 +4420,10 @@
         <v>18</v>
       </c>
       <c r="J96">
-        <v>5.03</v>
+        <v>6.2613365072224604E-3</v>
       </c>
       <c r="K96">
-        <v>4278.9040000000005</v>
+        <v>6.3001922092448499</v>
       </c>
       <c r="L96" s="4">
         <v>67863.719599999997</v>
@@ -4446,7 +4446,7 @@
         <v>1.70980097922856</v>
       </c>
       <c r="D97" s="4">
-        <v>220.209084327</v>
+        <v>27.984312623143499</v>
       </c>
       <c r="E97" s="5">
         <v>19</v>
@@ -4454,8 +4454,8 @@
       <c r="F97" s="9">
         <v>3.3079669169944198E-4</v>
       </c>
-      <c r="G97">
-        <v>2.3480247470700002</v>
+      <c r="G97" s="9">
+        <v>2.68561641261655E-4</v>
       </c>
       <c r="H97" s="4">
         <v>216.687479225</v>
@@ -4464,10 +4464,10 @@
         <v>19</v>
       </c>
       <c r="J97">
-        <v>6.02</v>
+        <v>6.2613365072224604E-3</v>
       </c>
       <c r="K97">
-        <v>13902.035599999999</v>
+        <v>1.10138273595738</v>
       </c>
       <c r="L97" s="4">
         <v>136284.32680000001</v>
@@ -4490,7 +4490,7 @@
         <v>2.2445248936963602</v>
       </c>
       <c r="D98" s="4">
-        <v>198.62909922599999</v>
+        <v>27.908780937963598</v>
       </c>
       <c r="E98" s="5">
         <v>20</v>
@@ -4498,8 +4498,8 @@
       <c r="F98" s="9">
         <v>2.6358980870733097E-4</v>
       </c>
-      <c r="G98">
-        <v>4.0851619958500001</v>
+      <c r="G98" s="9">
+        <v>7.7736912863601805E-4</v>
       </c>
       <c r="H98" s="4">
         <v>320.48983562000001</v>
@@ -4508,10 +4508,10 @@
         <v>20</v>
       </c>
       <c r="J98">
-        <v>4.99</v>
+        <v>6.2613365072224604E-3</v>
       </c>
       <c r="K98">
-        <v>14.93</v>
+        <v>5.7216384585226399</v>
       </c>
       <c r="L98" s="4">
         <v>100089.1308</v>
@@ -4534,7 +4534,7 @@
         <v>1.2385020211939</v>
       </c>
       <c r="D99" s="4">
-        <v>233.03996203599999</v>
+        <v>33.1237190184901</v>
       </c>
       <c r="E99" s="5">
         <v>21</v>
@@ -4542,8 +4542,8 @@
       <c r="F99" s="9">
         <v>3.7548910199425301E-4</v>
       </c>
-      <c r="G99">
-        <v>6.7698472062799997</v>
+      <c r="G99" s="9">
+        <v>5.7359597966477605E-4</v>
       </c>
       <c r="H99" s="4">
         <v>195.74149853899999</v>
@@ -4552,10 +4552,10 @@
         <v>21</v>
       </c>
       <c r="J99">
-        <v>3.7240000000000002</v>
+        <v>6.2613365072224604E-3</v>
       </c>
       <c r="K99">
-        <v>857.42079999999999</v>
+        <v>5.7653149210357997</v>
       </c>
       <c r="L99" s="4">
         <v>91337.357999999993</v>
@@ -4578,7 +4578,7 @@
         <v>1.2940544799610301</v>
       </c>
       <c r="D100" s="4">
-        <v>272.57215725899999</v>
+        <v>22.319047541794099</v>
       </c>
       <c r="E100" s="5">
         <v>22</v>
@@ -4586,8 +4586,8 @@
       <c r="F100" s="9">
         <v>2.07715397280705E-4</v>
       </c>
-      <c r="G100">
-        <v>2.7996913273400001</v>
+      <c r="G100" s="9">
+        <v>2.6446997483608998E-4</v>
       </c>
       <c r="H100" s="4">
         <v>210.49307276799999</v>
@@ -4596,10 +4596,10 @@
         <v>22</v>
       </c>
       <c r="J100">
-        <v>5.98</v>
+        <v>6.2613365072224604E-3</v>
       </c>
       <c r="K100">
-        <v>49.857999999999997</v>
+        <v>7.1540797063713697</v>
       </c>
       <c r="L100" s="4">
         <v>105722.6532</v>
@@ -4622,7 +4622,7 @@
         <v>2.2684193171629801</v>
       </c>
       <c r="D101" s="4">
-        <v>216.61610875900001</v>
+        <v>29.5337408310067</v>
       </c>
       <c r="E101" s="5">
         <v>23</v>
@@ -4630,8 +4630,8 @@
       <c r="F101" s="9">
         <v>9.5797370065819898E-5</v>
       </c>
-      <c r="G101">
-        <v>2.38401425161</v>
+      <c r="G101" s="9">
+        <v>5.2865535877621897E-4</v>
       </c>
       <c r="H101" s="4">
         <v>156.24476667600001</v>
@@ -4640,10 +4640,10 @@
         <v>23</v>
       </c>
       <c r="J101">
-        <v>55.049199999999999</v>
+        <v>6.2613365072224604E-3</v>
       </c>
       <c r="K101">
-        <v>14.341200000000001</v>
+        <v>4.0495502614305403</v>
       </c>
       <c r="L101" s="4">
         <v>59703.234400000001</v>
@@ -4666,7 +4666,7 @@
         <v>3.1791731803760501</v>
       </c>
       <c r="D102" s="4">
-        <v>233.79029008200001</v>
+        <v>26.403944456029201</v>
       </c>
       <c r="E102" s="5">
         <v>24</v>
@@ -4674,8 +4674,8 @@
       <c r="F102" s="9">
         <v>2.7492602703749203E-4</v>
       </c>
-      <c r="G102">
-        <v>2.88915472474</v>
+      <c r="G102" s="9">
+        <v>4.5604072869676E-4</v>
       </c>
       <c r="H102" s="4">
         <v>204.79149471100001</v>
@@ -4684,10 +4684,10 @@
         <v>24</v>
       </c>
       <c r="J102">
-        <v>4.0991999999999997</v>
+        <v>6.2613365072224604E-3</v>
       </c>
       <c r="K102">
-        <v>20.3964</v>
+        <v>5.8593424527936504</v>
       </c>
       <c r="L102" s="4">
         <v>99208.648000000001</v>
@@ -4710,7 +4710,7 @@
         <v>1.2146075977272599</v>
       </c>
       <c r="D103" s="4">
-        <v>242.75501206199999</v>
+        <v>23.716101736862001</v>
       </c>
       <c r="E103" s="5">
         <v>25</v>
@@ -4718,8 +4718,8 @@
       <c r="F103" s="9">
         <v>1.79777996420216E-4</v>
       </c>
-      <c r="G103">
-        <v>2.24951647473</v>
+      <c r="G103" s="9">
+        <v>3.3407150203934501E-4</v>
       </c>
       <c r="H103" s="4">
         <v>175.16593535000001</v>
@@ -4728,10 +4728,10 @@
         <v>25</v>
       </c>
       <c r="J103">
-        <v>3.9523999999999999</v>
+        <v>0.124406854575262</v>
       </c>
       <c r="K103">
-        <v>2099.9176000000002</v>
+        <v>1.12008916381485</v>
       </c>
       <c r="L103" s="4">
         <v>94613.171600000001</v>
@@ -4754,7 +4754,7 @@
         <v>3.2347256391432002</v>
       </c>
       <c r="D104" s="4">
-        <v>230.40819644300001</v>
+        <v>15.112080457122699</v>
       </c>
       <c r="E104" s="5">
         <v>26</v>
@@ -4762,8 +4762,8 @@
       <c r="F104" s="9">
         <v>2.4699049957244102E-4</v>
       </c>
-      <c r="G104">
-        <v>9.9386437934699998</v>
+      <c r="G104" s="9">
+        <v>4.5138592890470099E-4</v>
       </c>
       <c r="H104" s="4">
         <v>207.63553039999999</v>
@@ -4772,10 +4772,10 @@
         <v>26</v>
       </c>
       <c r="J104">
-        <v>5.98</v>
+        <v>6.2613365072224604E-3</v>
       </c>
       <c r="K104">
-        <v>33.345999999999997</v>
+        <v>3.5614034186556598</v>
       </c>
       <c r="L104" s="4">
         <v>128354.26760000001</v>
@@ -4798,7 +4798,7 @@
         <v>1.26240333525515</v>
       </c>
       <c r="D105" s="4">
-        <v>212.4213417</v>
+        <v>25.657793302330699</v>
       </c>
       <c r="E105" s="5">
         <v>27</v>
@@ -4806,8 +4806,8 @@
       <c r="F105" s="9">
         <v>1.79777996420216E-4</v>
       </c>
-      <c r="G105">
-        <v>3.2318803639000002</v>
+      <c r="G105" s="9">
+        <v>4.34092552727194E-4</v>
       </c>
       <c r="H105" s="4">
         <v>130.97930439999999</v>
@@ -4816,10 +4816,10 @@
         <v>27</v>
       </c>
       <c r="J105">
-        <v>133.03</v>
+        <v>8.4170775983744894E-2</v>
       </c>
       <c r="K105">
-        <v>243.7868</v>
+        <v>1.33515520130431</v>
       </c>
       <c r="L105" s="4">
         <v>169759.12239999999</v>
@@ -4842,7 +4842,7 @@
         <v>2.268419317163</v>
       </c>
       <c r="D106" s="4">
-        <v>151.03226055900001</v>
+        <v>21.1765871401658</v>
       </c>
       <c r="E106" s="5">
         <v>28</v>
@@ -4850,8 +4850,8 @@
       <c r="F106" s="9">
         <v>9.5797370065819898E-5</v>
       </c>
-      <c r="G106">
-        <v>3.8270356422799998</v>
+      <c r="G106" s="9">
+        <v>1.2295831479658401E-4</v>
       </c>
       <c r="H106" s="4">
         <v>316.25570872499998</v>
@@ -4860,10 +4860,10 @@
         <v>28</v>
       </c>
       <c r="J106">
-        <v>7.2972000000000001</v>
+        <v>6.2613365072224604E-3</v>
       </c>
       <c r="K106">
-        <v>41.002800000000001</v>
+        <v>0.65227597978180296</v>
       </c>
       <c r="L106" s="4">
         <v>79176.057199999996</v>
@@ -4886,7 +4886,7 @@
         <v>0.20858472522480201</v>
       </c>
       <c r="D107" s="4">
-        <v>260.72371644999998</v>
+        <v>15.352304427524301</v>
       </c>
       <c r="E107" s="5">
         <v>29</v>
@@ -4894,8 +4894,8 @@
       <c r="F107" s="9">
         <v>1.63015493456653E-4</v>
       </c>
-      <c r="G107">
-        <v>4.8651899684200002</v>
+      <c r="G107" s="9">
+        <v>3.2831940733979399E-4</v>
       </c>
       <c r="H107" s="4">
         <v>245.64631846099999</v>
@@ -4904,10 +4904,10 @@
         <v>29</v>
       </c>
       <c r="J107">
-        <v>3.9180000000000001</v>
+        <v>6.2613365072224604E-3</v>
       </c>
       <c r="K107">
-        <v>15.997199999999999</v>
+        <v>4.7275177059124296</v>
       </c>
       <c r="L107" s="4">
         <v>108322.7016</v>
@@ -4929,15 +4929,17 @@
       <c r="C108">
         <v>3.47867635905145</v>
       </c>
-      <c r="D108" s="4"/>
+      <c r="D108" s="4">
+        <v>29.777237208498001</v>
+      </c>
       <c r="E108" s="6">
         <v>30</v>
       </c>
       <c r="F108" s="9">
         <v>3.7548910199425301E-4</v>
       </c>
-      <c r="G108">
-        <v>2.4279092316500002</v>
+      <c r="G108" s="9">
+        <v>3.60907261502063E-4</v>
       </c>
       <c r="H108" s="4">
         <v>213.11110060199999</v>
@@ -4946,10 +4948,10 @@
         <v>30</v>
       </c>
       <c r="J108">
-        <v>2.8403999999999998</v>
+        <v>6.2613365072224604E-3</v>
       </c>
       <c r="K108">
-        <v>8086.6124</v>
+        <v>6.6740234087917898</v>
       </c>
       <c r="L108" s="4">
         <v>123046.4964</v>
@@ -4975,7 +4977,7 @@
       </c>
       <c r="D109" s="7">
         <f>_xlfn.STDEV.S(D79:D107)</f>
-        <v>101.94497098980156</v>
+        <v>4.9502680979130753</v>
       </c>
       <c r="E109" s="7"/>
       <c r="F109" s="7">
@@ -4984,7 +4986,7 @@
       </c>
       <c r="G109" s="7">
         <f>_xlfn.STDEV.S(G79:G108)</f>
-        <v>3.3729706288617907</v>
+        <v>1.6059715741623335E-4</v>
       </c>
       <c r="H109" s="7">
         <f>_xlfn.STDEV.S(H79:H108)</f>
@@ -4993,11 +4995,11 @@
       <c r="I109" s="7"/>
       <c r="J109" s="7">
         <f>_xlfn.STDEV.S(J79:J108)</f>
-        <v>35.220818472206716</v>
+        <v>0.13504355210965172</v>
       </c>
       <c r="K109" s="7">
         <f>_xlfn.STDEV.S(K79:K108)</f>
-        <v>3989.7994539180936</v>
+        <v>2.3445987678520561</v>
       </c>
       <c r="L109" s="7">
         <f>_xlfn.STDEV.S(L79:L108)</f>
@@ -5023,7 +5025,7 @@
       </c>
       <c r="D110" s="7">
         <f t="shared" si="2"/>
-        <v>142.94833057935256</v>
+        <v>26.962077145068445</v>
       </c>
       <c r="E110" s="7"/>
       <c r="F110" s="7">
@@ -5032,7 +5034,7 @@
       </c>
       <c r="G110" s="7">
         <f t="shared" si="2"/>
-        <v>3.6602563426305332</v>
+        <v>4.0223355266233034E-4</v>
       </c>
       <c r="H110" s="7">
         <f t="shared" si="2"/>
@@ -5041,11 +5043,11 @@
       <c r="I110" s="7"/>
       <c r="J110" s="7">
         <f t="shared" si="2"/>
-        <v>19.858040000000003</v>
+        <v>5.8623430512223643E-2</v>
       </c>
       <c r="K110" s="7">
         <f t="shared" si="2"/>
-        <v>2778.6943066666663</v>
+        <v>3.2678913957656874</v>
       </c>
       <c r="L110" s="7">
         <f t="shared" si="2"/>

</xml_diff>

<commit_message>
Genetic algorithm main classes for all functions
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="19">
   <si>
     <t>Rastrigin</t>
   </si>
@@ -48,12 +48,6 @@
   </si>
   <si>
     <t>Generations = 200</t>
-  </si>
-  <si>
-    <t>Algoritm Genetic [pop_size=50,crossover_pbb=0.4,mutation_pbb=0.1]</t>
-  </si>
-  <si>
-    <t>12.258187238.352997533613895908</t>
   </si>
   <si>
     <t>Hibridizare [pop_size=50,crossover_pbb=0.4,mutation_pbb=0.1, hillcimbing_pbb=0.3]</t>
@@ -81,6 +75,12 @@
   </si>
   <si>
     <t>Hill Climbing - First Improvement</t>
+  </si>
+  <si>
+    <t>Algoritm Genetic [pop_size=100,crossover_pbb=0.4,mutation_pbb=0.1]</t>
+  </si>
+  <si>
+    <t>Generations = 1000</t>
   </si>
 </sst>
 </file>
@@ -266,6 +266,9 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -278,9 +281,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="11" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -698,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F16" workbookViewId="0">
-      <selection activeCell="N36" sqref="N36"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="N43" sqref="N43:N72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -713,38 +713,38 @@
   <sheetData>
     <row r="1" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="12" t="s">
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="12" t="s">
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="14" t="s">
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="15"/>
+      <c r="N3" s="18"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
@@ -793,13 +793,13 @@
         <v>0</v>
       </c>
       <c r="Q4" t="s">
+        <v>10</v>
+      </c>
+      <c r="R4" t="s">
+        <v>11</v>
+      </c>
+      <c r="S4" t="s">
         <v>12</v>
-      </c>
-      <c r="R4" t="s">
-        <v>13</v>
-      </c>
-      <c r="S4" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.55000000000000004">
@@ -846,15 +846,15 @@
         <v>-0.97056248757917196</v>
       </c>
       <c r="P5" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q5" s="16">
+        <v>13</v>
+      </c>
+      <c r="Q5" s="12">
         <f>AVERAGE(B5:B34)</f>
         <v>12.46627977627489</v>
       </c>
-      <c r="R5" s="17">
+      <c r="R5" s="13">
         <f>AVERAGE(B43:B72)</f>
-        <v>29.668413300958274</v>
+        <v>6.3035194433569002</v>
       </c>
       <c r="S5">
         <f>AVERAGE(B81:B110)</f>
@@ -905,15 +905,15 @@
         <v>-0.74784721613453697</v>
       </c>
       <c r="P6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="Q6">
         <f>AVERAGE(C5:C34)</f>
         <v>31.655790932304605</v>
       </c>
-      <c r="R6" s="17">
+      <c r="R6" s="13">
         <f>AVERAGE(C43:C72)</f>
-        <v>95.530584825396929</v>
+        <v>26.938666239964512</v>
       </c>
       <c r="S6">
         <f>AVERAGE(C81:C110)</f>
@@ -964,15 +964,15 @@
         <v>-0.982009523598117</v>
       </c>
       <c r="P7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="Q7">
         <f>AVERAGE(D5:D34)</f>
         <v>85.050965060569709</v>
       </c>
-      <c r="R7" s="17">
+      <c r="R7" s="13">
         <f>AVERAGE(D43:D72)</f>
-        <v>405.19167140112046</v>
+        <v>282.30599825191518</v>
       </c>
       <c r="S7">
         <f>AVERAGE(D81:D110)</f>
@@ -1202,13 +1202,13 @@
         <v>1</v>
       </c>
       <c r="Q12" t="s">
+        <v>10</v>
+      </c>
+      <c r="R12" t="s">
+        <v>11</v>
+      </c>
+      <c r="S12" t="s">
         <v>12</v>
-      </c>
-      <c r="R12" t="s">
-        <v>13</v>
-      </c>
-      <c r="S12" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.55000000000000004">
@@ -1255,7 +1255,7 @@
         <v>-0.99511469963927401</v>
       </c>
       <c r="P13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Q13">
         <f>AVERAGE(F5:F34)</f>
@@ -1263,7 +1263,7 @@
       </c>
       <c r="R13">
         <f>AVERAGE(F43:F72)</f>
-        <v>19.645804055543941</v>
+        <v>0.41764158474993984</v>
       </c>
       <c r="S13" s="9">
         <f>AVERAGE(F81:F110)</f>
@@ -1314,7 +1314,7 @@
         <v>-1.0241175434207299</v>
       </c>
       <c r="P14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="Q14">
         <f>AVERAGE(G5:G34)</f>
@@ -1322,7 +1322,7 @@
       </c>
       <c r="R14">
         <f>AVERAGE(G43:G72)</f>
-        <v>95.39189242008959</v>
+        <v>3.8225688900805368</v>
       </c>
       <c r="S14" s="9">
         <f>AVERAGE(G81:G110)</f>
@@ -1373,7 +1373,7 @@
         <v>-0.99550048954989001</v>
       </c>
       <c r="P15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="Q15">
         <f>AVERAGE(H5:H34)</f>
@@ -1381,7 +1381,7 @@
       </c>
       <c r="R15">
         <f>AVERAGE(H43:H72)</f>
-        <v>520.38446509449091</v>
+        <v>293.12291565609064</v>
       </c>
       <c r="S15" s="9">
         <f>AVERAGE(H81:H110)</f>
@@ -1611,13 +1611,13 @@
         <v>2</v>
       </c>
       <c r="Q20" t="s">
+        <v>10</v>
+      </c>
+      <c r="R20" t="s">
+        <v>11</v>
+      </c>
+      <c r="S20" t="s">
         <v>12</v>
-      </c>
-      <c r="R20" t="s">
-        <v>13</v>
-      </c>
-      <c r="S20" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.55000000000000004">
@@ -1664,7 +1664,7 @@
         <v>-0.75312481486496696</v>
       </c>
       <c r="P21" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Q21">
         <f>AVERAGE(J5:J34)</f>
@@ -1672,7 +1672,7 @@
       </c>
       <c r="R21">
         <f>AVERAGE(J43:J72)</f>
-        <v>53.850898488580633</v>
+        <v>4.2569915407155747</v>
       </c>
       <c r="S21">
         <f>AVERAGE(J81:J110)</f>
@@ -1723,7 +1723,7 @@
         <v>-1.02992784328481</v>
       </c>
       <c r="P22" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="Q22">
         <f>AVERAGE(K5:K34)</f>
@@ -1731,7 +1731,7 @@
       </c>
       <c r="R22">
         <f>AVERAGE(K43:K72)</f>
-        <v>527.4909876682932</v>
+        <v>35.871749467243987</v>
       </c>
       <c r="S22">
         <f>AVERAGE(K81:K110)</f>
@@ -1782,7 +1782,7 @@
         <v>-0.70306507946305796</v>
       </c>
       <c r="P23" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="Q23">
         <f>AVERAGE(L5:L34)</f>
@@ -1790,7 +1790,7 @@
       </c>
       <c r="R23">
         <f>AVERAGE(L43:L72)</f>
-        <v>10039.443821531866</v>
+        <v>1327.7639171965789</v>
       </c>
       <c r="S23">
         <f>AVERAGE(L81:L110)</f>
@@ -2020,13 +2020,13 @@
         <v>3</v>
       </c>
       <c r="Q28" t="s">
+        <v>10</v>
+      </c>
+      <c r="R28" t="s">
+        <v>11</v>
+      </c>
+      <c r="S28" t="s">
         <v>12</v>
-      </c>
-      <c r="R28" t="s">
-        <v>13</v>
-      </c>
-      <c r="S28" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.55000000000000004">
@@ -2073,7 +2073,7 @@
         <v>-1.0308900958220399</v>
       </c>
       <c r="P29" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Q29">
         <f>AVERAGE(N5:N34)</f>
@@ -2081,7 +2081,7 @@
       </c>
       <c r="R29">
         <f>AVERAGE(N43:N72)</f>
-        <v>-1.003598585696712</v>
+        <v>-0.88030405655166488</v>
       </c>
       <c r="S29">
         <f>AVERAGE(N81:N110)</f>
@@ -2406,10 +2406,10 @@
     </row>
     <row r="39" spans="1:14" ht="20.399999999999999" x14ac:dyDescent="0.75">
       <c r="A39" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
@@ -2420,28 +2420,28 @@
       <c r="J39" s="10"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="12" t="s">
+      <c r="A41" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B41" s="12"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="12" t="s">
+      <c r="B41" s="15"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="F41" s="12"/>
-      <c r="G41" s="12"/>
-      <c r="H41" s="13"/>
-      <c r="I41" s="12" t="s">
+      <c r="F41" s="15"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="16"/>
+      <c r="I41" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="J41" s="12"/>
-      <c r="K41" s="12"/>
-      <c r="L41" s="13"/>
-      <c r="M41" s="14" t="s">
+      <c r="J41" s="15"/>
+      <c r="K41" s="15"/>
+      <c r="L41" s="16"/>
+      <c r="M41" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="N41" s="15"/>
+      <c r="N41" s="18"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="1" t="s">
@@ -2492,43 +2492,43 @@
         <v>1</v>
       </c>
       <c r="B43">
-        <v>28.2758676276001</v>
+        <v>2.1163381076173202</v>
       </c>
       <c r="C43">
-        <v>106.27582968890501</v>
-      </c>
-      <c r="D43" s="4">
-        <v>377.17587677000802</v>
+        <v>22.476191210003901</v>
+      </c>
+      <c r="D43">
+        <v>283.09733776411002</v>
       </c>
       <c r="E43" s="3">
         <v>1</v>
       </c>
       <c r="F43">
-        <v>17.312161788346302</v>
+        <v>0.57165005641437305</v>
       </c>
       <c r="G43">
-        <v>116.318401546345</v>
-      </c>
-      <c r="H43" s="4">
-        <v>529.29139347668797</v>
+        <v>5.2727911963315002</v>
+      </c>
+      <c r="H43">
+        <v>401.63116814442998</v>
       </c>
       <c r="I43" s="3">
         <v>1</v>
       </c>
       <c r="J43">
-        <v>72.937694924152396</v>
+        <v>3.8834967685808399</v>
       </c>
       <c r="K43">
-        <v>669.48974729520705</v>
-      </c>
-      <c r="L43" s="4">
-        <v>2212.6555720992701</v>
+        <v>40.5339785995236</v>
+      </c>
+      <c r="L43">
+        <v>1616.4914864316099</v>
       </c>
       <c r="M43" s="3">
         <v>1</v>
       </c>
-      <c r="N43" s="4">
-        <v>-1.02732441138881</v>
+      <c r="N43">
+        <v>-1.0277840748264</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -2536,43 +2536,43 @@
         <v>2</v>
       </c>
       <c r="B44">
-        <v>28.330123480707801</v>
+        <v>7.79063631256217</v>
       </c>
       <c r="C44">
-        <v>104.054330503274</v>
-      </c>
-      <c r="D44" s="4">
-        <v>388.84387136343798</v>
+        <v>33.225264518897497</v>
+      </c>
+      <c r="D44">
+        <v>258.75205398581801</v>
       </c>
       <c r="E44" s="5">
         <v>2</v>
       </c>
       <c r="F44">
-        <v>11.184149897808</v>
+        <v>0.84790488063509495</v>
       </c>
       <c r="G44">
-        <v>112.165842824301</v>
-      </c>
-      <c r="H44" s="4">
-        <v>453.42186877921398</v>
+        <v>2.39454443132548</v>
+      </c>
+      <c r="H44">
+        <v>357.16348956822998</v>
       </c>
       <c r="I44" s="5">
         <v>2</v>
       </c>
       <c r="J44">
-        <v>75.2110443973489</v>
+        <v>3.0626094155268899</v>
       </c>
       <c r="K44">
-        <v>354.41347430441198</v>
-      </c>
-      <c r="L44" s="4">
-        <v>6976.07308023522</v>
+        <v>9.3780664877674909</v>
+      </c>
+      <c r="L44">
+        <v>1648.4334239739601</v>
       </c>
       <c r="M44" s="5">
         <v>2</v>
       </c>
-      <c r="N44" s="4">
-        <v>-1.0104042726026301</v>
+      <c r="N44">
+        <v>-0.79087542891977403</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -2580,43 +2580,43 @@
         <v>3</v>
       </c>
       <c r="B45">
-        <v>32.877104628543101</v>
+        <v>5.2435579027770496</v>
       </c>
       <c r="C45">
-        <v>81.9422336847705</v>
-      </c>
-      <c r="D45" s="4">
-        <v>426.20721782317702</v>
+        <v>20.879368522773898</v>
+      </c>
+      <c r="D45">
+        <v>337.47213682682599</v>
       </c>
       <c r="E45" s="5">
         <v>3</v>
       </c>
       <c r="F45">
-        <v>21.404673696270699</v>
+        <v>0.190683456421396</v>
       </c>
       <c r="G45">
-        <v>98.832905458991405</v>
-      </c>
-      <c r="H45" s="4">
-        <v>563.85688737868895</v>
+        <v>2.7561095754454801</v>
+      </c>
+      <c r="H45">
+        <v>298.03185470900797</v>
       </c>
       <c r="I45" s="5">
         <v>3</v>
       </c>
       <c r="J45">
-        <v>25.375713229956499</v>
+        <v>4.31599106162101</v>
       </c>
       <c r="K45">
-        <v>148.070279249485</v>
-      </c>
-      <c r="L45" s="4">
-        <v>4665.0600506268502</v>
+        <v>12.3837466419977</v>
+      </c>
+      <c r="L45">
+        <v>1648.58634872579</v>
       </c>
       <c r="M45" s="5">
         <v>3</v>
       </c>
-      <c r="N45" s="4">
-        <v>-1.0062512475861001</v>
+      <c r="N45">
+        <v>-0.57820980712307402</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -2624,43 +2624,43 @@
         <v>4</v>
       </c>
       <c r="B46">
-        <v>38.315546725854297</v>
+        <v>15.0447193482364</v>
       </c>
       <c r="C46">
-        <v>106.99753195034</v>
-      </c>
-      <c r="D46" s="4">
-        <v>403.41887172396599</v>
+        <v>35.258649890191997</v>
+      </c>
+      <c r="D46">
+        <v>267.85935767022397</v>
       </c>
       <c r="E46" s="5">
         <v>4</v>
       </c>
       <c r="F46">
-        <v>6.5342951567957597</v>
+        <v>0.40999066716966698</v>
       </c>
       <c r="G46">
-        <v>124.915205944278</v>
-      </c>
-      <c r="H46" s="4">
-        <v>432.83473177965499</v>
+        <v>2.99098442647372</v>
+      </c>
+      <c r="H46">
+        <v>383.05714694038198</v>
       </c>
       <c r="I46" s="5">
         <v>4</v>
       </c>
       <c r="J46">
-        <v>32.415233346370599</v>
+        <v>4.0158680952489503</v>
       </c>
       <c r="K46">
-        <v>425.62170464830501</v>
-      </c>
-      <c r="L46" s="4">
-        <v>4331.4797394126299</v>
+        <v>122.569994761755</v>
+      </c>
+      <c r="L46">
+        <v>2235.4100382709598</v>
       </c>
       <c r="M46" s="5">
         <v>4</v>
       </c>
-      <c r="N46" s="4">
-        <v>-0.970582905676593</v>
+      <c r="N46">
+        <v>-0.73955251378164699</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -2668,43 +2668,43 @@
         <v>5</v>
       </c>
       <c r="B47">
-        <v>28.943261062467698</v>
+        <v>7.9391271135853501</v>
       </c>
       <c r="C47">
-        <v>87.326520679952395</v>
-      </c>
-      <c r="D47" s="4">
-        <v>402.61639336285202</v>
+        <v>23.0264047665578</v>
+      </c>
+      <c r="D47">
+        <v>208.46794782709401</v>
       </c>
       <c r="E47" s="5">
         <v>5</v>
       </c>
       <c r="F47">
-        <v>9.6308251690420903</v>
+        <v>0.39144609197181601</v>
       </c>
       <c r="G47">
-        <v>87.867943923521693</v>
-      </c>
-      <c r="H47" s="4">
-        <v>562.83591439311499</v>
+        <v>3.5945115892416299</v>
+      </c>
+      <c r="H47">
+        <v>185.21691363543701</v>
       </c>
       <c r="I47" s="5">
         <v>5</v>
       </c>
       <c r="J47">
-        <v>97.484552948229194</v>
+        <v>4.4386102728132704</v>
       </c>
       <c r="K47">
-        <v>285.01365462592003</v>
-      </c>
-      <c r="L47" s="4">
-        <v>5830.3522313526801</v>
+        <v>7.2160697459891301</v>
+      </c>
+      <c r="L47">
+        <v>1133.9936296619101</v>
       </c>
       <c r="M47" s="5">
         <v>5</v>
       </c>
-      <c r="N47" s="4">
-        <v>-1.0277685575066999</v>
+      <c r="N47">
+        <v>-1.02620690035041</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -2712,43 +2712,43 @@
         <v>6</v>
       </c>
       <c r="B48">
-        <v>21.9529677641621</v>
+        <v>5.5748348931797</v>
       </c>
       <c r="C48">
-        <v>90.752833926731995</v>
-      </c>
-      <c r="D48" s="4">
-        <v>419.96880452141198</v>
+        <v>32.369075634811999</v>
+      </c>
+      <c r="D48">
+        <v>283.76970177733398</v>
       </c>
       <c r="E48" s="5">
         <v>6</v>
       </c>
       <c r="F48">
-        <v>23.6081928429392</v>
+        <v>0.20281241205522599</v>
       </c>
       <c r="G48">
-        <v>128.53172354217</v>
-      </c>
-      <c r="H48" s="4">
-        <v>551.49775336644302</v>
+        <v>1.32993099213671</v>
+      </c>
+      <c r="H48">
+        <v>207.85684514082499</v>
       </c>
       <c r="I48" s="5">
         <v>6</v>
       </c>
       <c r="J48">
-        <v>15.825501183584301</v>
+        <v>4.2606587658938899</v>
       </c>
       <c r="K48">
-        <v>345.23058139567797</v>
-      </c>
-      <c r="L48" s="4">
-        <v>6246.4370987726497</v>
+        <v>13.1606896703372</v>
+      </c>
+      <c r="L48">
+        <v>1112.6404568156599</v>
       </c>
       <c r="M48" s="5">
         <v>6</v>
       </c>
-      <c r="N48" s="4">
-        <v>-1.0292333137148999</v>
+      <c r="N48">
+        <v>-0.99550048954989001</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -2756,43 +2756,43 @@
         <v>7</v>
       </c>
       <c r="B49">
-        <v>26.6141145947343</v>
+        <v>6.7607190165930904</v>
       </c>
       <c r="C49">
-        <v>105.13358432462201</v>
-      </c>
-      <c r="D49" s="4">
-        <v>398.71386624283599</v>
+        <v>32.272514136237298</v>
+      </c>
+      <c r="D49">
+        <v>222.25219652356199</v>
       </c>
       <c r="E49" s="5">
         <v>7</v>
       </c>
       <c r="F49">
-        <v>11.7458172073956</v>
+        <v>0.161450850149613</v>
       </c>
       <c r="G49">
-        <v>104.01113060407</v>
-      </c>
-      <c r="H49" s="4">
-        <v>503.999188867915</v>
+        <v>5.7511961492763097</v>
+      </c>
+      <c r="H49">
+        <v>167.77591781983199</v>
       </c>
       <c r="I49" s="5">
         <v>7</v>
       </c>
       <c r="J49">
-        <v>105.327897134154</v>
+        <v>3.9632247038700701</v>
       </c>
       <c r="K49">
-        <v>507.99738037682198</v>
-      </c>
-      <c r="L49" s="4">
-        <v>5509.51522065473</v>
+        <v>14.3971283424374</v>
+      </c>
+      <c r="L49">
+        <v>1557.34629795055</v>
       </c>
       <c r="M49" s="5">
         <v>7</v>
       </c>
-      <c r="N49" s="4">
-        <v>-1.0213708230949401</v>
+      <c r="N49">
+        <v>-0.88813820928890497</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -2800,43 +2800,43 @@
         <v>8</v>
       </c>
       <c r="B50">
-        <v>26.730492836003801</v>
+        <v>2.4397426003539602</v>
       </c>
       <c r="C50">
-        <v>101.64449829116199</v>
-      </c>
-      <c r="D50" s="4">
-        <v>419.22964548702902</v>
+        <v>40.650358241754098</v>
+      </c>
+      <c r="D50">
+        <v>308.612958399805</v>
       </c>
       <c r="E50" s="5">
         <v>8</v>
       </c>
       <c r="F50">
-        <v>23.877329501301201</v>
+        <v>0.70576411068940403</v>
       </c>
       <c r="G50">
-        <v>75.989091984055605</v>
-      </c>
-      <c r="H50" s="4">
-        <v>550.36027457572095</v>
+        <v>4.0047819242539102</v>
+      </c>
+      <c r="H50">
+        <v>213.89686292998201</v>
       </c>
       <c r="I50" s="5">
         <v>8</v>
       </c>
       <c r="J50">
-        <v>103.77342321723</v>
+        <v>4.1981765301922902</v>
       </c>
       <c r="K50">
-        <v>522.08640756144405</v>
-      </c>
-      <c r="L50" s="4">
-        <v>4843.4619039437102</v>
+        <v>94.309054521031399</v>
+      </c>
+      <c r="L50">
+        <v>1239.38052198168</v>
       </c>
       <c r="M50" s="5">
         <v>8</v>
       </c>
-      <c r="N50" s="4">
-        <v>-1.00749954388456</v>
+      <c r="N50">
+        <v>-0.94783075637275505</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -2844,43 +2844,43 @@
         <v>9</v>
       </c>
       <c r="B51">
-        <v>37.714205021931697</v>
+        <v>2.5798803444127301</v>
       </c>
       <c r="C51">
-        <v>104.964256398449</v>
-      </c>
-      <c r="D51" s="4">
-        <v>437.70605320643199</v>
+        <v>21.2115094773194</v>
+      </c>
+      <c r="D51">
+        <v>240.48467709758501</v>
       </c>
       <c r="E51" s="5">
         <v>9</v>
       </c>
       <c r="F51">
-        <v>18.778696754910399</v>
+        <v>0.71336583240916496</v>
       </c>
       <c r="G51">
-        <v>86.454623551348305</v>
-      </c>
-      <c r="H51" s="4">
-        <v>493.88255114780497</v>
+        <v>5.1214145602991401</v>
+      </c>
+      <c r="H51">
+        <v>308.63858886112303</v>
       </c>
       <c r="I51" s="5">
         <v>9</v>
       </c>
       <c r="J51">
-        <v>61.5619960349945</v>
+        <v>2.67834437696134</v>
       </c>
       <c r="K51">
-        <v>646.70098319367196</v>
-      </c>
-      <c r="L51" s="4">
-        <v>6560.4127305603897</v>
+        <v>39.203579151162202</v>
+      </c>
+      <c r="L51">
+        <v>1622.2939290284</v>
       </c>
       <c r="M51" s="5">
         <v>9</v>
       </c>
-      <c r="N51" s="4">
-        <v>-0.96463973036932205</v>
+      <c r="N51">
+        <v>-0.96557603709315298</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -2888,43 +2888,43 @@
         <v>10</v>
       </c>
       <c r="B52">
-        <v>23.785737030828201</v>
+        <v>5.0872420579817597</v>
       </c>
       <c r="C52">
-        <v>108.058001401232</v>
-      </c>
-      <c r="D52" s="4">
-        <v>430.48408182196698</v>
+        <v>36.723894935733597</v>
+      </c>
+      <c r="D52">
+        <v>322.51941235087497</v>
       </c>
       <c r="E52" s="5">
         <v>10</v>
       </c>
       <c r="F52">
-        <v>16.943148202582101</v>
+        <v>0.299668403175259</v>
       </c>
       <c r="G52">
-        <v>103.972981456529</v>
-      </c>
-      <c r="H52" s="4">
-        <v>494.21839219545097</v>
+        <v>2.7542283833266299</v>
+      </c>
+      <c r="H52">
+        <v>366.76023510903201</v>
       </c>
       <c r="I52" s="5">
         <v>10</v>
       </c>
       <c r="J52">
-        <v>94.656161794902999</v>
+        <v>1.63524722843349</v>
       </c>
       <c r="K52">
-        <v>599.53590355543201</v>
-      </c>
-      <c r="L52" s="4">
-        <v>5762.1672675712698</v>
+        <v>9.9975716187547299</v>
+      </c>
+      <c r="L52">
+        <v>1180.76680252249</v>
       </c>
       <c r="M52" s="5">
         <v>10</v>
       </c>
-      <c r="N52" s="4">
-        <v>-1.022553030481</v>
+      <c r="N52">
+        <v>-0.92423442513556098</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -2932,43 +2932,43 @@
         <v>11</v>
       </c>
       <c r="B53">
-        <v>32.301881728792601</v>
+        <v>2.3444667004699502</v>
       </c>
       <c r="C53">
-        <v>95.211113747550101</v>
-      </c>
-      <c r="D53" s="4">
-        <v>372.44187508965098</v>
+        <v>22.386565060811201</v>
+      </c>
+      <c r="D53">
+        <v>336.77101653010499</v>
       </c>
       <c r="E53" s="5">
         <v>11</v>
       </c>
       <c r="F53">
-        <v>22.288174912886198</v>
+        <v>0.48893068869817702</v>
       </c>
       <c r="G53">
-        <v>72.085358218364902</v>
-      </c>
-      <c r="H53" s="4">
-        <v>504.93329714921401</v>
+        <v>2.04089653253435</v>
+      </c>
+      <c r="H53">
+        <v>308.82452233606</v>
       </c>
       <c r="I53" s="5">
         <v>11</v>
       </c>
       <c r="J53">
-        <v>31.678909337258201</v>
+        <v>0.29756585143618303</v>
       </c>
       <c r="K53">
-        <v>918.05689089370799</v>
-      </c>
-      <c r="L53" s="4">
-        <v>7032.68117280755</v>
+        <v>5.8282901389889199</v>
+      </c>
+      <c r="L53">
+        <v>970.69749448106495</v>
       </c>
       <c r="M53" s="5">
         <v>11</v>
       </c>
-      <c r="N53" s="4">
-        <v>-1.0171519805646101</v>
+      <c r="N53">
+        <v>-0.791501840110856</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -2976,43 +2976,43 @@
         <v>12</v>
       </c>
       <c r="B54">
-        <v>17.932531006400001</v>
+        <v>2.0766146665004399</v>
       </c>
       <c r="C54">
-        <v>74.246610334877701</v>
-      </c>
-      <c r="D54" s="4">
-        <v>421.52604045272898</v>
+        <v>27.959165905513899</v>
+      </c>
+      <c r="D54">
+        <v>263.24922947249502</v>
       </c>
       <c r="E54" s="5">
         <v>12</v>
       </c>
       <c r="F54">
-        <v>9.3317266357990594</v>
+        <v>0.115626180623745</v>
       </c>
       <c r="G54">
-        <v>88.723988729692806</v>
-      </c>
-      <c r="H54" s="4">
-        <v>624.692565024239</v>
+        <v>3.3201120195714502</v>
+      </c>
+      <c r="H54">
+        <v>205.57582112808001</v>
       </c>
       <c r="I54" s="5">
         <v>12</v>
       </c>
       <c r="J54">
-        <v>35.034108306642501</v>
+        <v>4.2639742678585204</v>
       </c>
       <c r="K54">
-        <v>308.97461418624601</v>
-      </c>
-      <c r="L54" s="4">
-        <v>5437.2740694412196</v>
+        <v>11.565356639528501</v>
+      </c>
+      <c r="L54">
+        <v>1062.9647699627899</v>
       </c>
       <c r="M54" s="5">
         <v>12</v>
       </c>
-      <c r="N54" s="4">
-        <v>-0.98720849379143405</v>
+      <c r="N54">
+        <v>-0.73019004815709099</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3020,43 +3020,43 @@
         <v>13</v>
       </c>
       <c r="B55">
-        <v>25.917707445762201</v>
+        <v>7.4434536804093101</v>
       </c>
       <c r="C55">
-        <v>75.048460271215504</v>
-      </c>
-      <c r="D55" s="4">
-        <v>427.008736375019</v>
+        <v>25.950639386757601</v>
+      </c>
+      <c r="D55">
+        <v>286.02242693852003</v>
       </c>
       <c r="E55" s="5">
         <v>13</v>
       </c>
       <c r="F55">
-        <v>19.337345179925901</v>
+        <v>0.31911033582825099</v>
       </c>
       <c r="G55">
-        <v>69.884888087872895</v>
-      </c>
-      <c r="H55" s="4">
-        <v>514.389829811254</v>
+        <v>1.74703865452176</v>
+      </c>
+      <c r="H55">
+        <v>374.064647432556</v>
       </c>
       <c r="I55" s="5">
         <v>13</v>
       </c>
       <c r="J55">
-        <v>60.403410873275099</v>
+        <v>3.4094216031065701</v>
       </c>
       <c r="K55">
-        <v>596.10020208640503</v>
-      </c>
-      <c r="L55" s="4">
-        <v>6251.0983815064701</v>
+        <v>9.7282317445694702</v>
+      </c>
+      <c r="L55">
+        <v>1446.0164478678</v>
       </c>
       <c r="M55" s="5">
         <v>13</v>
       </c>
-      <c r="N55" s="4">
-        <v>-1.00697125889183</v>
+      <c r="N55">
+        <v>-0.57820980712307402</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3064,43 +3064,43 @@
         <v>14</v>
       </c>
       <c r="B56">
-        <v>37.187680960567199</v>
+        <v>2.1244104040283198</v>
       </c>
       <c r="C56">
-        <v>101.708545664122</v>
-      </c>
-      <c r="D56" s="4">
-        <v>411.03125408335097</v>
+        <v>24.5556509479621</v>
+      </c>
+      <c r="D56">
+        <v>278.23348448090701</v>
       </c>
       <c r="E56" s="5">
         <v>14</v>
       </c>
       <c r="F56">
-        <v>27.818188535299999</v>
+        <v>0.56573055693238805</v>
       </c>
       <c r="G56">
-        <v>127.65634069200399</v>
-      </c>
-      <c r="H56" s="4">
-        <v>465.509562633114</v>
+        <v>9.9110432091363307</v>
+      </c>
+      <c r="H56">
+        <v>218.92611087050199</v>
       </c>
       <c r="I56" s="5">
         <v>14</v>
       </c>
       <c r="J56">
-        <v>62.942534767280897</v>
+        <v>5.65238588954624</v>
       </c>
       <c r="K56">
-        <v>658.52161841009899</v>
-      </c>
-      <c r="L56" s="4">
-        <v>5308.1995455246197</v>
+        <v>36.9159285832149</v>
+      </c>
+      <c r="L56">
+        <v>788.99683813917898</v>
       </c>
       <c r="M56" s="5">
         <v>14</v>
       </c>
-      <c r="N56" s="4">
-        <v>-0.99072545193717199</v>
+      <c r="N56">
+        <v>-1.0277840748264</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3108,43 +3108,43 @@
         <v>15</v>
       </c>
       <c r="B57">
-        <v>20.5440863493805</v>
+        <v>4.0253512314989699</v>
       </c>
       <c r="C57">
-        <v>78.629480210276498</v>
-      </c>
-      <c r="D57" s="4">
-        <v>385.339869418288</v>
+        <v>20.148689306148501</v>
+      </c>
+      <c r="D57">
+        <v>261.70645986825002</v>
       </c>
       <c r="E57" s="5">
         <v>15</v>
       </c>
       <c r="F57">
-        <v>32.570681720028198</v>
+        <v>5.2261685760460801E-2</v>
       </c>
       <c r="G57">
-        <v>102.927511166801</v>
-      </c>
-      <c r="H57" s="4">
-        <v>467.22580163694602</v>
+        <v>1.74750201246564</v>
+      </c>
+      <c r="H57">
+        <v>201.49948669223301</v>
       </c>
       <c r="I57" s="5">
         <v>15</v>
       </c>
       <c r="J57">
-        <v>13.634399999999999</v>
+        <v>4.9141542864741998</v>
       </c>
       <c r="K57">
-        <v>580.17634245676004</v>
-      </c>
-      <c r="L57" s="4">
-        <v>5035.1028968135497</v>
+        <v>16.536864336441099</v>
+      </c>
+      <c r="L57">
+        <v>1460.5053578185</v>
       </c>
       <c r="M57" s="5">
         <v>15</v>
       </c>
-      <c r="N57" s="4">
-        <v>-1.0112694956197901</v>
+      <c r="N57">
+        <v>-0.86100014827261895</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3152,43 +3152,43 @@
         <v>16</v>
       </c>
       <c r="B58">
-        <v>25.484631991383502</v>
+        <v>12.9418602223646</v>
       </c>
       <c r="C58">
-        <v>103.41336767995</v>
-      </c>
-      <c r="D58" s="4">
-        <v>359.71101665336101</v>
+        <v>24.608740872808902</v>
+      </c>
+      <c r="D58">
+        <v>301.65810844652799</v>
       </c>
       <c r="E58" s="5">
         <v>16</v>
       </c>
       <c r="F58">
-        <v>29.629850828580999</v>
+        <v>0.46316696364092502</v>
       </c>
       <c r="G58">
-        <v>56.839365004756303</v>
-      </c>
-      <c r="H58" s="4">
-        <v>534.01484870908598</v>
+        <v>13.1774258389612</v>
+      </c>
+      <c r="H58">
+        <v>267.98003574813902</v>
       </c>
       <c r="I58" s="5">
         <v>16</v>
       </c>
       <c r="J58">
-        <v>12.571863552210401</v>
+        <v>4.2959586466674002</v>
       </c>
       <c r="K58">
-        <v>646.24431810439603</v>
-      </c>
-      <c r="L58" s="4">
-        <v>5612.21748862811</v>
+        <v>24.636599802261699</v>
+      </c>
+      <c r="L58">
+        <v>1907.6749614401001</v>
       </c>
       <c r="M58" s="5">
         <v>16</v>
       </c>
-      <c r="N58" s="4">
-        <v>-0.99147323787182495</v>
+      <c r="N58">
+        <v>-0.85978643865708004</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3196,43 +3196,43 @@
         <v>17</v>
       </c>
       <c r="B59">
-        <v>21.0908222962038</v>
+        <v>8.4814417818583703</v>
       </c>
       <c r="C59">
-        <v>102.04499829890899</v>
-      </c>
-      <c r="D59" s="4">
-        <v>451.63229410391898</v>
+        <v>19.9385228831832</v>
+      </c>
+      <c r="D59">
+        <v>317.33793322843297</v>
       </c>
       <c r="E59" s="5">
         <v>17</v>
       </c>
       <c r="F59">
-        <v>11.943917521008901</v>
+        <v>0.17447568031196001</v>
       </c>
       <c r="G59">
-        <v>18.4346515834333</v>
-      </c>
-      <c r="H59" s="4">
-        <v>565.87320194357096</v>
+        <v>6.1113631873471599</v>
+      </c>
+      <c r="H59">
+        <v>320.20050807265301</v>
       </c>
       <c r="I59" s="5">
         <v>17</v>
       </c>
       <c r="J59">
-        <v>78.071857412048104</v>
+        <v>3.9632247038700701</v>
       </c>
       <c r="K59">
-        <v>546.55146522913299</v>
-      </c>
-      <c r="L59" s="4">
-        <v>4857.1153969383404</v>
+        <v>54.747085522621497</v>
+      </c>
+      <c r="L59">
+        <v>851.25305508215604</v>
       </c>
       <c r="M59" s="5">
         <v>17</v>
       </c>
-      <c r="N59" s="4">
-        <v>-0.94526708873528698</v>
+      <c r="N59">
+        <v>-0.88943681607381297</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3240,87 +3240,87 @@
         <v>18</v>
       </c>
       <c r="B60">
-        <v>33.414928361052297</v>
+        <v>8.7808370580090092</v>
       </c>
       <c r="C60">
-        <v>99.403121983206802</v>
-      </c>
-      <c r="D60" s="4">
-        <v>447.81542617535598</v>
+        <v>24.314396997244199</v>
+      </c>
+      <c r="D60">
+        <v>273.33969522774998</v>
       </c>
       <c r="E60" s="5">
         <v>18</v>
       </c>
       <c r="F60">
-        <v>17.423861072420902</v>
+        <v>0.126895308316644</v>
       </c>
       <c r="G60">
-        <v>88.902775038860398</v>
-      </c>
-      <c r="H60" s="4">
-        <v>452.57357283358698</v>
+        <v>1.9232029532402</v>
+      </c>
+      <c r="H60">
+        <v>305.17096113574399</v>
       </c>
       <c r="I60" s="5">
         <v>18</v>
       </c>
       <c r="J60">
-        <v>14.8611755757192</v>
+        <v>19.5142579985575</v>
       </c>
       <c r="K60">
-        <v>499.694213289966</v>
-      </c>
-      <c r="L60" s="4">
-        <v>5957.31542094631</v>
+        <v>132.02803144365001</v>
+      </c>
+      <c r="L60">
+        <v>1423.24125365193</v>
       </c>
       <c r="M60" s="5">
         <v>18</v>
       </c>
-      <c r="N60" s="4">
-        <v>-0.97564858242666697</v>
+      <c r="N60">
+        <v>-1.0154687734864301</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="5">
         <v>19</v>
       </c>
-      <c r="B61" t="s">
-        <v>9</v>
+      <c r="B61">
+        <v>5.2435579027770496</v>
       </c>
       <c r="C61">
-        <v>87.516831133333</v>
-      </c>
-      <c r="D61" s="4">
-        <v>439.09812535128998</v>
+        <v>40.016704220898703</v>
+      </c>
+      <c r="D61">
+        <v>280.35675607264801</v>
       </c>
       <c r="E61" s="5">
         <v>19</v>
       </c>
       <c r="F61">
-        <v>22.485545037943002</v>
+        <v>0.27187565562141902</v>
       </c>
       <c r="G61">
-        <v>103.98620817910999</v>
-      </c>
-      <c r="H61" s="4">
-        <v>679.62581263844902</v>
+        <v>2.9147890643288799</v>
+      </c>
+      <c r="H61">
+        <v>283.58841576200302</v>
       </c>
       <c r="I61" s="5">
         <v>19</v>
       </c>
       <c r="J61">
-        <v>43.596796325038902</v>
+        <v>5.7351930169396397</v>
       </c>
       <c r="K61">
-        <v>716.04206530578597</v>
-      </c>
-      <c r="L61" s="4">
-        <v>8059.5269095233498</v>
+        <v>11.802907255144</v>
+      </c>
+      <c r="L61">
+        <v>1621.4032552737999</v>
       </c>
       <c r="M61" s="5">
         <v>19</v>
       </c>
-      <c r="N61" s="4">
-        <v>-1.0277685575066999</v>
+      <c r="N61">
+        <v>-0.96047668115104001</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3328,43 +3328,43 @@
         <v>20</v>
       </c>
       <c r="B62">
-        <v>28.192105425703701</v>
+        <v>7.6427554827595703</v>
       </c>
       <c r="C62">
-        <v>81.213582899568095</v>
-      </c>
-      <c r="D62" s="4">
-        <v>340.887415680044</v>
+        <v>25.306290212426099</v>
+      </c>
+      <c r="D62">
+        <v>251.03708822437099</v>
       </c>
       <c r="E62" s="5">
         <v>20</v>
       </c>
       <c r="F62">
-        <v>22.9286279811067</v>
+        <v>0.85406765017763897</v>
       </c>
       <c r="G62">
-        <v>103.98620817910999</v>
-      </c>
-      <c r="H62" s="4">
-        <v>514.23270238552004</v>
+        <v>6.5806982341822602</v>
+      </c>
+      <c r="H62">
+        <v>237.55174387917501</v>
       </c>
       <c r="I62" s="5">
         <v>20</v>
       </c>
       <c r="J62">
-        <v>17.253717903090902</v>
+        <v>4.0115859054995298</v>
       </c>
       <c r="K62">
-        <v>475.18916246549298</v>
-      </c>
-      <c r="L62" s="4">
-        <v>5280.9767876147898</v>
+        <v>12.3202435171996</v>
+      </c>
+      <c r="L62">
+        <v>912.15464707717797</v>
       </c>
       <c r="M62" s="5">
         <v>20</v>
       </c>
-      <c r="N62" s="4">
-        <v>-1.00369855806081</v>
+      <c r="N62">
+        <v>-0.92819829932904896</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3372,43 +3372,43 @@
         <v>21</v>
       </c>
       <c r="B63">
-        <v>30.682257425345199</v>
+        <v>5.08692528300673</v>
       </c>
       <c r="C63">
-        <v>96.371058530286604</v>
-      </c>
-      <c r="D63" s="4">
-        <v>408.89669054667002</v>
+        <v>37.283869678171698</v>
+      </c>
+      <c r="D63">
+        <v>236.761145530866</v>
       </c>
       <c r="E63" s="5">
         <v>21</v>
       </c>
       <c r="F63">
-        <v>15.738618658428701</v>
+        <v>0.71391309563510097</v>
       </c>
       <c r="G63">
-        <v>131.688062034106</v>
-      </c>
-      <c r="H63" s="4">
-        <v>536.10495539951205</v>
+        <v>2.90523152158918</v>
+      </c>
+      <c r="H63">
+        <v>280.32974215797702</v>
       </c>
       <c r="I63" s="5">
         <v>21</v>
       </c>
       <c r="J63">
-        <v>41.833581285098603</v>
+        <v>16.622771808475498</v>
       </c>
       <c r="K63">
-        <v>922.01157910316101</v>
-      </c>
-      <c r="L63" s="4">
-        <v>8263.5346912516707</v>
+        <v>22.596056919975599</v>
+      </c>
+      <c r="L63">
+        <v>1683.2790190462299</v>
       </c>
       <c r="M63" s="5">
         <v>21</v>
       </c>
-      <c r="N63" s="4">
-        <v>-1.0241175434207299</v>
+      <c r="N63">
+        <v>-0.960876241570775</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3416,43 +3416,43 @@
         <v>22</v>
       </c>
       <c r="B64">
-        <v>36.790098976324799</v>
+        <v>4.0570023762048502</v>
       </c>
       <c r="C64">
-        <v>95.910942468157501</v>
-      </c>
-      <c r="D64" s="4">
-        <v>432.19845930873902</v>
+        <v>25.521223417765199</v>
+      </c>
+      <c r="D64">
+        <v>251.455832544049</v>
       </c>
       <c r="E64" s="5">
         <v>22</v>
       </c>
       <c r="F64">
-        <v>4.7165869436461003</v>
+        <v>3.12199023374297E-2</v>
       </c>
       <c r="G64">
-        <v>76.882605720737999</v>
-      </c>
-      <c r="H64" s="4">
-        <v>525.25493313738605</v>
+        <v>1.6947035871062499</v>
+      </c>
+      <c r="H64">
+        <v>217.11626003444201</v>
       </c>
       <c r="I64" s="5">
         <v>22</v>
       </c>
       <c r="J64">
-        <v>50.126597912776802</v>
+        <v>1.04890896335876</v>
       </c>
       <c r="K64">
-        <v>480.59157895171199</v>
-      </c>
-      <c r="L64" s="4">
-        <v>4822.3866998207804</v>
+        <v>87.937850066022804</v>
+      </c>
+      <c r="L64">
+        <v>1033.6189862061899</v>
       </c>
       <c r="M64" s="5">
         <v>22</v>
       </c>
-      <c r="N64" s="4">
-        <v>-0.94783075637275505</v>
+      <c r="N64">
+        <v>-1.00543828719779</v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3460,43 +3460,43 @@
         <v>23</v>
       </c>
       <c r="B65">
-        <v>21.332633254709599</v>
+        <v>1.5260617343823799</v>
       </c>
       <c r="C65">
-        <v>104.60198409580499</v>
-      </c>
-      <c r="D65" s="4">
-        <v>379.40837041815399</v>
+        <v>10.1662922898447</v>
+      </c>
+      <c r="D65">
+        <v>301.149698338625</v>
       </c>
       <c r="E65" s="5">
         <v>23</v>
       </c>
       <c r="F65">
-        <v>19.6253152939911</v>
+        <v>0.59546413063947501</v>
       </c>
       <c r="G65">
-        <v>77.595024699717996</v>
-      </c>
-      <c r="H65" s="4">
-        <v>451.69367547469699</v>
+        <v>1.9272472166858501</v>
+      </c>
+      <c r="H65">
+        <v>447.10468097249401</v>
       </c>
       <c r="I65" s="5">
         <v>23</v>
       </c>
       <c r="J65">
-        <v>135.13688873077299</v>
+        <v>4.1981765301922902</v>
       </c>
       <c r="K65">
-        <v>352.17622053310998</v>
-      </c>
-      <c r="L65" s="4">
-        <v>5580.1891361500402</v>
+        <v>12.1519464439186</v>
+      </c>
+      <c r="L65">
+        <v>1160.8286889881001</v>
       </c>
       <c r="M65" s="5">
         <v>23</v>
       </c>
-      <c r="N65" s="4">
-        <v>-0.98751689339140603</v>
+      <c r="N65">
+        <v>-0.86418286331758098</v>
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3504,43 +3504,43 @@
         <v>24</v>
       </c>
       <c r="B66">
-        <v>43.922692069086999</v>
+        <v>8.6034364897872493</v>
       </c>
       <c r="C66">
-        <v>100.475428335728</v>
-      </c>
-      <c r="D66" s="4">
-        <v>409.43381959573702</v>
+        <v>21.1681603933406</v>
+      </c>
+      <c r="D66">
+        <v>298.75876462666702</v>
       </c>
       <c r="E66" s="5">
         <v>24</v>
       </c>
       <c r="F66">
-        <v>10.7919692268368</v>
+        <v>0.30439500494216898</v>
       </c>
       <c r="G66">
-        <v>126.944436812695</v>
-      </c>
-      <c r="H66" s="4">
-        <v>494.80943838434598</v>
+        <v>1.9469992705869901</v>
+      </c>
+      <c r="H66">
+        <v>294.89571684829099</v>
       </c>
       <c r="I66" s="5">
         <v>24</v>
       </c>
       <c r="J66">
-        <v>51.159398171348798</v>
+        <v>2.48878449247086</v>
       </c>
       <c r="K66">
-        <v>400.69479606108399</v>
-      </c>
-      <c r="L66" s="4">
-        <v>5479.7259624528997</v>
+        <v>49.572616244523999</v>
+      </c>
+      <c r="L66">
+        <v>1534.5345171128799</v>
       </c>
       <c r="M66" s="5">
         <v>24</v>
       </c>
-      <c r="N66" s="4">
-        <v>-1.02732441138881</v>
+      <c r="N66">
+        <v>-0.94908760578451501</v>
       </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3548,43 +3548,43 @@
         <v>25</v>
       </c>
       <c r="B67">
-        <v>41.965901219673199</v>
+        <v>11.0481955568348</v>
       </c>
       <c r="C67">
-        <v>88.744823953233194</v>
-      </c>
-      <c r="D67" s="4">
-        <v>401.53963264106602</v>
+        <v>29.1494222913432</v>
+      </c>
+      <c r="D67">
+        <v>312.633923699842</v>
       </c>
       <c r="E67" s="5">
         <v>25</v>
       </c>
       <c r="F67">
-        <v>31.389688354421398</v>
+        <v>0.53025602349941103</v>
       </c>
       <c r="G67">
-        <v>93.815854418206996</v>
-      </c>
-      <c r="H67" s="4">
-        <v>571.30508604801105</v>
+        <v>3.4829072846837699</v>
+      </c>
+      <c r="H67">
+        <v>381.80902066993002</v>
       </c>
       <c r="I67" s="5">
         <v>25</v>
       </c>
       <c r="J67">
-        <v>30.225346088721601</v>
+        <v>0.88725986761670295</v>
       </c>
       <c r="K67">
-        <v>504.71822962298802</v>
-      </c>
-      <c r="L67" s="4">
-        <v>5292.9924847784796</v>
+        <v>57.738018414478297</v>
+      </c>
+      <c r="L67">
+        <v>1644.46870985439</v>
       </c>
       <c r="M67" s="5">
         <v>25</v>
       </c>
-      <c r="N67" s="4">
-        <v>-1.01937061060783</v>
+      <c r="N67">
+        <v>-1.0214628289423</v>
       </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3592,43 +3592,43 @@
         <v>26</v>
       </c>
       <c r="B68">
-        <v>26.511517630990198</v>
+        <v>2.3841901415868301</v>
       </c>
       <c r="C68">
-        <v>109.224375601945</v>
-      </c>
-      <c r="D68" s="4">
-        <v>342.54686226513701</v>
+        <v>38.342558075928203</v>
+      </c>
+      <c r="D68">
+        <v>301.44608769295502</v>
       </c>
       <c r="E68" s="5">
         <v>26</v>
       </c>
       <c r="F68">
-        <v>27.4635819881989</v>
+        <v>0.50562275431814896</v>
       </c>
       <c r="G68">
-        <v>106.536068311525</v>
-      </c>
-      <c r="H68" s="4">
-        <v>563.426133062487</v>
+        <v>4.9252643069659898</v>
+      </c>
+      <c r="H68">
+        <v>357.08252042721699</v>
       </c>
       <c r="I68" s="5">
         <v>26</v>
       </c>
       <c r="J68">
-        <v>31.6580172220295</v>
+        <v>2.91659775052061</v>
       </c>
       <c r="K68">
-        <v>568.239866511694</v>
-      </c>
-      <c r="L68" s="4">
-        <v>7874.2052998196004</v>
+        <v>103.56830153811499</v>
+      </c>
+      <c r="L68">
+        <v>1277.56176353807</v>
       </c>
       <c r="M68" s="5">
         <v>26</v>
       </c>
-      <c r="N68" s="4">
-        <v>-1.0083020806288301</v>
+      <c r="N68">
+        <v>-0.61134762931110698</v>
       </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3636,43 +3636,43 @@
         <v>27</v>
       </c>
       <c r="B69">
-        <v>30.089815710804899</v>
+        <v>10.0140057446339</v>
       </c>
       <c r="C69">
-        <v>76.002221184457397</v>
-      </c>
-      <c r="D69" s="4">
-        <v>399.13115559890002</v>
+        <v>21.940193080587601</v>
+      </c>
+      <c r="D69">
+        <v>233.356140492588</v>
       </c>
       <c r="E69" s="5">
         <v>27</v>
       </c>
       <c r="F69">
-        <v>11.607498755232299</v>
+        <v>0.56419288588183103</v>
       </c>
       <c r="G69">
-        <v>119.047942527988</v>
-      </c>
-      <c r="H69" s="4">
-        <v>593.84647268380695</v>
+        <v>2.5077604297310598</v>
+      </c>
+      <c r="H69">
+        <v>323.23302186079098</v>
       </c>
       <c r="I69" s="5">
         <v>27</v>
       </c>
       <c r="J69">
-        <v>22.6464839166226</v>
+        <v>0.23626550725694401</v>
       </c>
       <c r="K69">
-        <v>451.41927329784397</v>
-      </c>
-      <c r="L69" s="4">
-        <v>7230.7701904964997</v>
+        <v>16.3584927776174</v>
+      </c>
+      <c r="L69">
+        <v>1270.04848675984</v>
       </c>
       <c r="M69" s="5">
         <v>27</v>
       </c>
-      <c r="N69" s="4">
-        <v>-1.022553030481</v>
+      <c r="N69">
+        <v>-0.97056248757917196</v>
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3680,43 +3680,43 @@
         <v>28</v>
       </c>
       <c r="B70">
-        <v>31.472989307850899</v>
+        <v>6.6082417253954198</v>
       </c>
       <c r="C70">
-        <v>103.487685324315</v>
-      </c>
-      <c r="D70" s="4">
-        <v>415.13695147632501</v>
+        <v>16.752264162985</v>
+      </c>
+      <c r="D70">
+        <v>290.884568174506</v>
       </c>
       <c r="E70" s="5">
         <v>28</v>
       </c>
       <c r="F70">
-        <v>27.044057472130401</v>
+        <v>0.79635527393743499</v>
       </c>
       <c r="G70">
-        <v>69.5116160529506</v>
-      </c>
-      <c r="H70" s="4">
-        <v>422.48130362500001</v>
+        <v>5.0684799118853396</v>
+      </c>
+      <c r="H70">
+        <v>333.12422577531299</v>
       </c>
       <c r="I70" s="5">
         <v>28</v>
       </c>
       <c r="J70">
-        <v>88.635029409864103</v>
+        <v>1.78376837227416</v>
       </c>
       <c r="K70">
-        <v>515.92907358319906</v>
-      </c>
-      <c r="L70" s="4">
-        <v>5773.3053952659702</v>
+        <v>24.609804586370501</v>
+      </c>
+      <c r="L70">
+        <v>1137.60080304808</v>
       </c>
       <c r="M70" s="5">
         <v>28</v>
       </c>
-      <c r="N70" s="4">
-        <v>-1.0062512475861001</v>
+      <c r="N70">
+        <v>-0.826111789721649</v>
       </c>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3724,43 +3724,43 @@
         <v>29</v>
       </c>
       <c r="B71">
-        <v>31.227848439030701</v>
+        <v>11.2720585240502</v>
       </c>
       <c r="C71">
-        <v>97.278776876277604</v>
-      </c>
-      <c r="D71" s="4">
-        <v>388.53066835700002</v>
+        <v>23.284130525903301</v>
+      </c>
+      <c r="D71">
+        <v>306.42444051625802</v>
       </c>
       <c r="E71" s="5">
         <v>29</v>
       </c>
       <c r="F71">
-        <v>19.675328543506801</v>
+        <v>0.34129449019553598</v>
       </c>
       <c r="G71">
-        <v>138.011034607591</v>
-      </c>
-      <c r="H71" s="4">
-        <v>508.25962719985898</v>
+        <v>2.5696191260662098</v>
+      </c>
+      <c r="H71">
+        <v>264.84881613142301</v>
       </c>
       <c r="I71" s="5">
         <v>29</v>
       </c>
       <c r="J71">
-        <v>67.756951708970504</v>
+        <v>4.2606587658938899</v>
       </c>
       <c r="K71">
-        <v>519.69214729786199</v>
-      </c>
-      <c r="L71" s="4">
-        <v>5957.31542094631</v>
+        <v>10.773658148664</v>
+      </c>
+      <c r="L71">
+        <v>1029.635854823</v>
       </c>
       <c r="M71" s="5">
         <v>29</v>
       </c>
-      <c r="N71" s="4">
-        <v>-0.99367355496180698</v>
+      <c r="N71">
+        <v>-0.847201280810438</v>
       </c>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3768,43 +3768,43 @@
         <v>30</v>
       </c>
       <c r="B72">
-        <v>30.782435355894599</v>
+        <v>6.8239188968495199</v>
       </c>
       <c r="C72">
-        <v>98.234515319253902</v>
-      </c>
-      <c r="D72" s="4">
-        <v>418.07079611976297</v>
+        <v>31.2732761550301</v>
+      </c>
+      <c r="D72">
+        <v>353.30936722785901</v>
       </c>
       <c r="E72" s="6">
         <v>30</v>
       </c>
       <c r="F72">
-        <v>44.544266787534497</v>
+        <v>0.219656514109037</v>
       </c>
       <c r="G72">
-        <v>49.236981701552999</v>
-      </c>
-      <c r="H72" s="4">
-        <v>485.08217709394802</v>
+        <v>2.2042891127157</v>
+      </c>
+      <c r="H72">
+        <v>280.73218888941398</v>
       </c>
       <c r="I72" s="6">
         <v>30</v>
       </c>
       <c r="J72">
-        <v>41.7306679477255</v>
+        <v>0.75660477430963602</v>
       </c>
       <c r="K72">
-        <v>659.54585645177394</v>
-      </c>
-      <c r="L72" s="4">
-        <v>133139.76639999999</v>
+        <v>11.5863203532579</v>
+      </c>
+      <c r="L72">
+        <v>621.08967036308104</v>
       </c>
       <c r="M72" s="6">
         <v>30</v>
       </c>
-      <c r="N72" s="4">
-        <v>-1.02620690035041</v>
+      <c r="N72">
+        <v>-0.82688911268558496</v>
       </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3813,46 +3813,46 @@
       </c>
       <c r="B73" s="7">
         <f>_xlfn.STDEV.S(B43:B72)</f>
-        <v>6.4495078121272664</v>
+        <v>3.5118361064355237</v>
       </c>
       <c r="C73" s="7">
         <f>_xlfn.STDEV.S(C43:C72)</f>
-        <v>10.750012097326463</v>
+        <v>7.3910232337129695</v>
       </c>
       <c r="D73" s="7">
         <f>_xlfn.STDEV.S(D43:D72)</f>
-        <v>28.26643704535763</v>
+        <v>35.430906609520534</v>
       </c>
       <c r="E73" s="7"/>
       <c r="F73" s="7">
         <f>_xlfn.STDEV.S(F43:F72)</f>
-        <v>8.7913687591226992</v>
+        <v>0.24126484764036105</v>
       </c>
       <c r="G73" s="7">
         <f>_xlfn.STDEV.S(G43:G72)</f>
-        <v>27.273523473747016</v>
+        <v>2.5864298653865423</v>
       </c>
       <c r="H73" s="7">
         <f>_xlfn.STDEV.S(H43:H72)</f>
-        <v>57.279436622865852</v>
+        <v>71.601259020318466</v>
       </c>
       <c r="I73" s="7"/>
       <c r="J73" s="7">
         <f>_xlfn.STDEV.S(J43:J72)</f>
-        <v>32.429704661406952</v>
+        <v>4.0642670347603733</v>
       </c>
       <c r="K73" s="7">
         <f>_xlfn.STDEV.S(K43:K72)</f>
-        <v>168.66695443607955</v>
+        <v>36.448156483314492</v>
       </c>
       <c r="L73" s="7">
         <f>_xlfn.STDEV.S(L43:L72)</f>
-        <v>23281.277522041877</v>
+        <v>358.66991048239953</v>
       </c>
       <c r="M73" s="7"/>
       <c r="N73" s="7">
         <f>_xlfn.STDEV.S(N43:N72)</f>
-        <v>2.3750470205233524E-2</v>
+        <v>0.13063988803178894</v>
       </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3861,46 +3861,46 @@
       </c>
       <c r="B74" s="7">
         <f>AVERAGE(B43:B72)</f>
-        <v>29.668413300958274</v>
+        <v>6.3035194433569002</v>
       </c>
       <c r="C74" s="7">
         <f>AVERAGE(C43:C72)</f>
-        <v>95.530584825396929</v>
+        <v>26.938666239964512</v>
       </c>
       <c r="D74" s="7">
         <f>AVERAGE(D43:D72)</f>
-        <v>405.19167140112046</v>
+        <v>282.30599825191518</v>
       </c>
       <c r="E74" s="7"/>
       <c r="F74" s="7">
         <f>AVERAGE(F43:F72)</f>
-        <v>19.645804055543941</v>
+        <v>0.41764158474993984</v>
       </c>
       <c r="G74" s="7">
         <f>AVERAGE(G43:G72)</f>
-        <v>95.39189242008959</v>
+        <v>3.8225688900805368</v>
       </c>
       <c r="H74" s="7">
         <f>AVERAGE(H43:H72)</f>
-        <v>520.38446509449091</v>
+        <v>293.12291565609064</v>
       </c>
       <c r="I74" s="7"/>
       <c r="J74" s="7">
         <f>AVERAGE(J43:J72)</f>
-        <v>53.850898488580633</v>
+        <v>4.2569915407155747</v>
       </c>
       <c r="K74" s="7">
         <f>AVERAGE(K43:K72)</f>
-        <v>527.4909876682932</v>
+        <v>35.871749467243987</v>
       </c>
       <c r="L74" s="7">
         <f>AVERAGE(L43:L72)</f>
-        <v>10039.443821531866</v>
+        <v>1327.7639171965789</v>
       </c>
       <c r="M74" s="7"/>
       <c r="N74" s="7">
         <f>AVERAGE(N43:N72)</f>
-        <v>-1.003598585696712</v>
+        <v>-0.88030405655166488</v>
       </c>
     </row>
     <row r="77" spans="1:14" ht="20.399999999999999" x14ac:dyDescent="0.75">
@@ -3908,7 +3908,7 @@
         <v>7</v>
       </c>
       <c r="C77" s="10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D77" s="10"/>
       <c r="E77" s="10"/>
@@ -3920,32 +3920,32 @@
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A79" s="12" t="s">
+      <c r="A79" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B79" s="12"/>
-      <c r="C79" s="12"/>
-      <c r="D79" s="13"/>
-      <c r="E79" s="12" t="s">
+      <c r="B79" s="15"/>
+      <c r="C79" s="15"/>
+      <c r="D79" s="16"/>
+      <c r="E79" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="F79" s="12"/>
-      <c r="G79" s="12"/>
-      <c r="H79" s="13"/>
-      <c r="I79" s="12" t="s">
+      <c r="F79" s="15"/>
+      <c r="G79" s="15"/>
+      <c r="H79" s="16"/>
+      <c r="I79" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="J79" s="12"/>
-      <c r="K79" s="12"/>
-      <c r="L79" s="13"/>
-      <c r="M79" s="14" t="s">
+      <c r="J79" s="15"/>
+      <c r="K79" s="15"/>
+      <c r="L79" s="16"/>
+      <c r="M79" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="N79" s="15"/>
+      <c r="N79" s="18"/>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="1" t="s">
@@ -5376,15 +5376,15 @@
         <v>26.962077145068445</v>
       </c>
       <c r="E112" s="7"/>
-      <c r="F112" s="18">
+      <c r="F112" s="14">
         <f>AVERAGE(F81:F110)</f>
         <v>2.3884062409033416E-4</v>
       </c>
-      <c r="G112" s="18">
+      <c r="G112" s="14">
         <f>AVERAGE(G81:G110)</f>
         <v>4.0223355266233034E-4</v>
       </c>
-      <c r="H112" s="18">
+      <c r="H112" s="14">
         <f>AVERAGE(H81:H110)</f>
         <v>6.4290707572003372E-4</v>
       </c>

</xml_diff>

<commit_message>
Hybrid and PSO algorithms main classes for all functions
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="22">
   <si>
     <t>Rastrigin</t>
   </si>
@@ -48,9 +48,6 @@
   </si>
   <si>
     <t>Generations = 200</t>
-  </si>
-  <si>
-    <t>Hibridizare [pop_size=50,crossover_pbb=0.4,mutation_pbb=0.1, hillcimbing_pbb=0.3]</t>
   </si>
   <si>
     <t>Iterations = 200</t>
@@ -81,6 +78,18 @@
   </si>
   <si>
     <t>Generations = 1000</t>
+  </si>
+  <si>
+    <t>Hibridizare [pop_size=100,crossover_pbb=0.4,mutation_pbb=0.1, hillcimbing_pbb=0.3]</t>
+  </si>
+  <si>
+    <t>Iterations = 1000</t>
+  </si>
+  <si>
+    <t>Particle Swarm Optimization [pop_size=100,min_speed=0.1, max_speed=0.1, maxW=1.0, minW=0.0, w2=2.0, w3=2.0]</t>
+  </si>
+  <si>
+    <t>PSO</t>
   </si>
 </sst>
 </file>
@@ -265,7 +274,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -281,11 +289,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -330,69 +374,75 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="P4:S7" totalsRowShown="0">
-  <autoFilter ref="P4:S7"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="P4:T7" totalsRowShown="0">
+  <autoFilter ref="P4:T7"/>
+  <tableColumns count="5">
     <tableColumn id="1" name="Rastrigin"/>
     <tableColumn id="2" name="HillClimbing"/>
-    <tableColumn id="3" name="Alg. Genetic" dataDxfId="9">
+    <tableColumn id="3" name="Alg. Genetic" dataDxfId="12">
       <calculatedColumnFormula>B73</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Hibridizare" dataDxfId="8">
+    <tableColumn id="4" name="Hibridizare" dataDxfId="11">
       <calculatedColumnFormula>L35</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="5" name="PSO"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="P12:S15" totalsRowShown="0">
-  <autoFilter ref="P12:S15"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="P12:T15" totalsRowShown="0">
+  <autoFilter ref="P12:T15"/>
+  <tableColumns count="5">
     <tableColumn id="1" name="Griewangk"/>
-    <tableColumn id="2" name="HillClimbing" dataDxfId="7">
+    <tableColumn id="2" name="HillClimbing" dataDxfId="10">
       <calculatedColumnFormula>F35</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Alg. Genetic" dataDxfId="6">
+    <tableColumn id="3" name="Alg. Genetic" dataDxfId="9">
       <calculatedColumnFormula>F73</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Hibridizare" dataDxfId="5">
+    <tableColumn id="4" name="Hibridizare" dataDxfId="8">
       <calculatedColumnFormula>L39</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="5" name="PSO" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table134" displayName="Table134" ref="P20:S23" totalsRowShown="0">
-  <autoFilter ref="P20:S23"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table134" displayName="Table134" ref="P20:T23" totalsRowShown="0">
+  <autoFilter ref="P20:T23"/>
+  <tableColumns count="5">
     <tableColumn id="1" name="Rosenbrock"/>
-    <tableColumn id="2" name="HillClimbing" dataDxfId="4">
+    <tableColumn id="2" name="HillClimbing" dataDxfId="7">
       <calculatedColumnFormula>L33</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Alg. Genetic" dataDxfId="3"/>
-    <tableColumn id="4" name="Hibridizare" dataDxfId="2"/>
+    <tableColumn id="3" name="Alg. Genetic" dataDxfId="6"/>
+    <tableColumn id="4" name="Hibridizare" dataDxfId="5"/>
+    <tableColumn id="5" name="PSO" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table135" displayName="Table135" ref="P28:S29" totalsRowShown="0">
-  <autoFilter ref="P28:S29"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table135" displayName="Table135" ref="P28:T29" totalsRowShown="0">
+  <autoFilter ref="P28:T29"/>
+  <tableColumns count="5">
     <tableColumn id="1" name="SHCB"/>
     <tableColumn id="2" name="HillClimbing">
       <calculatedColumnFormula>AVERAGE(N5:N34)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Alg. Genetic" dataDxfId="1">
+    <tableColumn id="3" name="Alg. Genetic" dataDxfId="4">
       <calculatedColumnFormula>AVERAGE(N43:N72)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Hibridizare" dataDxfId="0">
+    <tableColumn id="4" name="Hibridizare" dataDxfId="3">
       <calculatedColumnFormula>AVERAGE(N81:N110)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="PSO" dataDxfId="0">
+      <calculatedColumnFormula>AVERAGE(N119:N148)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -696,57 +746,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S112"/>
+  <dimension ref="A1:T150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="N43" sqref="N43:N72"/>
+    <sheetView tabSelected="1" topLeftCell="L3" workbookViewId="0">
+      <selection activeCell="L112" sqref="L112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="2" max="2" width="8.83984375" customWidth="1"/>
+    <col min="6" max="7" width="11.68359375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.68359375" customWidth="1"/>
     <col min="16" max="16" width="13.5234375" customWidth="1"/>
     <col min="17" max="17" width="14.62890625" customWidth="1"/>
     <col min="18" max="18" width="14.20703125" customWidth="1"/>
     <col min="19" max="19" width="13.1015625" customWidth="1"/>
+    <col min="20" max="20" width="13.62890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:20" ht="20.399999999999999" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="15" t="s">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="15" t="s">
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="15" t="s">
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="17" t="s">
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="18"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="N3" s="17"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -793,16 +846,19 @@
         <v>0</v>
       </c>
       <c r="Q4" t="s">
+        <v>9</v>
+      </c>
+      <c r="R4" t="s">
         <v>10</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>11</v>
       </c>
-      <c r="S4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="T4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -846,22 +902,26 @@
         <v>-0.97056248757917196</v>
       </c>
       <c r="P5" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q5" s="12">
+        <v>12</v>
+      </c>
+      <c r="Q5" s="11">
         <f>AVERAGE(B5:B34)</f>
         <v>12.46627977627489</v>
       </c>
-      <c r="R5" s="13">
+      <c r="R5" s="12">
         <f>AVERAGE(B43:B72)</f>
         <v>6.3035194433569002</v>
       </c>
       <c r="S5">
         <f>AVERAGE(B81:B110)</f>
-        <v>0.14514710689519539</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+        <v>0.91056052110121632</v>
+      </c>
+      <c r="T5" s="11">
+        <f>AVERAGE(B119:B148)</f>
+        <v>1.7245953631070927</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="5">
         <v>2</v>
       </c>
@@ -905,22 +965,26 @@
         <v>-0.74784721613453697</v>
       </c>
       <c r="P6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q6">
         <f>AVERAGE(C5:C34)</f>
         <v>31.655790932304605</v>
       </c>
-      <c r="R6" s="13">
+      <c r="R6" s="12">
         <f>AVERAGE(C43:C72)</f>
         <v>26.938666239964512</v>
       </c>
       <c r="S6">
         <f>AVERAGE(C81:C110)</f>
-        <v>2.1593347935221634</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+        <v>7.1719322031694466</v>
+      </c>
+      <c r="T6">
+        <f>AVERAGE(C119:C148)</f>
+        <v>9.3217664772135596</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="5">
         <v>3</v>
       </c>
@@ -964,22 +1028,26 @@
         <v>-0.982009523598117</v>
       </c>
       <c r="P7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Q7">
         <f>AVERAGE(D5:D34)</f>
         <v>85.050965060569709</v>
       </c>
-      <c r="R7" s="13">
+      <c r="R7" s="12">
         <f>AVERAGE(D43:D72)</f>
         <v>282.30599825191518</v>
       </c>
       <c r="S7">
         <f>AVERAGE(D81:D110)</f>
-        <v>26.962077145068445</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+        <v>70.854718563415943</v>
+      </c>
+      <c r="T7">
+        <f>AVERAGE(D119:D148)</f>
+        <v>59.441380355171873</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="5">
         <v>4</v>
       </c>
@@ -1023,7 +1091,7 @@
         <v>-0.99367355496180698</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="5">
         <v>5</v>
       </c>
@@ -1067,7 +1135,7 @@
         <v>-1.02992784328481</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="5">
         <v>6</v>
       </c>
@@ -1111,7 +1179,7 @@
         <v>-0.97056248757917196</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="5">
         <v>7</v>
       </c>
@@ -1155,7 +1223,7 @@
         <v>-0.99550048954989001</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="5">
         <v>8</v>
       </c>
@@ -1202,16 +1270,19 @@
         <v>1</v>
       </c>
       <c r="Q12" t="s">
+        <v>9</v>
+      </c>
+      <c r="R12" t="s">
         <v>10</v>
       </c>
-      <c r="R12" t="s">
+      <c r="S12" t="s">
         <v>11</v>
       </c>
-      <c r="S12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="T12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="5">
         <v>9</v>
       </c>
@@ -1255,7 +1326,7 @@
         <v>-0.99511469963927401</v>
       </c>
       <c r="P13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Q13">
         <f>AVERAGE(F5:F34)</f>
@@ -1267,10 +1338,14 @@
       </c>
       <c r="S13" s="9">
         <f>AVERAGE(F81:F110)</f>
-        <v>2.3884062409033416E-4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+        <v>0.12489978588344637</v>
+      </c>
+      <c r="T13" s="18">
+        <f>AVERAGE(F119:F148)</f>
+        <v>0.12626248149128086</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="5">
         <v>10</v>
       </c>
@@ -1314,7 +1389,7 @@
         <v>-1.0241175434207299</v>
       </c>
       <c r="P14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q14">
         <f>AVERAGE(G5:G34)</f>
@@ -1326,10 +1401,14 @@
       </c>
       <c r="S14" s="9">
         <f>AVERAGE(G81:G110)</f>
-        <v>4.0223355266233034E-4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+        <v>0.23506002199208054</v>
+      </c>
+      <c r="T14" s="12">
+        <f>AVERAGE(G119:G148)</f>
+        <v>0.19600730113449957</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="5">
         <v>11</v>
       </c>
@@ -1373,7 +1452,7 @@
         <v>-0.99550048954989001</v>
       </c>
       <c r="P15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Q15">
         <f>AVERAGE(H5:H34)</f>
@@ -1385,10 +1464,14 @@
       </c>
       <c r="S15" s="9">
         <f>AVERAGE(H81:H110)</f>
-        <v>6.4290707572003372E-4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+        <v>50.521245301983839</v>
+      </c>
+      <c r="T15" s="12">
+        <f>AVERAGE(H119:H148)</f>
+        <v>1.6013830574925039</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="5">
         <v>12</v>
       </c>
@@ -1432,7 +1515,7 @@
         <v>-0.74784721613453697</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="5">
         <v>13</v>
       </c>
@@ -1476,7 +1559,7 @@
         <v>0.75128030984111505</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="5">
         <v>14</v>
       </c>
@@ -1520,7 +1603,7 @@
         <v>-0.99511469963927401</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="5">
         <v>15</v>
       </c>
@@ -1564,7 +1647,7 @@
         <v>-0.99550048954989001</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="5">
         <v>16</v>
       </c>
@@ -1611,16 +1694,19 @@
         <v>2</v>
       </c>
       <c r="Q20" t="s">
+        <v>9</v>
+      </c>
+      <c r="R20" t="s">
         <v>10</v>
       </c>
-      <c r="R20" t="s">
+      <c r="S20" t="s">
         <v>11</v>
       </c>
-      <c r="S20" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="T20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="5">
         <v>17</v>
       </c>
@@ -1664,7 +1750,7 @@
         <v>-0.75312481486496696</v>
       </c>
       <c r="P21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Q21">
         <f>AVERAGE(J5:J34)</f>
@@ -1676,10 +1762,14 @@
       </c>
       <c r="S21">
         <f>AVERAGE(J81:J110)</f>
-        <v>5.8623430512223643E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+        <v>2.7573632080631114</v>
+      </c>
+      <c r="T21" s="18">
+        <f>AVERAGE(J119:J148)</f>
+        <v>0.40090916299244611</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="5">
         <v>18</v>
       </c>
@@ -1723,7 +1813,7 @@
         <v>-1.02992784328481</v>
       </c>
       <c r="P22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q22">
         <f>AVERAGE(K5:K34)</f>
@@ -1735,10 +1825,14 @@
       </c>
       <c r="S22">
         <f>AVERAGE(K81:K110)</f>
-        <v>3.2678913957656874</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+        <v>12.829960769469936</v>
+      </c>
+      <c r="T22" s="12">
+        <f>AVERAGE(K119:K148)</f>
+        <v>4.3864152256705893</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="5">
         <v>19</v>
       </c>
@@ -1782,7 +1876,7 @@
         <v>-0.70306507946305796</v>
       </c>
       <c r="P23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Q23">
         <f>AVERAGE(L5:L34)</f>
@@ -1794,10 +1888,14 @@
       </c>
       <c r="S23">
         <f>AVERAGE(L81:L110)</f>
-        <v>26.674175924372033</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+        <v>152.07539589330949</v>
+      </c>
+      <c r="T23" s="12">
+        <f>AVERAGE(L119:L148)</f>
+        <v>102.44028014327277</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="5">
         <v>20</v>
       </c>
@@ -1841,7 +1939,7 @@
         <v>-0.99550048954989001</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="5">
         <v>21</v>
       </c>
@@ -1885,7 +1983,7 @@
         <v>-0.982009523598117</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="5">
         <v>22</v>
       </c>
@@ -1929,7 +2027,7 @@
         <v>-0.99550048954989001</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="5">
         <v>23</v>
       </c>
@@ -1973,7 +2071,7 @@
         <v>-1.03124356431136</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="5">
         <v>24</v>
       </c>
@@ -2020,16 +2118,19 @@
         <v>3</v>
       </c>
       <c r="Q28" t="s">
+        <v>9</v>
+      </c>
+      <c r="R28" t="s">
         <v>10</v>
       </c>
-      <c r="R28" t="s">
+      <c r="S28" t="s">
         <v>11</v>
       </c>
-      <c r="S28" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="T28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="5">
         <v>25</v>
       </c>
@@ -2073,7 +2174,7 @@
         <v>-1.0308900958220399</v>
       </c>
       <c r="P29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Q29">
         <f>AVERAGE(N5:N34)</f>
@@ -2085,10 +2186,14 @@
       </c>
       <c r="S29">
         <f>AVERAGE(N81:N110)</f>
-        <v>-1.03124356431136</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+        <v>-1.0205903810606922</v>
+      </c>
+      <c r="T29" s="18">
+        <f>AVERAGE(N119:N148)</f>
+        <v>-1.0316284534898694</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="5">
         <v>26</v>
       </c>
@@ -2132,7 +2237,7 @@
         <v>-0.99511469963927401</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="5">
         <v>27</v>
       </c>
@@ -2176,7 +2281,7 @@
         <v>-1.02781076098617</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="5">
         <v>28</v>
       </c>
@@ -2406,10 +2511,10 @@
     </row>
     <row r="39" spans="1:14" ht="20.399999999999999" x14ac:dyDescent="0.75">
       <c r="A39" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
@@ -2420,28 +2525,28 @@
       <c r="J39" s="10"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="15" t="s">
+      <c r="A41" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B41" s="15"/>
-      <c r="C41" s="15"/>
-      <c r="D41" s="16"/>
-      <c r="E41" s="15" t="s">
+      <c r="B41" s="14"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="F41" s="15"/>
-      <c r="G41" s="15"/>
-      <c r="H41" s="16"/>
-      <c r="I41" s="15" t="s">
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="15"/>
+      <c r="I41" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="J41" s="15"/>
-      <c r="K41" s="15"/>
-      <c r="L41" s="16"/>
-      <c r="M41" s="17" t="s">
+      <c r="J41" s="14"/>
+      <c r="K41" s="14"/>
+      <c r="L41" s="15"/>
+      <c r="M41" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="N41" s="18"/>
+      <c r="N41" s="17"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="1" t="s">
@@ -3908,7 +4013,7 @@
         <v>7</v>
       </c>
       <c r="C77" s="10" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="D77" s="10"/>
       <c r="E77" s="10"/>
@@ -3918,34 +4023,29 @@
       <c r="I77" s="10"/>
       <c r="J77" s="10"/>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A78" t="s">
-        <v>9</v>
-      </c>
-    </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A79" s="15" t="s">
+      <c r="A79" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B79" s="15"/>
-      <c r="C79" s="15"/>
-      <c r="D79" s="16"/>
-      <c r="E79" s="15" t="s">
+      <c r="B79" s="14"/>
+      <c r="C79" s="14"/>
+      <c r="D79" s="15"/>
+      <c r="E79" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="F79" s="15"/>
-      <c r="G79" s="15"/>
-      <c r="H79" s="16"/>
-      <c r="I79" s="15" t="s">
+      <c r="F79" s="14"/>
+      <c r="G79" s="14"/>
+      <c r="H79" s="15"/>
+      <c r="I79" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="J79" s="15"/>
-      <c r="K79" s="15"/>
-      <c r="L79" s="16"/>
-      <c r="M79" s="17" t="s">
+      <c r="J79" s="14"/>
+      <c r="K79" s="14"/>
+      <c r="L79" s="15"/>
+      <c r="M79" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="N79" s="18"/>
+      <c r="N79" s="17"/>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="1" t="s">
@@ -3996,43 +4096,43 @@
         <v>1</v>
       </c>
       <c r="B81">
-        <v>0.104292362612405</v>
+        <v>2.48454803786444E-2</v>
       </c>
       <c r="C81">
-        <v>1.17488415661039</v>
-      </c>
-      <c r="D81" s="4">
-        <v>30.132480990226298</v>
+        <v>4.9162747484717002</v>
+      </c>
+      <c r="D81">
+        <v>55.856014452747402</v>
       </c>
       <c r="E81" s="3">
         <v>1</v>
       </c>
-      <c r="F81" s="9">
-        <v>5.1516244644644795E-4</v>
-      </c>
-      <c r="G81" s="9">
-        <v>5.0724415506575495E-4</v>
-      </c>
-      <c r="H81" s="11">
-        <v>5.89466946883221E-4</v>
+      <c r="F81">
+        <v>0.15334565735615499</v>
+      </c>
+      <c r="G81">
+        <v>0.12520357091616199</v>
+      </c>
+      <c r="H81">
+        <v>67.228441241153504</v>
       </c>
       <c r="I81" s="3">
         <v>1</v>
       </c>
       <c r="J81">
-        <v>0.50915290804257696</v>
+        <v>4.6517216383730604</v>
       </c>
       <c r="K81">
-        <v>1.69148420809235</v>
-      </c>
-      <c r="L81" s="4">
-        <v>28.394959030398802</v>
+        <v>9.8089216069104808</v>
+      </c>
+      <c r="L81">
+        <v>46.599145051534897</v>
       </c>
       <c r="M81" s="3">
         <v>1</v>
       </c>
-      <c r="N81" s="4">
-        <v>-1.03124356431136</v>
+      <c r="N81">
+        <v>-0.99511469963927401</v>
       </c>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -4040,43 +4140,43 @@
         <v>2</v>
       </c>
       <c r="B82">
-        <v>0.14401580372928499</v>
+        <v>1.13420965858149</v>
       </c>
       <c r="C82">
-        <v>0.20858472522480201</v>
-      </c>
-      <c r="D82" s="4">
-        <v>28.891567154662798</v>
+        <v>7.3760337126217497</v>
+      </c>
+      <c r="D82">
+        <v>70.952901955773299</v>
       </c>
       <c r="E82" s="5">
         <v>2</v>
       </c>
-      <c r="F82" s="9">
-        <v>9.5797370065819898E-5</v>
-      </c>
-      <c r="G82" s="9">
-        <v>4.9204262391100396E-4</v>
-      </c>
-      <c r="H82" s="11">
-        <v>9.15419064258182E-4</v>
+      <c r="F82">
+        <v>0.255016664910445</v>
+      </c>
+      <c r="G82">
+        <v>0.49714977513835601</v>
+      </c>
+      <c r="H82">
+        <v>49.658004634391702</v>
       </c>
       <c r="I82" s="5">
         <v>2</v>
       </c>
       <c r="J82">
-        <v>6.2613365072224604E-3</v>
+        <v>2.7379884994252301</v>
       </c>
       <c r="K82">
-        <v>4.5024864087076404</v>
-      </c>
-      <c r="L82" s="4">
-        <v>27.300634701195801</v>
+        <v>77.070242075013496</v>
+      </c>
+      <c r="L82">
+        <v>233.04427863855099</v>
       </c>
       <c r="M82" s="5">
         <v>2</v>
       </c>
-      <c r="N82" s="4">
-        <v>-1.03124356431136</v>
+      <c r="N82">
+        <v>-1.02781076098617</v>
       </c>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -4084,43 +4184,43 @@
         <v>3</v>
       </c>
       <c r="B83">
-        <v>2.48454803786444E-2</v>
+        <v>0.30212876410981998</v>
       </c>
       <c r="C83">
-        <v>3.69019557952761</v>
-      </c>
-      <c r="D83" s="4">
-        <v>25.0510166539806</v>
+        <v>7.9315273133426398</v>
+      </c>
+      <c r="D83">
+        <v>57.258099795005101</v>
       </c>
       <c r="E83" s="5">
         <v>3</v>
       </c>
-      <c r="F83" s="9">
-        <v>3.3079669169944198E-4</v>
-      </c>
-      <c r="G83" s="9">
-        <v>2.38231036261638E-4</v>
-      </c>
-      <c r="H83" s="11">
-        <v>4.46115599425311E-4</v>
+      <c r="F83">
+        <v>4.4383653365819897E-2</v>
+      </c>
+      <c r="G83">
+        <v>0.104403173964982</v>
+      </c>
+      <c r="H83">
+        <v>44.743460151735697</v>
       </c>
       <c r="I83" s="5">
         <v>3</v>
       </c>
       <c r="J83">
-        <v>6.2613365072224604E-3</v>
+        <v>0.40081652736490098</v>
       </c>
       <c r="K83">
-        <v>6.3001922092448499</v>
-      </c>
-      <c r="L83" s="4">
-        <v>28.094590243579699</v>
+        <v>6.9924839822581601</v>
+      </c>
+      <c r="L83">
+        <v>177.960767525629</v>
       </c>
       <c r="M83" s="5">
         <v>3</v>
       </c>
-      <c r="N83" s="4">
-        <v>-1.03124356431136</v>
+      <c r="N83">
+        <v>-1.0292333137148999</v>
       </c>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -4128,43 +4228,43 @@
         <v>4</v>
       </c>
       <c r="B84">
-        <v>2.48454803786444E-2</v>
+        <v>0.104292362612405</v>
       </c>
       <c r="C84">
-        <v>3.55519623852669</v>
-      </c>
-      <c r="D84" s="4">
-        <v>23.5488119446787</v>
+        <v>1.17488415661039</v>
+      </c>
+      <c r="D84">
+        <v>75.775365463339398</v>
       </c>
       <c r="E84" s="5">
         <v>4</v>
       </c>
-      <c r="F84" s="9">
-        <v>9.5797370065819898E-5</v>
-      </c>
-      <c r="G84" s="9">
-        <v>7.4985130940941004E-4</v>
-      </c>
-      <c r="H84" s="11">
-        <v>3.9812672190575599E-4</v>
+      <c r="F84">
+        <v>5.4332202889341298E-2</v>
+      </c>
+      <c r="G84">
+        <v>0.231005391657787</v>
+      </c>
+      <c r="H84">
+        <v>39.416696382765998</v>
       </c>
       <c r="I84" s="5">
         <v>4</v>
       </c>
       <c r="J84">
-        <v>8.4170775983744894E-2</v>
+        <v>4.14135505666626</v>
       </c>
       <c r="K84">
-        <v>1.55227442443659</v>
-      </c>
-      <c r="L84" s="4">
-        <v>27.139916641994201</v>
+        <v>8.7830484391684092</v>
+      </c>
+      <c r="L84">
+        <v>102.184531782728</v>
       </c>
       <c r="M84" s="5">
         <v>4</v>
       </c>
-      <c r="N84" s="4">
-        <v>-1.03124356431136</v>
+      <c r="N84">
+        <v>-1.02992784328481</v>
       </c>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -4172,43 +4272,43 @@
         <v>5</v>
       </c>
       <c r="B85">
-        <v>0.104292362612405</v>
+        <v>0.223462685963049</v>
       </c>
       <c r="C85">
-        <v>1.25433103884416</v>
-      </c>
-      <c r="D85" s="4">
-        <v>21.587819481901199</v>
+        <v>8.5330075308381996</v>
+      </c>
+      <c r="D85">
+        <v>76.647765116743997</v>
       </c>
       <c r="E85" s="5">
         <v>5</v>
       </c>
-      <c r="F85" s="9">
-        <v>2.07715397280705E-4</v>
-      </c>
-      <c r="G85" s="9">
-        <v>6.0571838485390297E-4</v>
-      </c>
-      <c r="H85" s="11">
-        <v>4.4600698069330303E-4</v>
+      <c r="F85">
+        <v>6.18301787139377E-2</v>
+      </c>
+      <c r="G85">
+        <v>9.36241692158198E-2</v>
+      </c>
+      <c r="H85">
+        <v>29.197646954847102</v>
       </c>
       <c r="I85" s="5">
         <v>5</v>
       </c>
       <c r="J85">
-        <v>6.2613365072224604E-3</v>
+        <v>0.64444930914777498</v>
       </c>
       <c r="K85">
-        <v>1.1600154865385699</v>
-      </c>
-      <c r="L85" s="4">
-        <v>26.6371719403779</v>
+        <v>7.8988932723132601</v>
+      </c>
+      <c r="L85">
+        <v>238.72337576720801</v>
       </c>
       <c r="M85" s="5">
         <v>5</v>
       </c>
-      <c r="N85" s="4">
-        <v>-1.03124356431136</v>
+      <c r="N85">
+        <v>-1.02992784328481</v>
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -4216,43 +4316,43 @@
         <v>6</v>
       </c>
       <c r="B86">
-        <v>1.0547627763477301</v>
+        <v>1.5260617343823899</v>
       </c>
       <c r="C86">
-        <v>3.6026764008828098</v>
-      </c>
-      <c r="D86" s="4">
-        <v>22.527166663907</v>
+        <v>12.358790565575999</v>
+      </c>
+      <c r="D86">
+        <v>59.157775697325199</v>
       </c>
       <c r="E86" s="5">
         <v>6</v>
       </c>
-      <c r="F86" s="9">
-        <v>4.3120992065681603E-4</v>
-      </c>
-      <c r="G86" s="9">
-        <v>1.65031461983544E-4</v>
-      </c>
-      <c r="H86" s="11">
-        <v>5.9766907777414303E-4</v>
+      <c r="F86">
+        <v>4.95087644549232E-2</v>
+      </c>
+      <c r="G86">
+        <v>5.1739015023810002E-2</v>
+      </c>
+      <c r="H86">
+        <v>35.888871150701902</v>
       </c>
       <c r="I86" s="5">
         <v>6</v>
       </c>
       <c r="J86">
-        <v>8.4170775983744894E-2</v>
+        <v>4.14135505666626</v>
       </c>
       <c r="K86">
-        <v>3.69685467612703</v>
-      </c>
-      <c r="L86" s="4">
-        <v>24.113198741239</v>
+        <v>6.7200259228933898</v>
+      </c>
+      <c r="L86">
+        <v>87.279259097479297</v>
       </c>
       <c r="M86" s="5">
         <v>6</v>
       </c>
-      <c r="N86" s="4">
-        <v>-1.03124356431136</v>
+      <c r="N86">
+        <v>-1.02992784328481</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -4260,43 +4360,43 @@
         <v>7</v>
       </c>
       <c r="B87">
-        <v>2.48454803786444E-2</v>
+        <v>2.2666943467585998</v>
       </c>
       <c r="C87">
-        <v>3.1949953074316801</v>
-      </c>
-      <c r="D87" s="4">
-        <v>27.8130334175043</v>
+        <v>14.7367839409394</v>
+      </c>
+      <c r="D87">
+        <v>58.248920609915601</v>
       </c>
       <c r="E87" s="5">
         <v>7</v>
       </c>
-      <c r="F87" s="9">
-        <v>4.3120992065681603E-4</v>
-      </c>
-      <c r="G87" s="9">
-        <v>2.5848405569506202E-4</v>
-      </c>
-      <c r="H87" s="11">
-        <v>6.36788123234199E-4</v>
+      <c r="F87">
+        <v>6.7672635242402607E-2</v>
+      </c>
+      <c r="G87">
+        <v>0.49800749396710597</v>
+      </c>
+      <c r="H87">
+        <v>32.025433492528798</v>
       </c>
       <c r="I87" s="5">
         <v>7</v>
       </c>
       <c r="J87">
-        <v>6.2613365072224604E-3</v>
+        <v>0.52983724368005902</v>
       </c>
       <c r="K87">
-        <v>1.3951854161677499</v>
-      </c>
-      <c r="L87" s="4">
-        <v>26.450227486336399</v>
+        <v>0.71603622165272496</v>
+      </c>
+      <c r="L87">
+        <v>278.052295349281</v>
       </c>
       <c r="M87" s="5">
         <v>7</v>
       </c>
-      <c r="N87" s="4">
-        <v>-1.03124356431136</v>
+      <c r="N87">
+        <v>-1.0292333137148999</v>
       </c>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -4304,43 +4404,43 @@
         <v>8</v>
       </c>
       <c r="B88">
-        <v>0.14401580372928799</v>
+        <v>6.4568921495528203E-2</v>
       </c>
       <c r="C88">
-        <v>1.15905513896014</v>
-      </c>
-      <c r="D88" s="4">
-        <v>29.1910841145273</v>
+        <v>9.7401261342824093</v>
+      </c>
+      <c r="D88">
+        <v>43.765872570506303</v>
       </c>
       <c r="E88" s="5">
         <v>8</v>
       </c>
-      <c r="F88" s="9">
-        <v>1.63015493456653E-4</v>
-      </c>
-      <c r="G88" s="9">
-        <v>3.5960935131029698E-4</v>
-      </c>
-      <c r="H88" s="11">
-        <v>4.6745096032019202E-4</v>
+      <c r="F88">
+        <v>5.2037463815874201E-2</v>
+      </c>
+      <c r="G88">
+        <v>5.2138970591847598E-2</v>
+      </c>
+      <c r="H88">
+        <v>72.148262213792506</v>
       </c>
       <c r="I88" s="5">
         <v>8</v>
       </c>
       <c r="J88">
-        <v>8.4170775983744894E-2</v>
+        <v>4.2639742678585204</v>
       </c>
       <c r="K88">
-        <v>0.16411688241304501</v>
-      </c>
-      <c r="L88" s="4">
-        <v>24.847434850742399</v>
+        <v>6.0729007500919803</v>
+      </c>
+      <c r="L88">
+        <v>67.170003418133305</v>
       </c>
       <c r="M88" s="5">
         <v>8</v>
       </c>
-      <c r="N88" s="4">
-        <v>-1.03124356431136</v>
+      <c r="N88">
+        <v>-1.02781076098617</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -4348,43 +4448,43 @@
         <v>9</v>
       </c>
       <c r="B89">
-        <v>6.4568921495524706E-2</v>
+        <v>1.00704340046774</v>
       </c>
       <c r="C89">
-        <v>1.15905513896012</v>
-      </c>
-      <c r="D89" s="4">
-        <v>26.029149723692701</v>
+        <v>6.80139344888671</v>
+      </c>
+      <c r="D89">
+        <v>77.551447565282899</v>
       </c>
       <c r="E89" s="5">
         <v>9</v>
       </c>
-      <c r="F89" s="9">
-        <v>1.63015493456653E-4</v>
-      </c>
-      <c r="G89" s="9">
-        <v>2.1269009470259399E-4</v>
-      </c>
-      <c r="H89" s="11">
-        <v>4.5301108138062703E-4</v>
+      <c r="F89">
+        <v>5.4450146902587898E-2</v>
+      </c>
+      <c r="G89">
+        <v>0.13464003151447801</v>
+      </c>
+      <c r="H89">
+        <v>81.259373107903102</v>
       </c>
       <c r="I89" s="5">
         <v>9</v>
       </c>
       <c r="J89">
-        <v>0.56653986967125303</v>
+        <v>1.0249072340218901</v>
       </c>
       <c r="K89">
-        <v>1.47436498496007</v>
-      </c>
-      <c r="L89" s="4">
-        <v>27.5480274695155</v>
+        <v>22.3656191412692</v>
+      </c>
+      <c r="L89">
+        <v>80.124780650232196</v>
       </c>
       <c r="M89" s="5">
         <v>9</v>
       </c>
-      <c r="N89" s="4">
-        <v>-1.03124356431136</v>
+      <c r="N89">
+        <v>-1.02781076098617</v>
       </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -4392,42 +4492,42 @@
         <v>10</v>
       </c>
       <c r="B90">
-        <v>2.48454803786444E-2</v>
+        <v>1.3939962867346201</v>
       </c>
       <c r="C90">
-        <v>3.6901886889329698</v>
-      </c>
-      <c r="D90" s="4">
-        <v>29.258685703975502</v>
+        <v>10.554146074660601</v>
+      </c>
+      <c r="D90">
+        <v>71.908871277231697</v>
       </c>
       <c r="E90" s="5">
         <v>10</v>
       </c>
-      <c r="F90" s="9">
-        <v>9.5797370065819898E-5</v>
-      </c>
-      <c r="G90" s="9">
-        <v>3.1884230988832302E-4</v>
-      </c>
-      <c r="H90" s="11">
-        <v>9.8950593781643704E-4</v>
+      <c r="F90">
+        <v>1.02302610325293E-2</v>
+      </c>
+      <c r="G90">
+        <v>0.15229209541896899</v>
+      </c>
+      <c r="H90">
+        <v>30.3743607481243</v>
       </c>
       <c r="I90" s="5">
         <v>10</v>
       </c>
       <c r="J90">
-        <v>6.2613365072224604E-3</v>
+        <v>4.0788728209646603</v>
       </c>
       <c r="K90">
-        <v>6.8006306533828003</v>
-      </c>
-      <c r="L90" s="4">
-        <v>26.9701673299753</v>
+        <v>11.612538835297499</v>
+      </c>
+      <c r="L90">
+        <v>151.80491053229201</v>
       </c>
       <c r="M90" s="5">
         <v>10</v>
       </c>
-      <c r="N90" s="4">
+      <c r="N90">
         <v>-1.03124356431136</v>
       </c>
     </row>
@@ -4436,42 +4536,42 @@
         <v>11</v>
       </c>
       <c r="B91">
-        <v>0.14401580372928799</v>
+        <v>0.104292362612405</v>
       </c>
       <c r="C91">
-        <v>1.1193316978432399</v>
-      </c>
-      <c r="D91" s="4">
-        <v>30.4520980058332</v>
+        <v>5.9145408997348801</v>
+      </c>
+      <c r="D91">
+        <v>121.079341885459</v>
       </c>
       <c r="E91" s="5">
         <v>11</v>
       </c>
-      <c r="F91" s="9">
-        <v>9.5797370065819898E-5</v>
-      </c>
-      <c r="G91" s="9">
-        <v>3.1435305250038199E-4</v>
-      </c>
-      <c r="H91" s="11">
-        <v>9.3359039716833705E-4</v>
+      <c r="F91">
+        <v>5.6815920379964802E-2</v>
+      </c>
+      <c r="G91">
+        <v>0.25995187235114098</v>
+      </c>
+      <c r="H91">
+        <v>54.663965576055197</v>
       </c>
       <c r="I91" s="5">
         <v>11</v>
       </c>
       <c r="J91">
-        <v>6.2613365072224604E-3</v>
+        <v>0.579751146184874</v>
       </c>
       <c r="K91">
-        <v>5.7276062855444803</v>
-      </c>
-      <c r="L91" s="4">
-        <v>29.109441068749302</v>
+        <v>6.83882316549359</v>
+      </c>
+      <c r="L91">
+        <v>43.867379594623998</v>
       </c>
       <c r="M91" s="5">
         <v>11</v>
       </c>
-      <c r="N91" s="4">
+      <c r="N91">
         <v>-1.03124356431136</v>
       </c>
     </row>
@@ -4480,43 +4580,43 @@
         <v>12</v>
       </c>
       <c r="B92">
-        <v>0.104292362612405</v>
+        <v>0.14401580372928499</v>
       </c>
       <c r="C92">
-        <v>3.1633441627257901</v>
-      </c>
-      <c r="D92" s="4">
-        <v>35.122347898334802</v>
+        <v>11.021093874958201</v>
+      </c>
+      <c r="D92">
+        <v>69.450881309698005</v>
       </c>
       <c r="E92" s="5">
         <v>12</v>
       </c>
-      <c r="F92" s="9">
-        <v>4.1475764827880702E-4</v>
-      </c>
-      <c r="G92" s="9">
-        <v>5.9035160652920395E-4</v>
-      </c>
-      <c r="H92" s="11">
-        <v>6.1775065139746399E-4</v>
+      <c r="F92">
+        <v>0.20984394431581799</v>
+      </c>
+      <c r="G92">
+        <v>0.38807975474248702</v>
+      </c>
+      <c r="H92">
+        <v>40.754590670165797</v>
       </c>
       <c r="I92" s="5">
         <v>12</v>
       </c>
       <c r="J92">
-        <v>6.2613365072224604E-3</v>
+        <v>3.4094216031065701</v>
       </c>
       <c r="K92">
-        <v>1.2738548571250701</v>
-      </c>
-      <c r="L92" s="4">
-        <v>26.039478958046899</v>
+        <v>9.1432898211414901</v>
+      </c>
+      <c r="L92">
+        <v>208.551274000832</v>
       </c>
       <c r="M92" s="5">
         <v>12</v>
       </c>
-      <c r="N92" s="4">
-        <v>-1.03124356431136</v>
+      <c r="N92">
+        <v>-1.02732441138881</v>
       </c>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -4524,42 +4624,42 @@
         <v>13</v>
       </c>
       <c r="B93">
-        <v>6.4568921495528203E-2</v>
+        <v>0.104292362612405</v>
       </c>
       <c r="C93">
-        <v>3.15527186631481</v>
-      </c>
-      <c r="D93" s="4">
-        <v>30.043217175964202</v>
+        <v>6.2689306791161004</v>
+      </c>
+      <c r="D93">
+        <v>68.256066878349799</v>
       </c>
       <c r="E93" s="5">
         <v>13</v>
       </c>
-      <c r="F93" s="9">
-        <v>9.5797370065819898E-5</v>
-      </c>
-      <c r="G93" s="9">
-        <v>2.16414811278431E-4</v>
-      </c>
-      <c r="H93" s="11">
-        <v>6.6825176374030095E-4</v>
+      <c r="F93">
+        <v>8.2638265025523502E-2</v>
+      </c>
+      <c r="G93">
+        <v>0.296407103806543</v>
+      </c>
+      <c r="H93">
+        <v>106.635093378748</v>
       </c>
       <c r="I93" s="5">
         <v>13</v>
       </c>
       <c r="J93">
-        <v>6.2613365072224604E-3</v>
+        <v>3.4767085185717002</v>
       </c>
       <c r="K93">
-        <v>1.1135808078815801</v>
-      </c>
-      <c r="L93" s="4">
-        <v>29.209481570366101</v>
+        <v>7.22109319935345</v>
+      </c>
+      <c r="L93">
+        <v>114.893631597466</v>
       </c>
       <c r="M93" s="5">
         <v>13</v>
       </c>
-      <c r="N93" s="4">
+      <c r="N93">
         <v>-1.03124356431136</v>
       </c>
     </row>
@@ -4568,43 +4668,43 @@
         <v>14</v>
       </c>
       <c r="B94">
-        <v>6.4568921495528203E-2</v>
+        <v>0.14401580372928799</v>
       </c>
       <c r="C94">
-        <v>2.4487590630823499</v>
-      </c>
-      <c r="D94" s="4">
-        <v>30.1918842256819</v>
+        <v>3.3546759306548801</v>
+      </c>
+      <c r="D94">
+        <v>66.669559782643105</v>
       </c>
       <c r="E94" s="5">
         <v>14</v>
       </c>
-      <c r="F94" s="9">
-        <v>1.63015493456653E-4</v>
-      </c>
-      <c r="G94" s="9">
-        <v>4.0616211098343198E-4</v>
-      </c>
-      <c r="H94" s="11">
-        <v>9.1908531982787202E-4</v>
+      <c r="F94">
+        <v>0.103919264892255</v>
+      </c>
+      <c r="G94">
+        <v>0.31103670468910399</v>
+      </c>
+      <c r="H94">
+        <v>16.569718815044801</v>
       </c>
       <c r="I94" s="5">
         <v>14</v>
       </c>
       <c r="J94">
-        <v>6.2613365072224604E-3</v>
+        <v>2.7671893566713002</v>
       </c>
       <c r="K94">
-        <v>0.93069554709332603</v>
-      </c>
-      <c r="L94" s="4">
-        <v>20.692894374424299</v>
+        <v>10.232002621242801</v>
+      </c>
+      <c r="L94">
+        <v>150.65720909816201</v>
       </c>
       <c r="M94" s="5">
         <v>14</v>
       </c>
-      <c r="N94" s="4">
-        <v>-1.03124356431136</v>
+      <c r="N94">
+        <v>-0.99511469963927401</v>
       </c>
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -4612,43 +4712,43 @@
         <v>15</v>
       </c>
       <c r="B95">
-        <v>6.4568921495524706E-2</v>
+        <v>0.183739244846165</v>
       </c>
       <c r="C95">
-        <v>1.1987785800770001</v>
-      </c>
-      <c r="D95" s="4">
-        <v>24.340199721112</v>
+        <v>4.5086005456151401</v>
+      </c>
+      <c r="D95">
+        <v>77.940345100008699</v>
       </c>
       <c r="E95" s="5">
         <v>15</v>
       </c>
-      <c r="F95" s="9">
-        <v>9.5797370065819898E-5</v>
-      </c>
-      <c r="G95" s="9">
-        <v>3.38797812932223E-4</v>
-      </c>
-      <c r="H95" s="11">
-        <v>4.8891514893789601E-4</v>
+      <c r="F95">
+        <v>0.150524552327023</v>
+      </c>
+      <c r="G95">
+        <v>4.7387705418459297E-2</v>
+      </c>
+      <c r="H95">
+        <v>55.600134900371003</v>
       </c>
       <c r="I95" s="5">
         <v>15</v>
       </c>
       <c r="J95">
-        <v>8.4170775983744894E-2</v>
+        <v>1.6866292726199501</v>
       </c>
       <c r="K95">
-        <v>4.3629473635155396</v>
-      </c>
-      <c r="L95" s="4">
-        <v>27.337200056622599</v>
+        <v>7.9659362728452399</v>
+      </c>
+      <c r="L95">
+        <v>159.57183092568499</v>
       </c>
       <c r="M95" s="5">
         <v>15</v>
       </c>
-      <c r="N95" s="4">
-        <v>-1.03124356431136</v>
+      <c r="N95">
+        <v>-0.99511469963927401</v>
       </c>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -4656,43 +4756,43 @@
         <v>16</v>
       </c>
       <c r="B96">
-        <v>1.01503933523085</v>
+        <v>1.5260617343823799</v>
       </c>
       <c r="C96">
-        <v>4.61116104722855</v>
-      </c>
-      <c r="D96" s="4">
-        <v>29.602187068574001</v>
+        <v>3.89610427743601</v>
+      </c>
+      <c r="D96">
+        <v>96.037119084598999</v>
       </c>
       <c r="E96" s="5">
         <v>16</v>
       </c>
-      <c r="F96" s="9">
-        <v>3.5889166675207002E-4</v>
-      </c>
-      <c r="G96" s="9">
-        <v>5.1788309756573003E-4</v>
-      </c>
-      <c r="H96" s="11">
-        <v>8.6690859082472205E-4</v>
+      <c r="F96">
+        <v>0.18636178220081001</v>
+      </c>
+      <c r="G96">
+        <v>0.186944421723552</v>
+      </c>
+      <c r="H96">
+        <v>59.823432862618901</v>
       </c>
       <c r="I96" s="5">
         <v>16</v>
       </c>
       <c r="J96">
-        <v>6.2613365072224604E-3</v>
+        <v>3.4767085185717002</v>
       </c>
       <c r="K96">
-        <v>0.943580494710764</v>
-      </c>
-      <c r="L96" s="4">
-        <v>22.2154187158464</v>
+        <v>7.6096116662345299</v>
+      </c>
+      <c r="L96">
+        <v>244.47403423080399</v>
       </c>
       <c r="M96" s="5">
         <v>16</v>
       </c>
-      <c r="N96" s="4">
-        <v>-1.03124356431136</v>
+      <c r="N96">
+        <v>-1.02781076098617</v>
       </c>
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -4700,43 +4800,43 @@
         <v>17</v>
       </c>
       <c r="B97">
-        <v>0.104292362612405</v>
+        <v>0.104292362612408</v>
       </c>
       <c r="C97">
-        <v>1.2146075977272801</v>
-      </c>
-      <c r="D97" s="4">
-        <v>31.335187071088299</v>
+        <v>9.78630101568322</v>
+      </c>
+      <c r="D97">
+        <v>54.754342051578703</v>
       </c>
       <c r="E97" s="5">
         <v>17</v>
       </c>
-      <c r="F97" s="9">
-        <v>3.5889166675207002E-4</v>
-      </c>
-      <c r="G97" s="9">
-        <v>4.1005281472439298E-4</v>
-      </c>
-      <c r="H97" s="11">
-        <v>5.7910353644074998E-4</v>
+      <c r="F97">
+        <v>4.6481016811383197E-2</v>
+      </c>
+      <c r="G97">
+        <v>8.1621516021107496E-2</v>
+      </c>
+      <c r="H97">
+        <v>63.779956415206598</v>
       </c>
       <c r="I97" s="5">
         <v>17</v>
       </c>
       <c r="J97">
-        <v>6.2613365072224604E-3</v>
+        <v>2.8643157898181202</v>
       </c>
       <c r="K97">
-        <v>0.92490554341207498</v>
-      </c>
-      <c r="L97" s="4">
-        <v>25.522259923633101</v>
+        <v>8.0126523897868207</v>
+      </c>
+      <c r="L97">
+        <v>149.96322424101999</v>
       </c>
       <c r="M97" s="5">
         <v>17</v>
       </c>
-      <c r="N97" s="4">
-        <v>-1.03124356431136</v>
+      <c r="N97">
+        <v>-1.0308900958220399</v>
       </c>
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -4744,43 +4844,43 @@
         <v>18</v>
       </c>
       <c r="B98">
-        <v>6.4568921495528203E-2</v>
+        <v>0.104292362612405</v>
       </c>
       <c r="C98">
-        <v>1.5777355315807799</v>
-      </c>
-      <c r="D98" s="4">
-        <v>35.6787276554778</v>
+        <v>3.6923417781991099</v>
+      </c>
+      <c r="D98">
+        <v>58.058498865319201</v>
       </c>
       <c r="E98" s="5">
         <v>18</v>
       </c>
-      <c r="F98" s="9">
-        <v>2.6358980870733097E-4</v>
-      </c>
-      <c r="G98" s="9">
-        <v>4.6481871109338403E-4</v>
-      </c>
-      <c r="H98" s="11">
-        <v>5.6049658163070904E-4</v>
+      <c r="F98">
+        <v>0.26606670660984</v>
+      </c>
+      <c r="G98">
+        <v>5.3009229277607303E-2</v>
+      </c>
+      <c r="H98">
+        <v>75.1139580706581</v>
       </c>
       <c r="I98" s="5">
         <v>18</v>
       </c>
       <c r="J98">
-        <v>6.2613365072224604E-3</v>
+        <v>4.14135505666626</v>
       </c>
       <c r="K98">
-        <v>6.3001922092448499</v>
-      </c>
-      <c r="L98" s="4">
-        <v>27.0417693039611</v>
+        <v>8.1961484884602704</v>
+      </c>
+      <c r="L98">
+        <v>155.72440513221301</v>
       </c>
       <c r="M98" s="5">
         <v>18</v>
       </c>
-      <c r="N98" s="4">
-        <v>-1.03124356431136</v>
+      <c r="N98">
+        <v>-1.02781076098617</v>
       </c>
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -4791,22 +4891,22 @@
         <v>0.104292362612405</v>
       </c>
       <c r="C99">
-        <v>1.70980097922856</v>
-      </c>
-      <c r="D99" s="4">
-        <v>27.984312623143499</v>
+        <v>5.0959430254969602</v>
+      </c>
+      <c r="D99">
+        <v>72.914245889241002</v>
       </c>
       <c r="E99" s="5">
         <v>19</v>
       </c>
-      <c r="F99" s="9">
-        <v>3.3079669169944198E-4</v>
-      </c>
-      <c r="G99" s="9">
-        <v>2.68561641261655E-4</v>
-      </c>
-      <c r="H99" s="11">
-        <v>7.0574069129947204E-4</v>
+      <c r="F99">
+        <v>0.14788293755533399</v>
+      </c>
+      <c r="G99">
+        <v>0.18689070219425499</v>
+      </c>
+      <c r="H99">
+        <v>67.575462662537205</v>
       </c>
       <c r="I99" s="5">
         <v>19</v>
@@ -4815,16 +4915,16 @@
         <v>6.2613365072224604E-3</v>
       </c>
       <c r="K99">
-        <v>1.10138273595738</v>
-      </c>
-      <c r="L99" s="4">
-        <v>25.7261086356256</v>
+        <v>6.64843284898609</v>
+      </c>
+      <c r="L99">
+        <v>144.10726366089099</v>
       </c>
       <c r="M99" s="5">
         <v>19</v>
       </c>
-      <c r="N99" s="4">
-        <v>-1.03124356431136</v>
+      <c r="N99">
+        <v>-0.99511469963927401</v>
       </c>
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -4832,43 +4932,43 @@
         <v>20</v>
       </c>
       <c r="B100">
-        <v>0.14401580372928499</v>
+        <v>2.9212600534711402</v>
       </c>
       <c r="C100">
-        <v>2.2445248936963602</v>
-      </c>
-      <c r="D100" s="4">
-        <v>27.908780937963598</v>
+        <v>6.3799206506247002</v>
+      </c>
+      <c r="D100">
+        <v>72.1238283458583</v>
       </c>
       <c r="E100" s="5">
         <v>20</v>
       </c>
-      <c r="F100" s="9">
-        <v>2.6358980870733097E-4</v>
-      </c>
-      <c r="G100" s="9">
-        <v>7.7736912863601805E-4</v>
-      </c>
-      <c r="H100" s="11">
-        <v>5.3081769801288604E-4</v>
+      <c r="F100">
+        <v>0.29113118678988498</v>
+      </c>
+      <c r="G100">
+        <v>0.28152177704444697</v>
+      </c>
+      <c r="H100">
+        <v>37.536135880259302</v>
       </c>
       <c r="I100" s="5">
         <v>20</v>
       </c>
       <c r="J100">
-        <v>6.2613365072224604E-3</v>
+        <v>2.7379884994252301</v>
       </c>
       <c r="K100">
-        <v>5.7216384585226399</v>
-      </c>
-      <c r="L100" s="4">
-        <v>25.870009050231801</v>
+        <v>74.243446188987093</v>
+      </c>
+      <c r="L100">
+        <v>159.07270422436699</v>
       </c>
       <c r="M100" s="5">
         <v>20</v>
       </c>
-      <c r="N100" s="4">
-        <v>-1.03124356431136</v>
+      <c r="N100">
+        <v>-0.99550048954989001</v>
       </c>
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -4876,43 +4976,43 @@
         <v>21</v>
       </c>
       <c r="B101">
-        <v>6.4568921495528203E-2</v>
+        <v>2.7760422173877202</v>
       </c>
       <c r="C101">
-        <v>1.2385020211939</v>
-      </c>
-      <c r="D101" s="4">
-        <v>33.1237190184901</v>
+        <v>6.9205637722373403</v>
+      </c>
+      <c r="D101">
+        <v>79.406432689268101</v>
       </c>
       <c r="E101" s="5">
         <v>21</v>
       </c>
-      <c r="F101" s="9">
-        <v>3.7548910199425301E-4</v>
-      </c>
-      <c r="G101" s="9">
-        <v>5.7359597966477605E-4</v>
-      </c>
-      <c r="H101" s="11">
-        <v>6.4949969456395897E-4</v>
+      <c r="F101">
+        <v>0.121063133374296</v>
+      </c>
+      <c r="G101">
+        <v>7.7956124823882006E-2</v>
+      </c>
+      <c r="H101">
+        <v>33.838965310762902</v>
       </c>
       <c r="I101" s="5">
         <v>21</v>
       </c>
       <c r="J101">
-        <v>6.2613365072224604E-3</v>
+        <v>2.5836371701596899</v>
       </c>
       <c r="K101">
-        <v>5.7653149210357997</v>
-      </c>
-      <c r="L101" s="4">
-        <v>26.989689257029401</v>
+        <v>8.4251373114855408</v>
+      </c>
+      <c r="L101">
+        <v>138.78312145404999</v>
       </c>
       <c r="M101" s="5">
         <v>21</v>
       </c>
-      <c r="N101" s="4">
-        <v>-1.03124356431136</v>
+      <c r="N101">
+        <v>-1.0292333137148999</v>
       </c>
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -4920,42 +5020,42 @@
         <v>22</v>
       </c>
       <c r="B102">
-        <v>6.4568921495524706E-2</v>
+        <v>0.104292362612408</v>
       </c>
       <c r="C102">
-        <v>1.2940544799610301</v>
-      </c>
-      <c r="D102" s="4">
-        <v>22.319047541794099</v>
+        <v>4.64873828967393</v>
+      </c>
+      <c r="D102">
+        <v>56.283898640792401</v>
       </c>
       <c r="E102" s="5">
         <v>22</v>
       </c>
-      <c r="F102" s="9">
-        <v>2.07715397280705E-4</v>
-      </c>
-      <c r="G102" s="9">
-        <v>2.6446997483608998E-4</v>
-      </c>
-      <c r="H102" s="11">
-        <v>5.8167089871175004E-4</v>
+      <c r="F102">
+        <v>0.102347932224424</v>
+      </c>
+      <c r="G102">
+        <v>0.13178871136800099</v>
+      </c>
+      <c r="H102">
+        <v>74.864586326571697</v>
       </c>
       <c r="I102" s="5">
         <v>22</v>
       </c>
       <c r="J102">
-        <v>6.2613365072224604E-3</v>
+        <v>4.2606587658938899</v>
       </c>
       <c r="K102">
-        <v>7.1540797063713697</v>
-      </c>
-      <c r="L102" s="4">
-        <v>27.411641993435399</v>
+        <v>6.6823417720937597</v>
+      </c>
+      <c r="L102">
+        <v>97.383327122885802</v>
       </c>
       <c r="M102" s="5">
         <v>22</v>
       </c>
-      <c r="N102" s="4">
+      <c r="N102">
         <v>-1.03124356431136</v>
       </c>
     </row>
@@ -4964,43 +5064,43 @@
         <v>23</v>
       </c>
       <c r="B103">
-        <v>6.4568921495524706E-2</v>
+        <v>0.14401580372928499</v>
       </c>
       <c r="C103">
-        <v>2.2684193171629801</v>
-      </c>
-      <c r="D103" s="4">
-        <v>29.5337408310067</v>
+        <v>9.0575146451112101</v>
+      </c>
+      <c r="D103">
+        <v>71.786404676318796</v>
       </c>
       <c r="E103" s="5">
         <v>23</v>
       </c>
-      <c r="F103" s="9">
-        <v>9.5797370065819898E-5</v>
-      </c>
-      <c r="G103" s="9">
-        <v>5.2865535877621897E-4</v>
-      </c>
-      <c r="H103" s="11">
-        <v>5.3440444233487905E-4</v>
+      <c r="F103">
+        <v>0.13725788611263801</v>
+      </c>
+      <c r="G103">
+        <v>0.24751228434749101</v>
+      </c>
+      <c r="H103">
+        <v>58.970485699666199</v>
       </c>
       <c r="I103" s="5">
         <v>23</v>
       </c>
       <c r="J103">
-        <v>6.2613365072224604E-3</v>
+        <v>5.64189945539127</v>
       </c>
       <c r="K103">
-        <v>4.0495502614305403</v>
-      </c>
-      <c r="L103" s="4">
-        <v>26.931945332211502</v>
+        <v>9.26259353036912</v>
+      </c>
+      <c r="L103">
+        <v>30.165400476482699</v>
       </c>
       <c r="M103" s="5">
         <v>23</v>
       </c>
-      <c r="N103" s="4">
-        <v>-1.03124356431136</v>
+      <c r="N103">
+        <v>-1.02781076098617</v>
       </c>
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -5008,43 +5108,43 @@
         <v>24</v>
       </c>
       <c r="B104">
-        <v>6.4568921495528203E-2</v>
+        <v>0.104292362612405</v>
       </c>
       <c r="C104">
-        <v>3.1791731803760501</v>
-      </c>
-      <c r="D104" s="4">
-        <v>26.403944456029201</v>
+        <v>8.4256998233325699</v>
+      </c>
+      <c r="D104">
+        <v>85.743204986678904</v>
       </c>
       <c r="E104" s="5">
         <v>24</v>
       </c>
-      <c r="F104" s="9">
-        <v>2.7492602703749203E-4</v>
-      </c>
-      <c r="G104" s="9">
-        <v>4.5604072869676E-4</v>
-      </c>
-      <c r="H104" s="11">
-        <v>4.9049451046989602E-4</v>
+      <c r="F104">
+        <v>5.2214257135916799E-2</v>
+      </c>
+      <c r="G104">
+        <v>6.5421438666227003E-2</v>
+      </c>
+      <c r="H104">
+        <v>30.552214673712299</v>
       </c>
       <c r="I104" s="5">
         <v>24</v>
       </c>
       <c r="J104">
-        <v>6.2613365072224604E-3</v>
+        <v>4.3601467032272803</v>
       </c>
       <c r="K104">
-        <v>5.8593424527936504</v>
-      </c>
-      <c r="L104" s="4">
-        <v>28.615002841256601</v>
+        <v>9.3250757660707109</v>
+      </c>
+      <c r="L104">
+        <v>196.69542924336099</v>
       </c>
       <c r="M104" s="5">
         <v>24</v>
       </c>
-      <c r="N104" s="4">
-        <v>-1.03124356431136</v>
+      <c r="N104">
+        <v>-1.02781076098617</v>
       </c>
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -5052,43 +5152,43 @@
         <v>25</v>
       </c>
       <c r="B105">
-        <v>6.4568921495524706E-2</v>
+        <v>0.18373924484616899</v>
       </c>
       <c r="C105">
-        <v>1.2146075977272599</v>
-      </c>
-      <c r="D105" s="4">
-        <v>23.716101736862001</v>
+        <v>5.0722346195860704</v>
+      </c>
+      <c r="D105">
+        <v>66.6664999837853</v>
       </c>
       <c r="E105" s="5">
         <v>25</v>
       </c>
-      <c r="F105" s="9">
-        <v>1.79777996420216E-4</v>
-      </c>
-      <c r="G105" s="9">
-        <v>3.3407150203934501E-4</v>
-      </c>
-      <c r="H105" s="11">
-        <v>5.3528838991179196E-4</v>
+      <c r="F105">
+        <v>0.46830152028668398</v>
+      </c>
+      <c r="G105">
+        <v>0.23867978869218101</v>
+      </c>
+      <c r="H105">
+        <v>33.499793177912501</v>
       </c>
       <c r="I105" s="5">
         <v>25</v>
       </c>
       <c r="J105">
-        <v>0.124406854575262</v>
+        <v>4.0755573190000298</v>
       </c>
       <c r="K105">
-        <v>1.12008916381485</v>
-      </c>
-      <c r="L105" s="4">
-        <v>28.116199641642901</v>
+        <v>8.6604292279761594</v>
+      </c>
+      <c r="L105">
+        <v>186.94427228309499</v>
       </c>
       <c r="M105" s="5">
         <v>25</v>
       </c>
-      <c r="N105" s="4">
-        <v>-1.03124356431136</v>
+      <c r="N105">
+        <v>-0.99511469963927401</v>
       </c>
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -5096,43 +5196,43 @@
         <v>26</v>
       </c>
       <c r="B106">
-        <v>0.104292362612405</v>
+        <v>2.3444667004699502</v>
       </c>
       <c r="C106">
-        <v>3.2347256391432002</v>
-      </c>
-      <c r="D106" s="4">
-        <v>15.112080457122699</v>
+        <v>11.2613303467871</v>
+      </c>
+      <c r="D106">
+        <v>62.785664117610402</v>
       </c>
       <c r="E106" s="5">
         <v>26</v>
       </c>
-      <c r="F106" s="9">
-        <v>2.4699049957244102E-4</v>
-      </c>
-      <c r="G106" s="9">
-        <v>4.5138592890470099E-4</v>
-      </c>
-      <c r="H106" s="11">
-        <v>6.1265190892012501E-4</v>
+      <c r="F106">
+        <v>0.18668731058749599</v>
+      </c>
+      <c r="G106">
+        <v>0.56337195215203595</v>
+      </c>
+      <c r="H106">
+        <v>14.3984418514823</v>
       </c>
       <c r="I106" s="5">
         <v>26</v>
       </c>
       <c r="J106">
-        <v>6.2613365072224604E-3</v>
+        <v>1.8731424026168999</v>
       </c>
       <c r="K106">
-        <v>3.5614034186556598</v>
-      </c>
-      <c r="L106" s="4">
-        <v>27.076010865596999</v>
+        <v>6.7023449809989204</v>
+      </c>
+      <c r="L106">
+        <v>263.86270072772402</v>
       </c>
       <c r="M106" s="5">
         <v>26</v>
       </c>
-      <c r="N106" s="4">
-        <v>-1.03124356431136</v>
+      <c r="N106">
+        <v>-1.0112694956197901</v>
       </c>
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -5140,42 +5240,42 @@
         <v>27</v>
       </c>
       <c r="B107">
-        <v>6.4568921495528203E-2</v>
+        <v>2.8815366123542598</v>
       </c>
       <c r="C107">
-        <v>1.26240333525515</v>
-      </c>
-      <c r="D107" s="4">
-        <v>25.657793302330699</v>
+        <v>4.0343676942273499</v>
+      </c>
+      <c r="D107">
+        <v>81.866973480391493</v>
       </c>
       <c r="E107" s="5">
         <v>27</v>
       </c>
-      <c r="F107" s="9">
-        <v>1.79777996420216E-4</v>
-      </c>
-      <c r="G107" s="9">
-        <v>4.34092552727194E-4</v>
-      </c>
-      <c r="H107" s="11">
-        <v>9.868347335927341E-4</v>
+      <c r="F107">
+        <v>9.9487783710024993E-2</v>
+      </c>
+      <c r="G107">
+        <v>0.366559981054289</v>
+      </c>
+      <c r="H107">
+        <v>43.398720295642001</v>
       </c>
       <c r="I107" s="5">
         <v>27</v>
       </c>
       <c r="J107">
-        <v>8.4170775983744894E-2</v>
+        <v>3.3743020021426302</v>
       </c>
       <c r="K107">
-        <v>1.33515520130431</v>
-      </c>
-      <c r="L107" s="4">
-        <v>26.8576181150226</v>
+        <v>6.5159873584495296</v>
+      </c>
+      <c r="L107">
+        <v>151.78222136075499</v>
       </c>
       <c r="M107" s="5">
         <v>27</v>
       </c>
-      <c r="N107" s="4">
+      <c r="N107">
         <v>-1.03124356431136</v>
       </c>
     </row>
@@ -5184,43 +5284,43 @@
         <v>28</v>
       </c>
       <c r="B108">
-        <v>0.14401580372928499</v>
+        <v>2.5820265430842402</v>
       </c>
       <c r="C108">
-        <v>2.268419317163</v>
-      </c>
-      <c r="D108" s="4">
-        <v>21.1765871401658</v>
+        <v>13.357523640642199</v>
+      </c>
+      <c r="D108">
+        <v>55.312956811815702</v>
       </c>
       <c r="E108" s="5">
         <v>28</v>
       </c>
-      <c r="F108" s="9">
-        <v>9.5797370065819898E-5</v>
-      </c>
-      <c r="G108" s="9">
-        <v>1.2295831479658401E-4</v>
-      </c>
-      <c r="H108" s="11">
-        <v>9.5015046742852305E-4</v>
+      <c r="F108">
+        <v>5.6764840037873403E-2</v>
+      </c>
+      <c r="G108">
+        <v>0.39937605412571497</v>
+      </c>
+      <c r="H108">
+        <v>30.679557054513101</v>
       </c>
       <c r="I108" s="5">
         <v>28</v>
       </c>
       <c r="J108">
-        <v>6.2613365072224604E-3</v>
+        <v>0.49490377369514899</v>
       </c>
       <c r="K108">
-        <v>0.65227597978180296</v>
-      </c>
-      <c r="L108" s="4">
-        <v>25.662348865846798</v>
+        <v>9.4476949772629695</v>
+      </c>
+      <c r="L108">
+        <v>43.218432292857699</v>
       </c>
       <c r="M108" s="5">
         <v>28</v>
       </c>
-      <c r="N108" s="4">
-        <v>-1.03124356431136</v>
+      <c r="N108">
+        <v>-1.02992784328481</v>
       </c>
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -5228,43 +5328,43 @@
         <v>29</v>
       </c>
       <c r="B109">
-        <v>6.4568921495524706E-2</v>
+        <v>1.3939962867346201</v>
       </c>
       <c r="C109">
-        <v>0.20858472522480201</v>
-      </c>
-      <c r="D109" s="4">
-        <v>15.352304427524301</v>
+        <v>1.6700775381116899</v>
+      </c>
+      <c r="D109">
+        <v>88.592697179645299</v>
       </c>
       <c r="E109" s="5">
         <v>29</v>
       </c>
-      <c r="F109" s="9">
-        <v>1.63015493456653E-4</v>
-      </c>
-      <c r="G109" s="9">
-        <v>3.2831940733979399E-4</v>
-      </c>
-      <c r="H109" s="11">
-        <v>4.3736155816709299E-4</v>
+      <c r="F109">
+        <v>6.9389199504553994E-2</v>
+      </c>
+      <c r="G109">
+        <v>0.43938130286958399</v>
+      </c>
+      <c r="H109">
+        <v>33.323461291893402</v>
       </c>
       <c r="I109" s="5">
         <v>29</v>
       </c>
       <c r="J109">
-        <v>6.2613365072224604E-3</v>
+        <v>0.15368684078870101</v>
       </c>
       <c r="K109">
-        <v>4.7275177059124296</v>
-      </c>
-      <c r="L109" s="4">
-        <v>29.336905515818501</v>
+        <v>6.1060557697383002</v>
+      </c>
+      <c r="L109">
+        <v>202.56656538166399</v>
       </c>
       <c r="M109" s="5">
         <v>29</v>
       </c>
-      <c r="N109" s="4">
-        <v>-1.03124356431136</v>
+      <c r="N109">
+        <v>-1.02373427886066</v>
       </c>
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -5272,43 +5372,43 @@
         <v>30</v>
       </c>
       <c r="B110">
-        <v>6.4568921495524706E-2</v>
+        <v>1.3145494045008601</v>
       </c>
       <c r="C110">
-        <v>3.47867635905145</v>
-      </c>
-      <c r="D110" s="4">
-        <v>29.777237208498001</v>
+        <v>6.6684954216249404</v>
+      </c>
+      <c r="D110">
+        <v>72.789560639546593</v>
       </c>
       <c r="E110" s="6">
         <v>30</v>
       </c>
-      <c r="F110" s="9">
-        <v>3.7548910199425301E-4</v>
-      </c>
-      <c r="G110" s="9">
-        <v>3.60907261502063E-4</v>
-      </c>
-      <c r="H110" s="11">
-        <v>6.98634794528474E-4</v>
+      <c r="F110">
+        <v>0.109006507937632</v>
+      </c>
+      <c r="G110">
+        <v>0.48869854698498899</v>
+      </c>
+      <c r="H110">
+        <v>102.118134067749</v>
       </c>
       <c r="I110" s="6">
         <v>30</v>
       </c>
       <c r="J110">
-        <v>6.2613365072224604E-3</v>
+        <v>4.14135505666626</v>
       </c>
       <c r="K110">
-        <v>6.6740234087917898</v>
-      </c>
-      <c r="L110" s="4">
-        <v>26.9675252104382</v>
+        <v>9.6190154802530898</v>
+      </c>
+      <c r="L110">
+        <v>257.03410193727501</v>
       </c>
       <c r="M110" s="6">
         <v>30</v>
       </c>
-      <c r="N110" s="4">
-        <v>-1.03124356431136</v>
+      <c r="N110">
+        <v>-0.99511469963927401</v>
       </c>
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -5317,46 +5417,46 @@
       </c>
       <c r="B111" s="7">
         <f>_xlfn.STDEV.S(B81:B110)</f>
-        <v>0.24469763973955411</v>
+        <v>1.0155115508285417</v>
       </c>
       <c r="C111" s="7">
         <f>_xlfn.STDEV.S(C81:C110)</f>
-        <v>1.1742291621182335</v>
+        <v>3.3765570259759587</v>
       </c>
       <c r="D111" s="7">
         <f>_xlfn.STDEV.S(D81:D109)</f>
-        <v>4.9502680979130753</v>
+        <v>15.204530712273581</v>
       </c>
       <c r="E111" s="7"/>
       <c r="F111" s="7">
         <f>_xlfn.STDEV.S(F81:F110)</f>
-        <v>1.2629892665104732E-4</v>
+        <v>9.731459451666595E-2</v>
       </c>
       <c r="G111" s="7">
         <f>_xlfn.STDEV.S(G81:G110)</f>
-        <v>1.6059715741623335E-4</v>
+        <v>0.15819214037055671</v>
       </c>
       <c r="H111" s="7">
         <f>_xlfn.STDEV.S(H81:H110)</f>
-        <v>1.8347562706033018E-4</v>
+        <v>23.022017115997787</v>
       </c>
       <c r="I111" s="7"/>
       <c r="J111" s="7">
         <f>_xlfn.STDEV.S(J81:J110)</f>
-        <v>0.13504355210965172</v>
+        <v>1.6204989154423699</v>
       </c>
       <c r="K111" s="7">
         <f>_xlfn.STDEV.S(K81:K110)</f>
-        <v>2.3445987678520561</v>
+        <v>17.389982683308958</v>
       </c>
       <c r="L111" s="7">
         <f>_xlfn.STDEV.S(L81:L110)</f>
-        <v>1.8864497943706144</v>
+        <v>70.700561972996766</v>
       </c>
       <c r="M111" s="7"/>
       <c r="N111" s="7">
         <f>_xlfn.STDEV.S(N81:N110)</f>
-        <v>0</v>
+        <v>1.4712182888767357E-2</v>
       </c>
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -5365,50 +5465,1553 @@
       </c>
       <c r="B112" s="7">
         <f>AVERAGE(B81:B110)</f>
-        <v>0.14514710689519539</v>
+        <v>0.91056052110121632</v>
       </c>
       <c r="C112" s="7">
         <f>AVERAGE(C81:C110)</f>
-        <v>2.1593347935221634</v>
+        <v>7.1719322031694466</v>
       </c>
       <c r="D112" s="7">
         <f>AVERAGE(D81:D110)</f>
-        <v>26.962077145068445</v>
+        <v>70.854718563415943</v>
       </c>
       <c r="E112" s="7"/>
-      <c r="F112" s="14">
+      <c r="F112" s="13">
         <f>AVERAGE(F81:F110)</f>
-        <v>2.3884062409033416E-4</v>
-      </c>
-      <c r="G112" s="14">
+        <v>0.12489978588344637</v>
+      </c>
+      <c r="G112" s="13">
         <f>AVERAGE(G81:G110)</f>
-        <v>4.0223355266233034E-4</v>
-      </c>
-      <c r="H112" s="14">
+        <v>0.23506002199208054</v>
+      </c>
+      <c r="H112" s="13">
         <f>AVERAGE(H81:H110)</f>
-        <v>6.4290707572003372E-4</v>
+        <v>50.521245301983839</v>
       </c>
       <c r="I112" s="7"/>
       <c r="J112" s="7">
         <f>AVERAGE(J81:J110)</f>
-        <v>5.8623430512223643E-2</v>
+        <v>2.7573632080631114</v>
       </c>
       <c r="K112" s="7">
         <f>AVERAGE(K81:K110)</f>
-        <v>3.2678913957656874</v>
+        <v>12.829960769469936</v>
       </c>
       <c r="L112" s="7">
         <f>AVERAGE(L81:L110)</f>
-        <v>26.674175924372033</v>
+        <v>152.07539589330949</v>
       </c>
       <c r="M112" s="7"/>
       <c r="N112" s="7">
         <f>AVERAGE(N81:N110)</f>
-        <v>-1.03124356431136</v>
+        <v>-1.0205903810606922</v>
+      </c>
+    </row>
+    <row r="115" spans="1:14" ht="20.399999999999999" x14ac:dyDescent="0.75">
+      <c r="A115" t="s">
+        <v>19</v>
+      </c>
+      <c r="C115" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D115" s="10"/>
+      <c r="E115" s="10"/>
+      <c r="F115" s="10"/>
+      <c r="G115" s="10"/>
+      <c r="H115" s="10"/>
+      <c r="I115" s="10"/>
+      <c r="J115" s="10"/>
+    </row>
+    <row r="117" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A117" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B117" s="14"/>
+      <c r="C117" s="14"/>
+      <c r="D117" s="15"/>
+      <c r="E117" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="F117" s="14"/>
+      <c r="G117" s="14"/>
+      <c r="H117" s="15"/>
+      <c r="I117" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="J117" s="14"/>
+      <c r="K117" s="14"/>
+      <c r="L117" s="15"/>
+      <c r="M117" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="N117" s="17"/>
+    </row>
+    <row r="118" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A118" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B118" s="1">
+        <v>5</v>
+      </c>
+      <c r="C118" s="1">
+        <v>10</v>
+      </c>
+      <c r="D118" s="2">
+        <v>30</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F118" s="1">
+        <v>5</v>
+      </c>
+      <c r="G118" s="1">
+        <v>10</v>
+      </c>
+      <c r="H118" s="2">
+        <v>30</v>
+      </c>
+      <c r="I118" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J118" s="1">
+        <v>5</v>
+      </c>
+      <c r="K118" s="1">
+        <v>10</v>
+      </c>
+      <c r="L118" s="2">
+        <v>30</v>
+      </c>
+      <c r="M118" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N118" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A119" s="3">
+        <v>1</v>
+      </c>
+      <c r="B119">
+        <v>1.9899181141865701</v>
+      </c>
+      <c r="C119">
+        <v>6.9647083697034997</v>
+      </c>
+      <c r="D119">
+        <v>41.887724661491703</v>
+      </c>
+      <c r="E119" s="3">
+        <v>1</v>
+      </c>
+      <c r="F119">
+        <v>9.3569190481166895E-2</v>
+      </c>
+      <c r="G119">
+        <v>0.47971491457079002</v>
+      </c>
+      <c r="H119">
+        <v>1.0663696924044099</v>
+      </c>
+      <c r="I119" s="3">
+        <v>1</v>
+      </c>
+      <c r="J119">
+        <v>0</v>
+      </c>
+      <c r="K119">
+        <v>2.2540928482041198</v>
+      </c>
+      <c r="L119">
+        <v>28.929758132054399</v>
+      </c>
+      <c r="M119" s="3">
+        <v>1</v>
+      </c>
+      <c r="N119">
+        <v>-1.0316284534898701</v>
+      </c>
+    </row>
+    <row r="120" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A120" s="5">
+        <v>2</v>
+      </c>
+      <c r="B120">
+        <v>2.9848771712798601</v>
+      </c>
+      <c r="C120">
+        <v>4.9747953469404997</v>
+      </c>
+      <c r="D120">
+        <v>48.651328335336899</v>
+      </c>
+      <c r="E120" s="5">
+        <v>2</v>
+      </c>
+      <c r="F120">
+        <v>0.103455970025146</v>
+      </c>
+      <c r="G120">
+        <v>9.5925010283977194E-2</v>
+      </c>
+      <c r="H120">
+        <v>0.98419674949678504</v>
+      </c>
+      <c r="I120" s="5">
+        <v>2</v>
+      </c>
+      <c r="J120">
+        <v>0</v>
+      </c>
+      <c r="K120">
+        <v>1.5119844121653701</v>
+      </c>
+      <c r="L120">
+        <v>28.774294380370399</v>
+      </c>
+      <c r="M120" s="5">
+        <v>2</v>
+      </c>
+      <c r="N120">
+        <v>-1.0316284534898701</v>
+      </c>
+    </row>
+    <row r="121" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A121" s="5">
+        <v>3</v>
+      </c>
+      <c r="B121">
+        <v>1.9899181141865701</v>
+      </c>
+      <c r="C121">
+        <v>13.9293914891344</v>
+      </c>
+      <c r="D121">
+        <v>53.078081713392898</v>
+      </c>
+      <c r="E121" s="5">
+        <v>3</v>
+      </c>
+      <c r="F121">
+        <v>0.110861840729007</v>
+      </c>
+      <c r="G121">
+        <v>7.1295419232095397E-2</v>
+      </c>
+      <c r="H121">
+        <v>0.95328746839721401</v>
+      </c>
+      <c r="I121" s="5">
+        <v>3</v>
+      </c>
+      <c r="J121">
+        <v>0</v>
+      </c>
+      <c r="K121">
+        <v>1.67441616665052</v>
+      </c>
+      <c r="L121">
+        <v>28.3093517123068</v>
+      </c>
+      <c r="M121" s="5">
+        <v>3</v>
+      </c>
+      <c r="N121">
+        <v>-1.0316284534898701</v>
+      </c>
+    </row>
+    <row r="122" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A122" s="5">
+        <v>4</v>
+      </c>
+      <c r="B122">
+        <v>0.99495905709328902</v>
+      </c>
+      <c r="C122">
+        <v>11.9415213208114</v>
+      </c>
+      <c r="D122">
+        <v>73.228011126704601</v>
+      </c>
+      <c r="E122" s="5">
+        <v>4</v>
+      </c>
+      <c r="F122">
+        <v>8.6281426938601705E-2</v>
+      </c>
+      <c r="G122">
+        <v>0.32986685854671299</v>
+      </c>
+      <c r="H122">
+        <v>1.0989282828876501</v>
+      </c>
+      <c r="I122" s="5">
+        <v>4</v>
+      </c>
+      <c r="J122">
+        <v>0.23475658737432401</v>
+      </c>
+      <c r="K122">
+        <v>75.604873122503705</v>
+      </c>
+      <c r="L122">
+        <v>28.6271953150831</v>
+      </c>
+      <c r="M122" s="5">
+        <v>4</v>
+      </c>
+      <c r="N122">
+        <v>-1.0316284534898701</v>
+      </c>
+    </row>
+    <row r="123" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A123" s="5">
+        <v>5</v>
+      </c>
+      <c r="B123">
+        <v>0</v>
+      </c>
+      <c r="C123">
+        <v>13.929416723667901</v>
+      </c>
+      <c r="D123">
+        <v>44.155972428451101</v>
+      </c>
+      <c r="E123" s="5">
+        <v>5</v>
+      </c>
+      <c r="F123">
+        <v>0.123165632137446</v>
+      </c>
+      <c r="G123">
+        <v>0.174741364577677</v>
+      </c>
+      <c r="H123">
+        <v>1.0366333049766701</v>
+      </c>
+      <c r="I123" s="5">
+        <v>5</v>
+      </c>
+      <c r="J123">
+        <v>0</v>
+      </c>
+      <c r="K123" s="9">
+        <v>3.4353856929576601E-6</v>
+      </c>
+      <c r="L123">
+        <v>29.290032376046302</v>
+      </c>
+      <c r="M123" s="5">
+        <v>5</v>
+      </c>
+      <c r="N123">
+        <v>-1.0316284534898701</v>
+      </c>
+    </row>
+    <row r="124" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A124" s="5">
+        <v>6</v>
+      </c>
+      <c r="B124">
+        <v>2.9848771712798601</v>
+      </c>
+      <c r="C124">
+        <v>6.9649647681889402</v>
+      </c>
+      <c r="D124">
+        <v>93.4949265211594</v>
+      </c>
+      <c r="E124" s="5">
+        <v>6</v>
+      </c>
+      <c r="F124">
+        <v>9.6064858848379495E-2</v>
+      </c>
+      <c r="G124">
+        <v>0.16246242137150499</v>
+      </c>
+      <c r="H124">
+        <v>0.69222577131455898</v>
+      </c>
+      <c r="I124" s="5">
+        <v>6</v>
+      </c>
+      <c r="J124">
+        <v>0</v>
+      </c>
+      <c r="K124">
+        <v>2.2309590438667599</v>
+      </c>
+      <c r="L124">
+        <v>28.980594225543701</v>
+      </c>
+      <c r="M124" s="5">
+        <v>6</v>
+      </c>
+      <c r="N124">
+        <v>-1.0316284534898701</v>
+      </c>
+    </row>
+    <row r="125" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A125" s="5">
+        <v>7</v>
+      </c>
+      <c r="B125">
+        <v>0.99495905709328902</v>
+      </c>
+      <c r="C125">
+        <v>4.97855359954821</v>
+      </c>
+      <c r="D125">
+        <v>57.595409335274297</v>
+      </c>
+      <c r="E125" s="5">
+        <v>7</v>
+      </c>
+      <c r="F125">
+        <v>0.120674855577348</v>
+      </c>
+      <c r="G125">
+        <v>0.15749554809147601</v>
+      </c>
+      <c r="H125">
+        <v>1.0609594431068601</v>
+      </c>
+      <c r="I125" s="5">
+        <v>7</v>
+      </c>
+      <c r="J125">
+        <v>3.9308394341330199</v>
+      </c>
+      <c r="K125">
+        <v>0.55799625911086004</v>
+      </c>
+      <c r="L125">
+        <v>28.868049481373198</v>
+      </c>
+      <c r="M125" s="5">
+        <v>7</v>
+      </c>
+      <c r="N125">
+        <v>-1.0316284534898701</v>
+      </c>
+    </row>
+    <row r="126" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A126" s="5">
+        <v>8</v>
+      </c>
+      <c r="B126">
+        <v>0.99495905709328902</v>
+      </c>
+      <c r="C126">
+        <v>2.9848771712804298</v>
+      </c>
+      <c r="D126">
+        <v>59.9350445526876</v>
+      </c>
+      <c r="E126" s="5">
+        <v>8</v>
+      </c>
+      <c r="F126">
+        <v>6.4056360232641898E-2</v>
+      </c>
+      <c r="G126">
+        <v>0.132802019682668</v>
+      </c>
+      <c r="H126">
+        <v>0.97141803019763395</v>
+      </c>
+      <c r="I126" s="5">
+        <v>8</v>
+      </c>
+      <c r="J126">
+        <v>0</v>
+      </c>
+      <c r="K126">
+        <v>0.50862302098912104</v>
+      </c>
+      <c r="L126">
+        <v>97.731428411434393</v>
+      </c>
+      <c r="M126" s="5">
+        <v>8</v>
+      </c>
+      <c r="N126">
+        <v>-1.0316284534898701</v>
+      </c>
+    </row>
+    <row r="127" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A127" s="5">
+        <v>9</v>
+      </c>
+      <c r="B127">
+        <v>0.99495905709328902</v>
+      </c>
+      <c r="C127">
+        <v>8.9546264760788894</v>
+      </c>
+      <c r="D127">
+        <v>82.588260767113695</v>
+      </c>
+      <c r="E127" s="5">
+        <v>9</v>
+      </c>
+      <c r="F127">
+        <v>0.118275142369982</v>
+      </c>
+      <c r="G127">
+        <v>0.45992674426823499</v>
+      </c>
+      <c r="H127">
+        <v>1.00768040783928</v>
+      </c>
+      <c r="I127" s="5">
+        <v>9</v>
+      </c>
+      <c r="J127">
+        <v>0</v>
+      </c>
+      <c r="K127">
+        <v>4.0697902688932297</v>
+      </c>
+      <c r="L127">
+        <v>28.234708439286901</v>
+      </c>
+      <c r="M127" s="5">
+        <v>9</v>
+      </c>
+      <c r="N127">
+        <v>-1.0316284534898701</v>
+      </c>
+    </row>
+    <row r="128" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A128" s="5">
+        <v>10</v>
+      </c>
+      <c r="B128">
+        <v>1.9899181141865701</v>
+      </c>
+      <c r="C128">
+        <v>25.869032235770199</v>
+      </c>
+      <c r="D128">
+        <v>63.255009314771598</v>
+      </c>
+      <c r="E128" s="5">
+        <v>10</v>
+      </c>
+      <c r="F128">
+        <v>8.6222352528917107E-2</v>
+      </c>
+      <c r="G128">
+        <v>3.1998722453121603E-2</v>
+      </c>
+      <c r="H128">
+        <v>1.03736890441344</v>
+      </c>
+      <c r="I128" s="5">
+        <v>10</v>
+      </c>
+      <c r="J128">
+        <v>0</v>
+      </c>
+      <c r="K128">
+        <v>1.1344763208373001</v>
+      </c>
+      <c r="L128">
+        <v>28.633825117895</v>
+      </c>
+      <c r="M128" s="5">
+        <v>10</v>
+      </c>
+      <c r="N128">
+        <v>-1.0316284534898701</v>
+      </c>
+    </row>
+    <row r="129" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A129" s="5">
+        <v>11</v>
+      </c>
+      <c r="B129">
+        <v>0.99495905709328902</v>
+      </c>
+      <c r="C129">
+        <v>7.9596674189274097</v>
+      </c>
+      <c r="D129">
+        <v>47.572117289489697</v>
+      </c>
+      <c r="E129" s="5">
+        <v>11</v>
+      </c>
+      <c r="F129">
+        <v>0.17002275692288199</v>
+      </c>
+      <c r="G129">
+        <v>9.3554507301592704E-2</v>
+      </c>
+      <c r="H129">
+        <v>0.77192994544576798</v>
+      </c>
+      <c r="I129" s="5">
+        <v>11</v>
+      </c>
+      <c r="J129">
+        <v>0</v>
+      </c>
+      <c r="K129">
+        <v>0.235408964331804</v>
+      </c>
+      <c r="L129">
+        <v>29.309168575566002</v>
+      </c>
+      <c r="M129" s="5">
+        <v>11</v>
+      </c>
+      <c r="N129">
+        <v>-1.0316284534898701</v>
+      </c>
+    </row>
+    <row r="130" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A130" s="5">
+        <v>12</v>
+      </c>
+      <c r="B130">
+        <v>0.99495905709328902</v>
+      </c>
+      <c r="C130">
+        <v>8.9546264761501693</v>
+      </c>
+      <c r="D130">
+        <v>91.166776337329793</v>
+      </c>
+      <c r="E130" s="5">
+        <v>12</v>
+      </c>
+      <c r="F130">
+        <v>0.105951666972413</v>
+      </c>
+      <c r="G130">
+        <v>8.6040758008425797E-2</v>
+      </c>
+      <c r="H130">
+        <v>1.10557070319575</v>
+      </c>
+      <c r="I130" s="5">
+        <v>12</v>
+      </c>
+      <c r="J130">
+        <v>0</v>
+      </c>
+      <c r="K130">
+        <v>4.0448894091445</v>
+      </c>
+      <c r="L130">
+        <v>26.806733055002901</v>
+      </c>
+      <c r="M130" s="5">
+        <v>12</v>
+      </c>
+      <c r="N130">
+        <v>-1.0316284534898701</v>
+      </c>
+    </row>
+    <row r="131" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A131" s="5">
+        <v>13</v>
+      </c>
+      <c r="B131">
+        <v>2.9848771712798601</v>
+      </c>
+      <c r="C131">
+        <v>10.9445445902077</v>
+      </c>
+      <c r="D131">
+        <v>47.264365242693401</v>
+      </c>
+      <c r="E131" s="5">
+        <v>13</v>
+      </c>
+      <c r="F131">
+        <v>0.14781004781238599</v>
+      </c>
+      <c r="G131">
+        <v>0.24613246959867099</v>
+      </c>
+      <c r="H131">
+        <v>1.0308945984839299</v>
+      </c>
+      <c r="I131" s="5">
+        <v>13</v>
+      </c>
+      <c r="J131">
+        <v>0</v>
+      </c>
+      <c r="K131">
+        <v>1.71651994085057</v>
+      </c>
+      <c r="L131">
+        <v>28.550773518775301</v>
+      </c>
+      <c r="M131" s="5">
+        <v>13</v>
+      </c>
+      <c r="N131">
+        <v>-1.0316284534898701</v>
+      </c>
+    </row>
+    <row r="132" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A132" s="5">
+        <v>14</v>
+      </c>
+      <c r="B132">
+        <v>1.9899181141865701</v>
+      </c>
+      <c r="C132">
+        <v>2.98487771672663</v>
+      </c>
+      <c r="D132">
+        <v>51.769628961806099</v>
+      </c>
+      <c r="E132" s="5">
+        <v>14</v>
+      </c>
+      <c r="F132">
+        <v>0.118211188918062</v>
+      </c>
+      <c r="G132">
+        <v>0.37142269514593002</v>
+      </c>
+      <c r="H132">
+        <v>1.0489576296488701</v>
+      </c>
+      <c r="I132" s="5">
+        <v>14</v>
+      </c>
+      <c r="J132">
+        <v>0</v>
+      </c>
+      <c r="K132">
+        <v>1.05484754521933</v>
+      </c>
+      <c r="L132">
+        <v>29.0347619437328</v>
+      </c>
+      <c r="M132" s="5">
+        <v>14</v>
+      </c>
+      <c r="N132">
+        <v>-1.0316284534898701</v>
+      </c>
+    </row>
+    <row r="133" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A133" s="5">
+        <v>15</v>
+      </c>
+      <c r="B133">
+        <v>1.9899181141865701</v>
+      </c>
+      <c r="C133">
+        <v>7.9603621633008297</v>
+      </c>
+      <c r="D133">
+        <v>51.302686693069603</v>
+      </c>
+      <c r="E133" s="5">
+        <v>15</v>
+      </c>
+      <c r="F133">
+        <v>0.184672233207372</v>
+      </c>
+      <c r="G133">
+        <v>0.19672363579501001</v>
+      </c>
+      <c r="H133">
+        <v>1.1040752250860499</v>
+      </c>
+      <c r="I133" s="5">
+        <v>15</v>
+      </c>
+      <c r="J133">
+        <v>0</v>
+      </c>
+      <c r="K133">
+        <v>2.0903890075566198</v>
+      </c>
+      <c r="L133">
+        <v>31.8111692238977</v>
+      </c>
+      <c r="M133" s="5">
+        <v>15</v>
+      </c>
+      <c r="N133">
+        <v>-1.0316284534898701</v>
+      </c>
+    </row>
+    <row r="134" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A134" s="5">
+        <v>16</v>
+      </c>
+      <c r="B134">
+        <v>0.99495905709328902</v>
+      </c>
+      <c r="C134">
+        <v>9.9495855331620202</v>
+      </c>
+      <c r="D134">
+        <v>72.774542312458607</v>
+      </c>
+      <c r="E134" s="5">
+        <v>16</v>
+      </c>
+      <c r="F134">
+        <v>8.3802928679961905E-2</v>
+      </c>
+      <c r="G134">
+        <v>5.4113144090342701E-2</v>
+      </c>
+      <c r="H134">
+        <v>0.88066094109394899</v>
+      </c>
+      <c r="I134" s="5">
+        <v>16</v>
+      </c>
+      <c r="J134">
+        <v>0</v>
+      </c>
+      <c r="K134">
+        <v>3.7882375964408199</v>
+      </c>
+      <c r="L134">
+        <v>28.405238052929001</v>
+      </c>
+      <c r="M134" s="5">
+        <v>16</v>
+      </c>
+      <c r="N134">
+        <v>-1.0316284534898701</v>
+      </c>
+    </row>
+    <row r="135" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A135" s="5">
+        <v>17</v>
+      </c>
+      <c r="B135">
+        <v>0.99495905709328902</v>
+      </c>
+      <c r="C135">
+        <v>5.9697543425597503</v>
+      </c>
+      <c r="D135">
+        <v>79.795725447226303</v>
+      </c>
+      <c r="E135" s="5">
+        <v>17</v>
+      </c>
+      <c r="F135">
+        <v>9.11423598552209E-2</v>
+      </c>
+      <c r="G135">
+        <v>0.33226394171069301</v>
+      </c>
+      <c r="H135">
+        <v>1.0234646153282001</v>
+      </c>
+      <c r="I135" s="5">
+        <v>17</v>
+      </c>
+      <c r="J135">
+        <v>3.9308394341330199</v>
+      </c>
+      <c r="K135" s="9">
+        <v>2.7330101441276801E-4</v>
+      </c>
+      <c r="L135">
+        <v>25.2505944878775</v>
+      </c>
+      <c r="M135" s="5">
+        <v>17</v>
+      </c>
+      <c r="N135">
+        <v>-1.0316284534898701</v>
+      </c>
+    </row>
+    <row r="136" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A136" s="5">
+        <v>18</v>
+      </c>
+      <c r="B136">
+        <v>0.99495905709328902</v>
+      </c>
+      <c r="C136">
+        <v>15.9200394674665</v>
+      </c>
+      <c r="D136">
+        <v>56.105247035514502</v>
+      </c>
+      <c r="E136" s="5">
+        <v>18</v>
+      </c>
+      <c r="F136">
+        <v>0.18479024242390399</v>
+      </c>
+      <c r="G136">
+        <v>6.4021972180924203E-2</v>
+      </c>
+      <c r="H136">
+        <v>0.92974371352303897</v>
+      </c>
+      <c r="I136" s="5">
+        <v>18</v>
+      </c>
+      <c r="J136">
+        <v>0</v>
+      </c>
+      <c r="K136">
+        <v>3.2336653272498599</v>
+      </c>
+      <c r="L136">
+        <v>29.1047565026679</v>
+      </c>
+      <c r="M136" s="5">
+        <v>18</v>
+      </c>
+      <c r="N136">
+        <v>-1.0316284534898701</v>
+      </c>
+    </row>
+    <row r="137" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A137" s="5">
+        <v>19</v>
+      </c>
+      <c r="B137">
+        <v>1.9899181141865701</v>
+      </c>
+      <c r="C137">
+        <v>6.9647133996531103</v>
+      </c>
+      <c r="D137">
+        <v>72.629870367304903</v>
+      </c>
+      <c r="E137" s="5">
+        <v>19</v>
+      </c>
+      <c r="F137">
+        <v>0.16013353928783899</v>
+      </c>
+      <c r="G137">
+        <v>0.12790405591238499</v>
+      </c>
+      <c r="H137">
+        <v>1.0387725504063401</v>
+      </c>
+      <c r="I137" s="5">
+        <v>19</v>
+      </c>
+      <c r="J137">
+        <v>0</v>
+      </c>
+      <c r="K137" s="9">
+        <v>6.12453176830273E-9</v>
+      </c>
+      <c r="L137">
+        <v>28.840458194214701</v>
+      </c>
+      <c r="M137" s="5">
+        <v>19</v>
+      </c>
+      <c r="N137">
+        <v>-1.0316284534898701</v>
+      </c>
+    </row>
+    <row r="138" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A138" s="5">
+        <v>20</v>
+      </c>
+      <c r="B138">
+        <v>1.9899181141865701</v>
+      </c>
+      <c r="C138">
+        <v>6.9679434060875103</v>
+      </c>
+      <c r="D138">
+        <v>109.56941909200199</v>
+      </c>
+      <c r="E138" s="5">
+        <v>20</v>
+      </c>
+      <c r="F138">
+        <v>8.0633636230664094E-2</v>
+      </c>
+      <c r="G138">
+        <v>8.1142828165025604E-2</v>
+      </c>
+      <c r="H138">
+        <v>0.943592549485884</v>
+      </c>
+      <c r="I138" s="5">
+        <v>20</v>
+      </c>
+      <c r="J138">
+        <v>0</v>
+      </c>
+      <c r="K138" s="9">
+        <v>4.3982011750285203E-9</v>
+      </c>
+      <c r="L138">
+        <v>35.764750473961797</v>
+      </c>
+      <c r="M138" s="5">
+        <v>20</v>
+      </c>
+      <c r="N138">
+        <v>-1.0316284534898701</v>
+      </c>
+    </row>
+    <row r="139" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A139" s="5">
+        <v>21</v>
+      </c>
+      <c r="B139">
+        <v>0</v>
+      </c>
+      <c r="C139">
+        <v>13.929416723667901</v>
+      </c>
+      <c r="D139">
+        <v>43.844444719496501</v>
+      </c>
+      <c r="E139" s="5">
+        <v>21</v>
+      </c>
+      <c r="F139">
+        <v>0.184672233207372</v>
+      </c>
+      <c r="G139">
+        <v>6.15337985864816E-2</v>
+      </c>
+      <c r="H139">
+        <v>0.91629590234568203</v>
+      </c>
+      <c r="I139" s="5">
+        <v>21</v>
+      </c>
+      <c r="J139">
+        <v>0</v>
+      </c>
+      <c r="K139">
+        <v>0.235423739004855</v>
+      </c>
+      <c r="L139">
+        <v>28.7207440606233</v>
+      </c>
+      <c r="M139" s="5">
+        <v>21</v>
+      </c>
+      <c r="N139">
+        <v>-1.0316284534898701</v>
+      </c>
+    </row>
+    <row r="140" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A140" s="5">
+        <v>22</v>
+      </c>
+      <c r="B140">
+        <v>0.99495905709328902</v>
+      </c>
+      <c r="C140">
+        <v>9.9617052841235196</v>
+      </c>
+      <c r="D140">
+        <v>43.606997425394297</v>
+      </c>
+      <c r="E140" s="5">
+        <v>22</v>
+      </c>
+      <c r="F140">
+        <v>9.1159579720755904E-2</v>
+      </c>
+      <c r="G140">
+        <v>0.16967657295157099</v>
+      </c>
+      <c r="H140">
+        <v>0.953918443266913</v>
+      </c>
+      <c r="I140" s="5">
+        <v>22</v>
+      </c>
+      <c r="J140">
+        <v>0</v>
+      </c>
+      <c r="K140">
+        <v>4.4108623821928798</v>
+      </c>
+      <c r="L140">
+        <v>27.916009062089</v>
+      </c>
+      <c r="M140" s="5">
+        <v>22</v>
+      </c>
+      <c r="N140">
+        <v>-1.0316284534898701</v>
+      </c>
+    </row>
+    <row r="141" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A141" s="5">
+        <v>23</v>
+      </c>
+      <c r="B141">
+        <v>2.9848771712798601</v>
+      </c>
+      <c r="C141">
+        <v>8.9546264760207901</v>
+      </c>
+      <c r="D141">
+        <v>54.206227086749699</v>
+      </c>
+      <c r="E141" s="5">
+        <v>23</v>
+      </c>
+      <c r="F141">
+        <v>6.4076038102982097E-2</v>
+      </c>
+      <c r="G141">
+        <v>9.1014817647518398E-2</v>
+      </c>
+      <c r="H141">
+        <v>0.86271672169237801</v>
+      </c>
+      <c r="I141" s="5">
+        <v>23</v>
+      </c>
+      <c r="J141">
+        <v>0</v>
+      </c>
+      <c r="K141">
+        <v>2.0923664540805298</v>
+      </c>
+      <c r="L141">
+        <v>990.77904692273103</v>
+      </c>
+      <c r="M141" s="5">
+        <v>23</v>
+      </c>
+      <c r="N141">
+        <v>-1.0316284534898701</v>
+      </c>
+    </row>
+    <row r="142" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A142" s="5">
+        <v>24</v>
+      </c>
+      <c r="B142">
+        <v>5.9697493047406596</v>
+      </c>
+      <c r="C142">
+        <v>7.9871816371284998</v>
+      </c>
+      <c r="D142">
+        <v>61.022082623270002</v>
+      </c>
+      <c r="E142" s="5">
+        <v>24</v>
+      </c>
+      <c r="F142">
+        <v>7.6360119607640206E-2</v>
+      </c>
+      <c r="G142">
+        <v>0.34202011322151499</v>
+      </c>
+      <c r="H142">
+        <v>1.0489611662792</v>
+      </c>
+      <c r="I142" s="5">
+        <v>24</v>
+      </c>
+      <c r="J142">
+        <v>0</v>
+      </c>
+      <c r="K142">
+        <v>5.2328612076557999</v>
+      </c>
+      <c r="L142">
+        <v>28.118056510773702</v>
+      </c>
+      <c r="M142" s="5">
+        <v>24</v>
+      </c>
+      <c r="N142">
+        <v>-1.0316284534898701</v>
+      </c>
+    </row>
+    <row r="143" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A143" s="5">
+        <v>25</v>
+      </c>
+      <c r="B143">
+        <v>0.99495905709328902</v>
+      </c>
+      <c r="C143">
+        <v>3.9798363025441601</v>
+      </c>
+      <c r="D143">
+        <v>54.9608171085995</v>
+      </c>
+      <c r="E143" s="5">
+        <v>25</v>
+      </c>
+      <c r="F143">
+        <v>0.164942892756508</v>
+      </c>
+      <c r="G143">
+        <v>0.216354561721082</v>
+      </c>
+      <c r="H143">
+        <v>0.94779133625482404</v>
+      </c>
+      <c r="I143" s="5">
+        <v>25</v>
+      </c>
+      <c r="J143">
+        <v>3.9308394341330199</v>
+      </c>
+      <c r="K143">
+        <v>0.100354924893996</v>
+      </c>
+      <c r="L143">
+        <v>984.17480478553398</v>
+      </c>
+      <c r="M143" s="5">
+        <v>25</v>
+      </c>
+      <c r="N143">
+        <v>-1.0316284534898701</v>
+      </c>
+    </row>
+    <row r="144" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A144" s="5">
+        <v>26</v>
+      </c>
+      <c r="B144">
+        <v>2.9848771712798601</v>
+      </c>
+      <c r="C144">
+        <v>8.9546264760205894</v>
+      </c>
+      <c r="D144">
+        <v>47.304677690811801</v>
+      </c>
+      <c r="E144" s="5">
+        <v>26</v>
+      </c>
+      <c r="F144">
+        <v>0.14781004781238599</v>
+      </c>
+      <c r="G144">
+        <v>0.11573055787809999</v>
+      </c>
+      <c r="H144">
+        <v>1.0477107347982499</v>
+      </c>
+      <c r="I144" s="5">
+        <v>26</v>
+      </c>
+      <c r="J144">
+        <v>0</v>
+      </c>
+      <c r="K144">
+        <v>0.67608745382382196</v>
+      </c>
+      <c r="L144">
+        <v>106.370274346909</v>
+      </c>
+      <c r="M144" s="5">
+        <v>26</v>
+      </c>
+      <c r="N144">
+        <v>-1.0316284534898701</v>
+      </c>
+    </row>
+    <row r="145" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A145" s="5">
+        <v>27</v>
+      </c>
+      <c r="B145">
+        <v>0</v>
+      </c>
+      <c r="C145">
+        <v>11.939498609481801</v>
+      </c>
+      <c r="D145">
+        <v>80.245263381135601</v>
+      </c>
+      <c r="E145" s="5">
+        <v>27</v>
+      </c>
+      <c r="F145">
+        <v>3.4491896342113797E-2</v>
+      </c>
+      <c r="G145">
+        <v>0.32016401805712502</v>
+      </c>
+      <c r="H145">
+        <v>0.71182439164641298</v>
+      </c>
+      <c r="I145" s="5">
+        <v>27</v>
+      </c>
+      <c r="J145">
+        <v>0</v>
+      </c>
+      <c r="K145">
+        <v>0.916186837260342</v>
+      </c>
+      <c r="L145">
+        <v>29.368048113376901</v>
+      </c>
+      <c r="M145" s="5">
+        <v>27</v>
+      </c>
+      <c r="N145">
+        <v>-1.0316284534898701</v>
+      </c>
+    </row>
+    <row r="146" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A146" s="5">
+        <v>28</v>
+      </c>
+      <c r="B146">
+        <v>3.97983119055408</v>
+      </c>
+      <c r="C146">
+        <v>0.99495905910401194</v>
+      </c>
+      <c r="D146">
+        <v>32.603692796141097</v>
+      </c>
+      <c r="E146" s="5">
+        <v>28</v>
+      </c>
+      <c r="F146">
+        <v>0.12808075148951101</v>
+      </c>
+      <c r="G146">
+        <v>0.33478909891083702</v>
+      </c>
+      <c r="H146">
+        <v>1.0075912954398301</v>
+      </c>
+      <c r="I146" s="5">
+        <v>28</v>
+      </c>
+      <c r="J146">
+        <v>0</v>
+      </c>
+      <c r="K146">
+        <v>3.3245914765528499</v>
+      </c>
+      <c r="L146">
+        <v>27.950047782063798</v>
+      </c>
+      <c r="M146" s="5">
+        <v>28</v>
+      </c>
+      <c r="N146">
+        <v>-1.0316284534898701</v>
+      </c>
+    </row>
+    <row r="147" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A147" s="5">
+        <v>29</v>
+      </c>
+      <c r="B147">
+        <v>0</v>
+      </c>
+      <c r="C147">
+        <v>4.9940626281733804</v>
+      </c>
+      <c r="D147">
+        <v>40.860344350771904</v>
+      </c>
+      <c r="E147" s="5">
+        <v>29</v>
+      </c>
+      <c r="F147">
+        <v>0.18223559161986699</v>
+      </c>
+      <c r="G147">
+        <v>0.31725476761141602</v>
+      </c>
+      <c r="H147">
+        <v>8.7121205002846391</v>
+      </c>
+      <c r="I147" s="5">
+        <v>29</v>
+      </c>
+      <c r="J147">
+        <v>0</v>
+      </c>
+      <c r="K147">
+        <v>2.9995044407196199</v>
+      </c>
+      <c r="L147">
+        <v>86.327995972493099</v>
+      </c>
+      <c r="M147" s="5">
+        <v>29</v>
+      </c>
+      <c r="N147">
+        <v>-1.0316284534898701</v>
+      </c>
+    </row>
+    <row r="148" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A148" s="6">
+        <v>30</v>
+      </c>
+      <c r="B148">
+        <v>1.9899181141865701</v>
+      </c>
+      <c r="C148">
+        <v>21.889079104776101</v>
+      </c>
+      <c r="D148">
+        <v>26.766715937506799</v>
+      </c>
+      <c r="E148" s="6">
+        <v>30</v>
+      </c>
+      <c r="F148">
+        <v>0.384247063899949</v>
+      </c>
+      <c r="G148">
+        <v>0.162131696462083</v>
+      </c>
+      <c r="H148">
+        <v>12.0458307060347</v>
+      </c>
+      <c r="I148" s="6">
+        <v>30</v>
+      </c>
+      <c r="J148">
+        <v>0</v>
+      </c>
+      <c r="K148">
+        <v>5.8927718529956197</v>
+      </c>
+      <c r="L148">
+        <v>114.22573512157</v>
+      </c>
+      <c r="M148" s="6">
+        <v>30</v>
+      </c>
+      <c r="N148">
+        <v>-1.0316284534898701</v>
+      </c>
+    </row>
+    <row r="149" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A149" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B149" s="7">
+        <f>_xlfn.STDEV.S(B119:B148)</f>
+        <v>1.3047012909413502</v>
+      </c>
+      <c r="C149" s="7">
+        <f>_xlfn.STDEV.S(C119:C148)</f>
+        <v>5.3507161530901088</v>
+      </c>
+      <c r="D149" s="7">
+        <f>_xlfn.STDEV.S(D119:D147)</f>
+        <v>18.386590622006004</v>
+      </c>
+      <c r="E149" s="7"/>
+      <c r="F149" s="7">
+        <f>_xlfn.STDEV.S(F119:F148)</f>
+        <v>6.3503793769885658E-2</v>
+      </c>
+      <c r="G149" s="7">
+        <f>_xlfn.STDEV.S(G119:G148)</f>
+        <v>0.12675147708539752</v>
+      </c>
+      <c r="H149" s="7">
+        <f>_xlfn.STDEV.S(H119:H148)</f>
+        <v>2.4281129772138379</v>
+      </c>
+      <c r="I149" s="7"/>
+      <c r="J149" s="7">
+        <f>_xlfn.STDEV.S(J119:J148)</f>
+        <v>1.1975227579290526</v>
+      </c>
+      <c r="K149" s="7">
+        <f>_xlfn.STDEV.S(K119:K148)</f>
+        <v>13.556334347739213</v>
+      </c>
+      <c r="L149" s="7">
+        <f>_xlfn.STDEV.S(L119:L148)</f>
+        <v>241.89707685900444</v>
+      </c>
+      <c r="M149" s="7"/>
+      <c r="N149" s="7">
+        <f>_xlfn.STDEV.S(N119:N148)</f>
+        <v>6.7752154249004421E-16</v>
+      </c>
+    </row>
+    <row r="150" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A150" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B150" s="7">
+        <f>AVERAGE(B119:B148)</f>
+        <v>1.7245953631070927</v>
+      </c>
+      <c r="C150" s="7">
+        <f>AVERAGE(C119:C148)</f>
+        <v>9.3217664772135596</v>
+      </c>
+      <c r="D150" s="7">
+        <f>AVERAGE(D119:D148)</f>
+        <v>59.441380355171873</v>
+      </c>
+      <c r="E150" s="7"/>
+      <c r="F150" s="13">
+        <f>AVERAGE(F119:F148)</f>
+        <v>0.12626248149128086</v>
+      </c>
+      <c r="G150" s="13">
+        <f>AVERAGE(G119:G148)</f>
+        <v>0.19600730113449957</v>
+      </c>
+      <c r="H150" s="13">
+        <f>AVERAGE(H119:H148)</f>
+        <v>1.6013830574925039</v>
+      </c>
+      <c r="I150" s="7"/>
+      <c r="J150" s="7">
+        <f>AVERAGE(J119:J148)</f>
+        <v>0.40090916299244611</v>
+      </c>
+      <c r="K150" s="7">
+        <f>AVERAGE(K119:K148)</f>
+        <v>4.3864152256705893</v>
+      </c>
+      <c r="L150" s="7">
+        <f>AVERAGE(L119:L148)</f>
+        <v>102.44028014327277</v>
+      </c>
+      <c r="M150" s="7"/>
+      <c r="N150" s="7">
+        <f>AVERAGE(N119:N148)</f>
+        <v>-1.0316284534898694</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="16">
+    <mergeCell ref="A117:D117"/>
+    <mergeCell ref="E117:H117"/>
+    <mergeCell ref="I117:L117"/>
+    <mergeCell ref="M117:N117"/>
     <mergeCell ref="A79:D79"/>
     <mergeCell ref="E79:H79"/>
     <mergeCell ref="I79:L79"/>

</xml_diff>

<commit_message>
Restart Hill Climbing in order to have graphic for Rastrigin minimum
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -461,693 +461,8 @@
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>HillClimbing</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$P$58:$P$162</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="105"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>43</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>56</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>62</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>72</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>74</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>76</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>87</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>104</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>111</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>124</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>133</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>138</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>140</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>147</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>152</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>162</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>175</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>180</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>182</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>186</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>192</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>198</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>201</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>204</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>209</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>211</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>217</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>219</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>221</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>227</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>229</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>241</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>244</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>246</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>258</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>262</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>269</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>271</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>284</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>289</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>295</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>298</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>301</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>323</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>347</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>368</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>375</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>384</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>395</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>416</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>421</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>427</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>461</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>465</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>476</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>479</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>496</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>505</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>515</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>520</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>525</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>543</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>561</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>576</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>603</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>634</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>648</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>651</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>710</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>731</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>733</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>745</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>785</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>790</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>814</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>818</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>849</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>901</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>943</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>954</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>981</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>1020</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>1144</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>1326</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>1407</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$Q$58:$Q$162</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="105"/>
-                <c:pt idx="0">
-                  <c:v>534.38676939410698</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>511.35478949163701</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>496.60817697231801</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>495.47418135194903</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>495.46090765926999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>482.83606530139701</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>467.70101011858299</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>466.98608048052</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>462.63177579325497</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>445.20613359179498</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>426.88033729756501</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>424.27255895189103</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>415.669118579447</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>405.77750714438002</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>405.04775497140901</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>398.57468521407702</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>394.97325405522503</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>394.632341505125</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>383.039094209658</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>373.18058309271601</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>373.10850638550897</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>364.72382791764301</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>361.35153184937002</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>357.24204363587398</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>354.90407109683599</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>337.80434090511699</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>334.37815211151099</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>333.67386199482502</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>333.46559177087698</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>333.225558931563</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>308.23531573979301</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>307.50528127142201</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>287.60307504328898</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>287.05362691868299</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>283.96868817554503</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>279.10713057950301</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>278.89259680819401</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>278.77273842378003</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>276.34595201453101</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>275.99258890799803</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>260.78383648646798</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>260.02641540641503</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>259.29731053315601</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>250.48182381784</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>230.68629280871201</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>230.544235986812</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>230.53727039002001</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>230.43485569230501</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>221.456723749448</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>217.79305681861899</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>216.36544986513701</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>215.268557495701</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>204.06301720437401</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>202.39065742268801</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>201.34612070822701</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>199.74276013230599</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>199.40906530867099</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>198.12623909844501</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>197.603178858185</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>196.78985929328999</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>195.66055436577599</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>184.33799192277201</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>183.798919157028</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>181.24544189678301</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>164.89428043405499</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>163.40797727202801</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>162.85730176921101</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>162.23930418114301</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>161.33579992398899</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>140.355863568052</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>129.676698595809</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>129.431162336326</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>129.22705091280301</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>129.108036873868</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>123.158776373419</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>118.92953077714699</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>115.438556068355</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>111.774889137526</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>108.111222206698</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>108.039974879228</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>103.178417283187</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>102.01386957946799</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>98.943107862214703</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>98.871860534744798</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>98.209729776593704</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>98.107315078879097</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>97.988301039943593</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>86.968276906884796</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>86.565780812035399</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>83.935430951605795</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>82.883186729377101</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>79.996944612326104</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>79.648737387694595</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>79.577490060224704</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>79.149080373024205</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>78.345238308432101</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>78.203181486532202</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>78.186911126288294</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>77.568913538220798</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>76.5044700682067</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>76.123409911047503</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>76.052162583577598</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>75.339855231598705</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>74.944960763177704</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>74.873713435707899</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-878C-4C8E-9828-EC3D5CC2C246}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
           <c:tx>
             <c:v>Genetic Alg.</c:v>
           </c:tx>
@@ -1676,7 +991,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="1"/>
           <c:tx>
             <c:v>Hybrid Alg.</c:v>
           </c:tx>
@@ -2103,7 +1418,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
-          <c:order val="3"/>
+          <c:order val="2"/>
           <c:tx>
             <c:v>PSO</c:v>
           </c:tx>
@@ -6299,6 +5614,799 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000010-878C-4C8E-9828-EC3D5CC2C246}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Hill Climbing Alg.</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$P$58:$P$180</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="123"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>141</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>147</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>157</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>161</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>172</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>174</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>177</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>199</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>204</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>223</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>235</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>261</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>267</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>278</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>285</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>314</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>316</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>323</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>349</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>363</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>368</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>378</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>392</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>402</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>405</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>433</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>448</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>454</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>473</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>486</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>490</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>493</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>513</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>522</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>532</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>537</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>556</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>567</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>603</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>627</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>637</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>643</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>679</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>685</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>692</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>711</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>727</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>745</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>810</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>823</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>905</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>992</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>1009</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>1077</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>1097</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>1157</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>1161</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>1191</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>1320</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>1348</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>1601</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>1854</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>1971</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>2049</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>2271</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>66698</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>221684</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>221717</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>221721</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>221736</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>221738</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>221798</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>221802</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>221967</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>222101</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>222352</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$Q$58:$Q$180</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="123"/>
+                <c:pt idx="0">
+                  <c:v>636.40892204701004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>619.89933217810994</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>600.86038138603305</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>585.25444455179195</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>581.55369947020995</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>565.40814477792503</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>565.39187441768104</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>561.78670249545905</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>552.76212462777903</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>545.45108508953501</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>542.52071706981599</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>541.61241908692296</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>526.35922953298302</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>505.88835807549998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>501.11502428491599</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>492.25949948448499</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>468.52490929633097</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>447.017204146469</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>439.203332323908</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>438.96851007814001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>422.61734861541203</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>422.55187808982902</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>417.56781447117402</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>400.89455890896397</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>394.685631765567</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>388.631076259471</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>386.42773508500898</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>382.28891685580697</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>375.24977736505201</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>372.792696253543</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>362.15377560980602</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>348.02404647775001</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>337.66573545539399</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>334.674407701029</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>301.52069106782602</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>279.53982741900302</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>275.75914149298598</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>273.76641998935798</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>272.06959455058802</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>261.39042957834403</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>261.02447628597201</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>260.621399981092</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>258.20301874418402</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>252.24340388661</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>235.12376765484001</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>227.610312651046</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>227.269400100947</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>223.040154504676</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>222.82562073336601</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>221.91555447055501</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>219.63021415703301</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>219.422815277273</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>219.06504047900199</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>217.90049277528399</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>215.72273005096</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>214.23642688893301</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>209.404011568584</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>201.29854545648399</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>199.79524417330799</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>192.51284020534999</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>192.19964828664601</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>182.52607969821801</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>181.521368043747</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>181.50509768350301</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>178.689101840192</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>178.402787878673</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>177.852112375856</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>177.61207953654099</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>177.18366984934099</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>172.95442425306899</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>171.67497879571499</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>162.477466298938</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>142.010280321084</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>140.88346901981399</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>140.812221692344</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>134.98706239743501</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>134.91581506996499</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>131.602363507478</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>130.69885925032401</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>129.507122823586</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>115.005308387729</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>114.19198882283401</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>113.23706170102901</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>112.68638619821201</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>109.139676059664</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>105.64870135087099</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>105.25380688244999</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>104.87526848343801</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>104.020134435938</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>103.82229803444</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>101.167103576019</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>99.261160862737398</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>98.710485359920099</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>96.080135499490595</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>93.193893382439597</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>92.738770464522105</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>91.835266207367994</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>91.454206050208796</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>89.486666068736199</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>85.8229991379079</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>82.332024429115194</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>81.950964271955996</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>79.064722154904899</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>78.993474827435094</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>78.612414670275896</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>76.248931850500099</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>75.445089785907996</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>75.428819425664102</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>74.364375955650104</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>73.956443648235407</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>73.596199369928996</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>73.524952042459105</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>72.604876843816299</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>70.673273963682703</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>68.042924103253199</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>65.768640015449506</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>62.1049730846212</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>61.710078616200299</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>61.693808255956398</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>59.330325436180601</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>59.259078108710803</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>59.187830781240898</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>58.9899943797435</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4814-492D-AC84-882BBCB608F4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -7485,8 +7593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W748"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N31" workbookViewId="0">
-      <selection activeCell="U334" sqref="U334"/>
+    <sheetView tabSelected="1" topLeftCell="K38" workbookViewId="0">
+      <selection activeCell="P180" sqref="P180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -10048,7 +10156,7 @@
         <v>2</v>
       </c>
       <c r="Q58">
-        <v>534.38676939410698</v>
+        <v>636.40892204701004</v>
       </c>
       <c r="R58">
         <v>301</v>
@@ -10116,7 +10224,7 @@
         <v>4</v>
       </c>
       <c r="Q59">
-        <v>511.35478949163701</v>
+        <v>619.89933217810994</v>
       </c>
       <c r="R59">
         <v>602</v>
@@ -10184,7 +10292,7 @@
         <v>6</v>
       </c>
       <c r="Q60">
-        <v>496.60817697231801</v>
+        <v>600.86038138603305</v>
       </c>
       <c r="R60">
         <v>1204</v>
@@ -10252,7 +10360,7 @@
         <v>9</v>
       </c>
       <c r="Q61">
-        <v>495.47418135194903</v>
+        <v>585.25444455179195</v>
       </c>
       <c r="R61">
         <v>1806</v>
@@ -10317,10 +10425,10 @@
         <v>-0.92819829932904896</v>
       </c>
       <c r="P62">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="Q62">
-        <v>495.46090765926999</v>
+        <v>581.55369947020995</v>
       </c>
       <c r="R62">
         <v>2408</v>
@@ -10385,10 +10493,10 @@
         <v>-0.960876241570775</v>
       </c>
       <c r="P63">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="Q63">
-        <v>482.83606530139701</v>
+        <v>565.40814477792503</v>
       </c>
       <c r="R63">
         <v>3010</v>
@@ -10453,10 +10561,10 @@
         <v>-1.00543828719779</v>
       </c>
       <c r="P64">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="Q64">
-        <v>467.70101011858299</v>
+        <v>565.39187441768104</v>
       </c>
       <c r="R64">
         <v>3311</v>
@@ -10521,10 +10629,10 @@
         <v>-0.86418286331758098</v>
       </c>
       <c r="P65">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="Q65">
-        <v>466.98608048052</v>
+        <v>561.78670249545905</v>
       </c>
       <c r="R65">
         <v>8428</v>
@@ -10589,10 +10697,10 @@
         <v>-0.94908760578451501</v>
       </c>
       <c r="P66">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="Q66">
-        <v>462.63177579325497</v>
+        <v>552.76212462777903</v>
       </c>
       <c r="R66">
         <v>9632</v>
@@ -10657,10 +10765,10 @@
         <v>-1.0214628289423</v>
       </c>
       <c r="P67">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="Q67">
-        <v>445.20613359179498</v>
+        <v>545.45108508953501</v>
       </c>
       <c r="R67">
         <v>10234</v>
@@ -10725,10 +10833,10 @@
         <v>-0.61134762931110698</v>
       </c>
       <c r="P68">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="Q68">
-        <v>426.88033729756501</v>
+        <v>542.52071706981599</v>
       </c>
       <c r="R68">
         <v>10836</v>
@@ -10793,10 +10901,10 @@
         <v>-0.97056248757917196</v>
       </c>
       <c r="P69">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="Q69">
-        <v>424.27255895189103</v>
+        <v>541.61241908692296</v>
       </c>
       <c r="R69">
         <v>11137</v>
@@ -10861,10 +10969,10 @@
         <v>-0.826111789721649</v>
       </c>
       <c r="P70">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="Q70">
-        <v>415.669118579447</v>
+        <v>526.35922953298302</v>
       </c>
       <c r="R70">
         <v>15652</v>
@@ -10929,10 +11037,10 @@
         <v>-0.847201280810438</v>
       </c>
       <c r="P71">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="Q71">
-        <v>405.77750714438002</v>
+        <v>505.88835807549998</v>
       </c>
       <c r="R71">
         <v>15953</v>
@@ -10997,10 +11105,10 @@
         <v>-0.82688911268558496</v>
       </c>
       <c r="P72">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="Q72">
-        <v>405.04775497140901</v>
+        <v>501.11502428491599</v>
       </c>
       <c r="R72">
         <v>18060</v>
@@ -11069,10 +11177,10 @@
         <v>0.13063988803178894</v>
       </c>
       <c r="P73">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="Q73">
-        <v>398.57468521407702</v>
+        <v>492.25949948448499</v>
       </c>
       <c r="R73">
         <v>18662</v>
@@ -11141,10 +11249,10 @@
         <v>-0.88030405655166488</v>
       </c>
       <c r="P74">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="Q74">
-        <v>394.97325405522503</v>
+        <v>468.52490929633097</v>
       </c>
       <c r="R74">
         <v>21070</v>
@@ -11167,10 +11275,10 @@
     </row>
     <row r="75" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="P75">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="Q75">
-        <v>394.632341505125</v>
+        <v>447.017204146469</v>
       </c>
       <c r="R75">
         <v>22876</v>
@@ -11193,10 +11301,10 @@
     </row>
     <row r="76" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="P76">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="Q76">
-        <v>383.039094209658</v>
+        <v>439.203332323908</v>
       </c>
       <c r="R76">
         <v>27692</v>
@@ -11232,10 +11340,10 @@
       <c r="I77" s="10"/>
       <c r="J77" s="10"/>
       <c r="P77">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="Q77">
-        <v>373.18058309271601</v>
+        <v>438.96851007814001</v>
       </c>
       <c r="R77">
         <v>27993</v>
@@ -11258,10 +11366,10 @@
     </row>
     <row r="78" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="P78">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="Q78">
-        <v>373.10850638550897</v>
+        <v>422.61734861541203</v>
       </c>
       <c r="R78">
         <v>28294</v>
@@ -11306,10 +11414,10 @@
       </c>
       <c r="N79" s="18"/>
       <c r="P79">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="Q79">
-        <v>364.72382791764301</v>
+        <v>422.55187808982902</v>
       </c>
       <c r="R79">
         <v>28595</v>
@@ -11374,10 +11482,10 @@
         <v>2</v>
       </c>
       <c r="P80">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="Q80">
-        <v>361.35153184937002</v>
+        <v>417.56781447117402</v>
       </c>
       <c r="R80">
         <v>45451</v>
@@ -11442,10 +11550,10 @@
         <v>-0.99511469963927401</v>
       </c>
       <c r="P81">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="Q81">
-        <v>357.24204363587398</v>
+        <v>400.89455890896397</v>
       </c>
       <c r="R81">
         <v>50568</v>
@@ -11510,10 +11618,10 @@
         <v>-1.02781076098617</v>
       </c>
       <c r="P82">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="Q82">
-        <v>354.90407109683599</v>
+        <v>394.685631765567</v>
       </c>
       <c r="R82">
         <v>51772</v>
@@ -11578,10 +11686,10 @@
         <v>-1.0292333137148999</v>
       </c>
       <c r="P83">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="Q83">
-        <v>337.80434090511699</v>
+        <v>388.631076259471</v>
       </c>
       <c r="R83">
         <v>52675</v>
@@ -11646,10 +11754,10 @@
         <v>-1.02992784328481</v>
       </c>
       <c r="P84">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="Q84">
-        <v>334.37815211151099</v>
+        <v>386.42773508500898</v>
       </c>
       <c r="R84">
         <v>57190</v>
@@ -11717,7 +11825,7 @@
         <v>104</v>
       </c>
       <c r="Q85">
-        <v>333.67386199482502</v>
+        <v>382.28891685580697</v>
       </c>
       <c r="R85">
         <v>58394</v>
@@ -11782,10 +11890,10 @@
         <v>-1.02992784328481</v>
       </c>
       <c r="P86">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="Q86">
-        <v>333.46559177087698</v>
+        <v>375.24977736505201</v>
       </c>
       <c r="R86">
         <v>58695</v>
@@ -11850,10 +11958,10 @@
         <v>-1.0292333137148999</v>
       </c>
       <c r="P87">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="Q87">
-        <v>333.225558931563</v>
+        <v>372.792696253543</v>
       </c>
       <c r="R87">
         <v>59297</v>
@@ -11918,10 +12026,10 @@
         <v>-1.02781076098617</v>
       </c>
       <c r="P88">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="Q88">
-        <v>308.23531573979301</v>
+        <v>362.15377560980602</v>
       </c>
       <c r="R88">
         <v>60501</v>
@@ -11986,10 +12094,10 @@
         <v>-1.02781076098617</v>
       </c>
       <c r="P89">
-        <v>138</v>
+        <v>118</v>
       </c>
       <c r="Q89">
-        <v>307.50528127142201</v>
+        <v>348.02404647775001</v>
       </c>
       <c r="R89">
         <v>61103</v>
@@ -12054,10 +12162,10 @@
         <v>-1.03124356431136</v>
       </c>
       <c r="P90">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="Q90">
-        <v>287.60307504328898</v>
+        <v>337.66573545539399</v>
       </c>
       <c r="R90">
         <v>61404</v>
@@ -12122,10 +12230,10 @@
         <v>-1.03124356431136</v>
       </c>
       <c r="P91">
-        <v>147</v>
+        <v>128</v>
       </c>
       <c r="Q91">
-        <v>287.05362691868299</v>
+        <v>334.674407701029</v>
       </c>
       <c r="R91">
         <v>62608</v>
@@ -12190,10 +12298,10 @@
         <v>-1.02732441138881</v>
       </c>
       <c r="P92">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="Q92">
-        <v>283.96868817554503</v>
+        <v>301.52069106782602</v>
       </c>
       <c r="R92">
         <v>63511</v>
@@ -12258,10 +12366,10 @@
         <v>-1.03124356431136</v>
       </c>
       <c r="P93">
-        <v>162</v>
+        <v>144</v>
       </c>
       <c r="Q93">
-        <v>279.10713057950301</v>
+        <v>279.53982741900302</v>
       </c>
       <c r="R93">
         <v>63812</v>
@@ -12326,10 +12434,10 @@
         <v>-0.99511469963927401</v>
       </c>
       <c r="P94">
-        <v>175</v>
+        <v>147</v>
       </c>
       <c r="Q94">
-        <v>278.89259680819401</v>
+        <v>275.75914149298598</v>
       </c>
       <c r="R94">
         <v>65016</v>
@@ -12394,10 +12502,10 @@
         <v>-0.99511469963927401</v>
       </c>
       <c r="P95">
-        <v>180</v>
+        <v>155</v>
       </c>
       <c r="Q95">
-        <v>278.77273842378003</v>
+        <v>273.76641998935798</v>
       </c>
       <c r="R95">
         <v>67123</v>
@@ -12462,10 +12570,10 @@
         <v>-1.02781076098617</v>
       </c>
       <c r="P96">
-        <v>182</v>
+        <v>157</v>
       </c>
       <c r="Q96">
-        <v>276.34595201453101</v>
+        <v>272.06959455058802</v>
       </c>
       <c r="R96">
         <v>69230</v>
@@ -12530,10 +12638,10 @@
         <v>-1.0308900958220399</v>
       </c>
       <c r="P97">
-        <v>186</v>
+        <v>159</v>
       </c>
       <c r="Q97">
-        <v>275.99258890799803</v>
+        <v>261.39042957834403</v>
       </c>
       <c r="R97">
         <v>73444</v>
@@ -12598,10 +12706,10 @@
         <v>-1.02781076098617</v>
       </c>
       <c r="P98">
-        <v>192</v>
+        <v>161</v>
       </c>
       <c r="Q98">
-        <v>260.78383648646798</v>
+        <v>261.02447628597201</v>
       </c>
       <c r="R98">
         <v>75852</v>
@@ -12666,10 +12774,10 @@
         <v>-0.99511469963927401</v>
       </c>
       <c r="P99">
-        <v>198</v>
+        <v>172</v>
       </c>
       <c r="Q99">
-        <v>260.02641540641503</v>
+        <v>260.621399981092</v>
       </c>
       <c r="R99">
         <v>76454</v>
@@ -12734,10 +12842,10 @@
         <v>-0.99550048954989001</v>
       </c>
       <c r="P100">
-        <v>201</v>
+        <v>174</v>
       </c>
       <c r="Q100">
-        <v>259.29731053315601</v>
+        <v>258.20301874418402</v>
       </c>
       <c r="R100">
         <v>78260</v>
@@ -12802,10 +12910,10 @@
         <v>-1.0292333137148999</v>
       </c>
       <c r="P101">
-        <v>204</v>
+        <v>177</v>
       </c>
       <c r="Q101">
-        <v>250.48182381784</v>
+        <v>252.24340388661</v>
       </c>
       <c r="R101">
         <v>80668</v>
@@ -12870,10 +12978,10 @@
         <v>-1.03124356431136</v>
       </c>
       <c r="P102">
-        <v>209</v>
+        <v>180</v>
       </c>
       <c r="Q102">
-        <v>230.68629280871201</v>
+        <v>235.12376765484001</v>
       </c>
       <c r="R102">
         <v>81571</v>
@@ -12938,10 +13046,10 @@
         <v>-1.02781076098617</v>
       </c>
       <c r="P103">
-        <v>211</v>
+        <v>192</v>
       </c>
       <c r="Q103">
-        <v>230.544235986812</v>
+        <v>227.610312651046</v>
       </c>
       <c r="R103">
         <v>83076</v>
@@ -13006,10 +13114,10 @@
         <v>-1.02781076098617</v>
       </c>
       <c r="P104">
-        <v>217</v>
+        <v>197</v>
       </c>
       <c r="Q104">
-        <v>230.53727039002001</v>
+        <v>227.269400100947</v>
       </c>
       <c r="R104">
         <v>84280</v>
@@ -13074,10 +13182,10 @@
         <v>-0.99511469963927401</v>
       </c>
       <c r="P105">
-        <v>219</v>
+        <v>199</v>
       </c>
       <c r="Q105">
-        <v>230.43485569230501</v>
+        <v>223.040154504676</v>
       </c>
       <c r="R105">
         <v>86989</v>
@@ -13142,10 +13250,10 @@
         <v>-1.0112694956197901</v>
       </c>
       <c r="P106">
-        <v>221</v>
+        <v>204</v>
       </c>
       <c r="Q106">
-        <v>221.456723749448</v>
+        <v>222.82562073336601</v>
       </c>
       <c r="R106">
         <v>88795</v>
@@ -13210,10 +13318,10 @@
         <v>-1.03124356431136</v>
       </c>
       <c r="P107">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="Q107">
-        <v>217.79305681861899</v>
+        <v>221.91555447055501</v>
       </c>
       <c r="R107">
         <v>89397</v>
@@ -13278,10 +13386,10 @@
         <v>-1.02992784328481</v>
       </c>
       <c r="P108">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="Q108">
-        <v>216.36544986513701</v>
+        <v>219.63021415703301</v>
       </c>
       <c r="R108">
         <v>92708</v>
@@ -13346,10 +13454,10 @@
         <v>-1.02373427886066</v>
       </c>
       <c r="P109">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="Q109">
-        <v>215.268557495701</v>
+        <v>219.422815277273</v>
       </c>
       <c r="R109">
         <v>93310</v>
@@ -13414,10 +13522,10 @@
         <v>-0.99511469963927401</v>
       </c>
       <c r="P110">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="Q110">
-        <v>204.06301720437401</v>
+        <v>219.06504047900199</v>
       </c>
       <c r="R110">
         <v>96922</v>
@@ -13486,10 +13594,10 @@
         <v>1.4712182888767357E-2</v>
       </c>
       <c r="P111">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="Q111">
-        <v>202.39065742268801</v>
+        <v>217.90049277528399</v>
       </c>
       <c r="R111">
         <v>98427</v>
@@ -13558,10 +13666,10 @@
         <v>-1.0205903810606922</v>
       </c>
       <c r="P112">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="Q112">
-        <v>201.34612070822701</v>
+        <v>215.72273005096</v>
       </c>
       <c r="R112">
         <v>98728</v>
@@ -13584,10 +13692,10 @@
     </row>
     <row r="113" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="P113">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="Q113">
-        <v>199.74276013230599</v>
+        <v>214.23642688893301</v>
       </c>
       <c r="R113">
         <v>101136</v>
@@ -13610,10 +13718,10 @@
     </row>
     <row r="114" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="P114">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="Q114">
-        <v>199.40906530867099</v>
+        <v>209.404011568584</v>
       </c>
       <c r="R114">
         <v>104447</v>
@@ -13649,10 +13757,10 @@
       <c r="I115" s="10"/>
       <c r="J115" s="10"/>
       <c r="P115">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="Q115">
-        <v>198.12623909844501</v>
+        <v>201.29854545648399</v>
       </c>
       <c r="R115">
         <v>105651</v>
@@ -13675,10 +13783,10 @@
     </row>
     <row r="116" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="P116">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="Q116">
-        <v>197.603178858185</v>
+        <v>199.79524417330799</v>
       </c>
       <c r="R116">
         <v>108059</v>
@@ -13723,10 +13831,10 @@
       </c>
       <c r="N117" s="18"/>
       <c r="P117">
-        <v>289</v>
+        <v>314</v>
       </c>
       <c r="Q117">
-        <v>196.78985929328999</v>
+        <v>192.51284020534999</v>
       </c>
       <c r="R117">
         <v>108661</v>
@@ -13791,10 +13899,10 @@
         <v>2</v>
       </c>
       <c r="P118">
-        <v>295</v>
+        <v>316</v>
       </c>
       <c r="Q118">
-        <v>195.66055436577599</v>
+        <v>192.19964828664601</v>
       </c>
       <c r="R118">
         <v>120099</v>
@@ -13859,10 +13967,10 @@
         <v>-1.0316284534898701</v>
       </c>
       <c r="P119">
-        <v>298</v>
+        <v>320</v>
       </c>
       <c r="Q119">
-        <v>184.33799192277201</v>
+        <v>182.52607969821801</v>
       </c>
       <c r="R119">
         <v>147189</v>
@@ -13927,10 +14035,10 @@
         <v>-1.0316284534898701</v>
       </c>
       <c r="P120">
-        <v>301</v>
+        <v>323</v>
       </c>
       <c r="Q120">
-        <v>183.798919157028</v>
+        <v>181.521368043747</v>
       </c>
       <c r="R120">
         <v>155015</v>
@@ -13989,10 +14097,10 @@
         <v>-1.0316284534898701</v>
       </c>
       <c r="P121">
-        <v>323</v>
+        <v>349</v>
       </c>
       <c r="Q121">
-        <v>181.24544189678301</v>
+        <v>181.50509768350301</v>
       </c>
       <c r="R121">
         <v>155316</v>
@@ -14051,10 +14159,10 @@
         <v>-1.0316284534898701</v>
       </c>
       <c r="P122">
-        <v>347</v>
+        <v>363</v>
       </c>
       <c r="Q122">
-        <v>164.89428043405499</v>
+        <v>178.689101840192</v>
       </c>
       <c r="R122">
         <v>168560</v>
@@ -14116,7 +14224,7 @@
         <v>368</v>
       </c>
       <c r="Q123">
-        <v>163.40797727202801</v>
+        <v>178.402787878673</v>
       </c>
       <c r="R123">
         <v>168861</v>
@@ -14175,10 +14283,10 @@
         <v>-1.0316284534898701</v>
       </c>
       <c r="P124">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="Q124">
-        <v>162.85730176921101</v>
+        <v>177.852112375856</v>
       </c>
       <c r="R124">
         <v>180600</v>
@@ -14237,10 +14345,10 @@
         <v>-1.0316284534898701</v>
       </c>
       <c r="P125">
-        <v>384</v>
+        <v>392</v>
       </c>
       <c r="Q125">
-        <v>162.23930418114301</v>
+        <v>177.61207953654099</v>
       </c>
       <c r="R125">
         <v>200466</v>
@@ -14299,10 +14407,10 @@
         <v>-1.0316284534898701</v>
       </c>
       <c r="P126">
-        <v>395</v>
+        <v>400</v>
       </c>
       <c r="Q126">
-        <v>161.33579992398899</v>
+        <v>177.18366984934099</v>
       </c>
       <c r="R126">
         <v>201971</v>
@@ -14361,10 +14469,10 @@
         <v>-1.0316284534898701</v>
       </c>
       <c r="P127">
-        <v>416</v>
+        <v>402</v>
       </c>
       <c r="Q127">
-        <v>140.355863568052</v>
+        <v>172.95442425306899</v>
       </c>
       <c r="R127">
         <v>202573</v>
@@ -14423,10 +14531,10 @@
         <v>-1.0316284534898701</v>
       </c>
       <c r="P128">
-        <v>421</v>
+        <v>405</v>
       </c>
       <c r="Q128">
-        <v>129.676698595809</v>
+        <v>171.67497879571499</v>
       </c>
       <c r="R128">
         <v>207088</v>
@@ -14485,10 +14593,10 @@
         <v>-1.0316284534898701</v>
       </c>
       <c r="P129">
-        <v>427</v>
+        <v>433</v>
       </c>
       <c r="Q129">
-        <v>129.431162336326</v>
+        <v>162.477466298938</v>
       </c>
       <c r="R129">
         <v>233877</v>
@@ -14547,10 +14655,10 @@
         <v>-1.0316284534898701</v>
       </c>
       <c r="P130">
-        <v>461</v>
+        <v>448</v>
       </c>
       <c r="Q130">
-        <v>129.22705091280301</v>
+        <v>142.010280321084</v>
       </c>
       <c r="R130">
         <v>234178</v>
@@ -14609,10 +14717,10 @@
         <v>-1.0316284534898701</v>
       </c>
       <c r="P131">
-        <v>465</v>
+        <v>454</v>
       </c>
       <c r="Q131">
-        <v>129.108036873868</v>
+        <v>140.88346901981399</v>
       </c>
       <c r="R131">
         <v>237188</v>
@@ -14671,10 +14779,10 @@
         <v>-1.0316284534898701</v>
       </c>
       <c r="P132">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="Q132">
-        <v>123.158776373419</v>
+        <v>140.812221692344</v>
       </c>
       <c r="R132">
         <v>240198</v>
@@ -14733,10 +14841,10 @@
         <v>-1.0316284534898701</v>
       </c>
       <c r="P133">
-        <v>479</v>
+        <v>486</v>
       </c>
       <c r="Q133">
-        <v>118.92953077714699</v>
+        <v>134.98706239743501</v>
       </c>
       <c r="R133">
         <v>240800</v>
@@ -14795,10 +14903,10 @@
         <v>-1.0316284534898701</v>
       </c>
       <c r="P134">
-        <v>496</v>
+        <v>490</v>
       </c>
       <c r="Q134">
-        <v>115.438556068355</v>
+        <v>134.91581506996499</v>
       </c>
       <c r="R134">
         <v>253743</v>
@@ -14857,10 +14965,10 @@
         <v>-1.0316284534898701</v>
       </c>
       <c r="P135">
-        <v>505</v>
+        <v>493</v>
       </c>
       <c r="Q135">
-        <v>111.774889137526</v>
+        <v>131.602363507478</v>
       </c>
       <c r="R135">
         <v>254044</v>
@@ -14919,10 +15027,10 @@
         <v>-1.0316284534898701</v>
       </c>
       <c r="P136">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="Q136">
-        <v>108.111222206698</v>
+        <v>130.69885925032401</v>
       </c>
       <c r="R136">
         <v>255850</v>
@@ -14981,10 +15089,10 @@
         <v>-1.0316284534898701</v>
       </c>
       <c r="P137">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="Q137">
-        <v>108.039974879228</v>
+        <v>129.507122823586</v>
       </c>
       <c r="V137">
         <v>33300</v>
@@ -15037,10 +15145,10 @@
         <v>-1.0316284534898701</v>
       </c>
       <c r="P138">
-        <v>525</v>
+        <v>532</v>
       </c>
       <c r="Q138">
-        <v>103.178417283187</v>
+        <v>115.005308387729</v>
       </c>
       <c r="V138">
         <v>33400</v>
@@ -15093,10 +15201,10 @@
         <v>-1.0316284534898701</v>
       </c>
       <c r="P139">
-        <v>543</v>
+        <v>537</v>
       </c>
       <c r="Q139">
-        <v>102.01386957946799</v>
+        <v>114.19198882283401</v>
       </c>
       <c r="V139">
         <v>33500</v>
@@ -15149,10 +15257,10 @@
         <v>-1.0316284534898701</v>
       </c>
       <c r="P140">
-        <v>561</v>
+        <v>556</v>
       </c>
       <c r="Q140">
-        <v>98.943107862214703</v>
+        <v>113.23706170102901</v>
       </c>
       <c r="V140">
         <v>33600</v>
@@ -15205,10 +15313,10 @@
         <v>-1.0316284534898701</v>
       </c>
       <c r="P141">
-        <v>576</v>
+        <v>567</v>
       </c>
       <c r="Q141">
-        <v>98.871860534744798</v>
+        <v>112.68638619821201</v>
       </c>
       <c r="V141">
         <v>33800</v>
@@ -15264,7 +15372,7 @@
         <v>603</v>
       </c>
       <c r="Q142">
-        <v>98.209729776593704</v>
+        <v>109.139676059664</v>
       </c>
       <c r="V142">
         <v>34000</v>
@@ -15317,10 +15425,10 @@
         <v>-1.0316284534898701</v>
       </c>
       <c r="P143">
-        <v>634</v>
+        <v>627</v>
       </c>
       <c r="Q143">
-        <v>98.107315078879097</v>
+        <v>105.64870135087099</v>
       </c>
       <c r="V143">
         <v>34100</v>
@@ -15373,10 +15481,10 @@
         <v>-1.0316284534898701</v>
       </c>
       <c r="P144">
-        <v>648</v>
+        <v>637</v>
       </c>
       <c r="Q144">
-        <v>97.988301039943593</v>
+        <v>105.25380688244999</v>
       </c>
       <c r="V144">
         <v>34200</v>
@@ -15429,10 +15537,10 @@
         <v>-1.0316284534898701</v>
       </c>
       <c r="P145">
-        <v>651</v>
+        <v>643</v>
       </c>
       <c r="Q145">
-        <v>86.968276906884796</v>
+        <v>104.87526848343801</v>
       </c>
       <c r="V145">
         <v>34300</v>
@@ -15485,10 +15593,10 @@
         <v>-1.0316284534898701</v>
       </c>
       <c r="P146">
-        <v>710</v>
+        <v>679</v>
       </c>
       <c r="Q146">
-        <v>86.565780812035399</v>
+        <v>104.020134435938</v>
       </c>
       <c r="V146">
         <v>34400</v>
@@ -15541,10 +15649,10 @@
         <v>-1.0316284534898701</v>
       </c>
       <c r="P147">
-        <v>731</v>
+        <v>685</v>
       </c>
       <c r="Q147">
-        <v>83.935430951605795</v>
+        <v>103.82229803444</v>
       </c>
       <c r="V147">
         <v>34500</v>
@@ -15597,10 +15705,10 @@
         <v>-1.0316284534898701</v>
       </c>
       <c r="P148">
-        <v>733</v>
+        <v>692</v>
       </c>
       <c r="Q148">
-        <v>82.883186729377101</v>
+        <v>101.167103576019</v>
       </c>
       <c r="V148">
         <v>34600</v>
@@ -15657,10 +15765,10 @@
         <v>6.7752154249004421E-16</v>
       </c>
       <c r="P149">
-        <v>745</v>
+        <v>711</v>
       </c>
       <c r="Q149">
-        <v>79.996944612326104</v>
+        <v>99.261160862737398</v>
       </c>
       <c r="V149">
         <v>34700</v>
@@ -15717,10 +15825,10 @@
         <v>-1.0316284534898694</v>
       </c>
       <c r="P150">
-        <v>785</v>
+        <v>727</v>
       </c>
       <c r="Q150">
-        <v>79.648737387694595</v>
+        <v>98.710485359920099</v>
       </c>
       <c r="V150">
         <v>34900</v>
@@ -15731,10 +15839,10 @@
     </row>
     <row r="151" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="P151">
-        <v>790</v>
+        <v>745</v>
       </c>
       <c r="Q151">
-        <v>79.577490060224704</v>
+        <v>96.080135499490595</v>
       </c>
       <c r="V151">
         <v>35000</v>
@@ -15745,10 +15853,10 @@
     </row>
     <row r="152" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="P152">
-        <v>814</v>
+        <v>810</v>
       </c>
       <c r="Q152">
-        <v>79.149080373024205</v>
+        <v>93.193893382439597</v>
       </c>
       <c r="V152">
         <v>35100</v>
@@ -15759,10 +15867,10 @@
     </row>
     <row r="153" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="P153">
-        <v>818</v>
+        <v>823</v>
       </c>
       <c r="Q153">
-        <v>78.345238308432101</v>
+        <v>92.738770464522105</v>
       </c>
       <c r="V153">
         <v>35200</v>
@@ -15773,10 +15881,10 @@
     </row>
     <row r="154" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="P154">
-        <v>849</v>
+        <v>905</v>
       </c>
       <c r="Q154">
-        <v>78.203181486532202</v>
+        <v>91.835266207367994</v>
       </c>
       <c r="V154">
         <v>35300</v>
@@ -15787,10 +15895,10 @@
     </row>
     <row r="155" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="P155">
-        <v>901</v>
+        <v>992</v>
       </c>
       <c r="Q155">
-        <v>78.186911126288294</v>
+        <v>91.454206050208796</v>
       </c>
       <c r="V155">
         <v>35400</v>
@@ -15801,10 +15909,10 @@
     </row>
     <row r="156" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="P156">
-        <v>943</v>
+        <v>1009</v>
       </c>
       <c r="Q156">
-        <v>77.568913538220798</v>
+        <v>89.486666068736199</v>
       </c>
       <c r="V156">
         <v>35500</v>
@@ -15815,10 +15923,10 @@
     </row>
     <row r="157" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="P157">
-        <v>954</v>
+        <v>1077</v>
       </c>
       <c r="Q157">
-        <v>76.5044700682067</v>
+        <v>85.8229991379079</v>
       </c>
       <c r="V157">
         <v>35600</v>
@@ -15829,10 +15937,10 @@
     </row>
     <row r="158" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="P158">
-        <v>981</v>
+        <v>1097</v>
       </c>
       <c r="Q158">
-        <v>76.123409911047503</v>
+        <v>82.332024429115194</v>
       </c>
       <c r="V158">
         <v>35700</v>
@@ -15843,10 +15951,10 @@
     </row>
     <row r="159" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="P159">
-        <v>1020</v>
+        <v>1157</v>
       </c>
       <c r="Q159">
-        <v>76.052162583577598</v>
+        <v>81.950964271955996</v>
       </c>
       <c r="V159">
         <v>35900</v>
@@ -15857,10 +15965,10 @@
     </row>
     <row r="160" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="P160">
-        <v>1144</v>
+        <v>1161</v>
       </c>
       <c r="Q160">
-        <v>75.339855231598705</v>
+        <v>79.064722154904899</v>
       </c>
       <c r="V160">
         <v>36000</v>
@@ -15871,10 +15979,10 @@
     </row>
     <row r="161" spans="16:23" x14ac:dyDescent="0.55000000000000004">
       <c r="P161">
-        <v>1326</v>
+        <v>1191</v>
       </c>
       <c r="Q161">
-        <v>74.944960763177704</v>
+        <v>78.993474827435094</v>
       </c>
       <c r="V161">
         <v>36100</v>
@@ -15885,10 +15993,10 @@
     </row>
     <row r="162" spans="16:23" x14ac:dyDescent="0.55000000000000004">
       <c r="P162">
-        <v>1407</v>
+        <v>1320</v>
       </c>
       <c r="Q162">
-        <v>74.873713435707899</v>
+        <v>78.612414670275896</v>
       </c>
       <c r="V162">
         <v>36200</v>
@@ -15898,6 +16006,12 @@
       </c>
     </row>
     <row r="163" spans="16:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="P163">
+        <v>1348</v>
+      </c>
+      <c r="Q163">
+        <v>76.248931850500099</v>
+      </c>
       <c r="V163">
         <v>36300</v>
       </c>
@@ -15906,6 +16020,12 @@
       </c>
     </row>
     <row r="164" spans="16:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="P164">
+        <v>1400</v>
+      </c>
+      <c r="Q164">
+        <v>75.445089785907996</v>
+      </c>
       <c r="V164">
         <v>36400</v>
       </c>
@@ -15914,6 +16034,12 @@
       </c>
     </row>
     <row r="165" spans="16:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="P165">
+        <v>1601</v>
+      </c>
+      <c r="Q165">
+        <v>75.428819425664102</v>
+      </c>
       <c r="V165">
         <v>36500</v>
       </c>
@@ -15922,6 +16048,12 @@
       </c>
     </row>
     <row r="166" spans="16:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="P166">
+        <v>1854</v>
+      </c>
+      <c r="Q166">
+        <v>74.364375955650104</v>
+      </c>
       <c r="V166">
         <v>36600</v>
       </c>
@@ -15930,6 +16062,12 @@
       </c>
     </row>
     <row r="167" spans="16:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="P167">
+        <v>1971</v>
+      </c>
+      <c r="Q167">
+        <v>73.956443648235407</v>
+      </c>
       <c r="V167">
         <v>36700</v>
       </c>
@@ -15938,6 +16076,12 @@
       </c>
     </row>
     <row r="168" spans="16:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="P168">
+        <v>2049</v>
+      </c>
+      <c r="Q168">
+        <v>73.596199369928996</v>
+      </c>
       <c r="V168">
         <v>36800</v>
       </c>
@@ -15946,6 +16090,12 @@
       </c>
     </row>
     <row r="169" spans="16:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="P169">
+        <v>2271</v>
+      </c>
+      <c r="Q169">
+        <v>73.524952042459105</v>
+      </c>
       <c r="V169">
         <v>36900</v>
       </c>
@@ -15954,6 +16104,12 @@
       </c>
     </row>
     <row r="170" spans="16:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="P170">
+        <v>66698</v>
+      </c>
+      <c r="Q170">
+        <v>72.604876843816299</v>
+      </c>
       <c r="V170">
         <v>37100</v>
       </c>
@@ -15962,6 +16118,12 @@
       </c>
     </row>
     <row r="171" spans="16:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="P171">
+        <v>221684</v>
+      </c>
+      <c r="Q171">
+        <v>70.673273963682703</v>
+      </c>
       <c r="V171">
         <v>37200</v>
       </c>
@@ -15970,6 +16132,12 @@
       </c>
     </row>
     <row r="172" spans="16:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="P172">
+        <v>221717</v>
+      </c>
+      <c r="Q172">
+        <v>68.042924103253199</v>
+      </c>
       <c r="V172">
         <v>37300</v>
       </c>
@@ -15978,6 +16146,12 @@
       </c>
     </row>
     <row r="173" spans="16:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="P173">
+        <v>221721</v>
+      </c>
+      <c r="Q173">
+        <v>65.768640015449506</v>
+      </c>
       <c r="V173">
         <v>37600</v>
       </c>
@@ -15986,6 +16160,12 @@
       </c>
     </row>
     <row r="174" spans="16:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="P174">
+        <v>221736</v>
+      </c>
+      <c r="Q174">
+        <v>62.1049730846212</v>
+      </c>
       <c r="V174">
         <v>37700</v>
       </c>
@@ -15994,6 +16174,12 @@
       </c>
     </row>
     <row r="175" spans="16:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="P175">
+        <v>221738</v>
+      </c>
+      <c r="Q175">
+        <v>61.710078616200299</v>
+      </c>
       <c r="V175">
         <v>37800</v>
       </c>
@@ -16002,6 +16188,12 @@
       </c>
     </row>
     <row r="176" spans="16:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="P176">
+        <v>221798</v>
+      </c>
+      <c r="Q176">
+        <v>61.693808255956398</v>
+      </c>
       <c r="V176">
         <v>37900</v>
       </c>
@@ -16009,7 +16201,13 @@
         <v>30.278916276151602</v>
       </c>
     </row>
-    <row r="177" spans="22:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="177" spans="16:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="P177">
+        <v>221802</v>
+      </c>
+      <c r="Q177">
+        <v>59.330325436180601</v>
+      </c>
       <c r="V177">
         <v>38000</v>
       </c>
@@ -16017,7 +16215,13 @@
         <v>30.2376470216036</v>
       </c>
     </row>
-    <row r="178" spans="22:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="178" spans="16:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="P178">
+        <v>221967</v>
+      </c>
+      <c r="Q178">
+        <v>59.259078108710803</v>
+      </c>
       <c r="V178">
         <v>38100</v>
       </c>
@@ -16025,7 +16229,13 @@
         <v>30.116283111097399</v>
       </c>
     </row>
-    <row r="179" spans="22:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="179" spans="16:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="P179">
+        <v>222101</v>
+      </c>
+      <c r="Q179">
+        <v>59.187830781240898</v>
+      </c>
       <c r="V179">
         <v>38200</v>
       </c>
@@ -16033,7 +16243,13 @@
         <v>30.063329461795998</v>
       </c>
     </row>
-    <row r="180" spans="22:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="180" spans="16:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="P180">
+        <v>222352</v>
+      </c>
+      <c r="Q180">
+        <v>58.9899943797435</v>
+      </c>
       <c r="V180">
         <v>38300</v>
       </c>
@@ -16041,7 +16257,7 @@
         <v>29.3517141056541</v>
       </c>
     </row>
-    <row r="181" spans="22:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="181" spans="16:23" x14ac:dyDescent="0.55000000000000004">
       <c r="V181">
         <v>38400</v>
       </c>
@@ -16049,7 +16265,7 @@
         <v>29.232215579755</v>
       </c>
     </row>
-    <row r="182" spans="22:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="182" spans="16:23" x14ac:dyDescent="0.55000000000000004">
       <c r="V182">
         <v>38500</v>
       </c>
@@ -16057,7 +16273,7 @@
         <v>29.1223139291004</v>
       </c>
     </row>
-    <row r="183" spans="22:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="183" spans="16:23" x14ac:dyDescent="0.55000000000000004">
       <c r="V183">
         <v>38600</v>
       </c>
@@ -16065,7 +16281,7 @@
         <v>29.0269831421523</v>
       </c>
     </row>
-    <row r="184" spans="22:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="184" spans="16:23" x14ac:dyDescent="0.55000000000000004">
       <c r="V184">
         <v>38700</v>
       </c>
@@ -16073,7 +16289,7 @@
         <v>28.7677597390202</v>
       </c>
     </row>
-    <row r="185" spans="22:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="185" spans="16:23" x14ac:dyDescent="0.55000000000000004">
       <c r="V185">
         <v>38800</v>
       </c>
@@ -16081,7 +16297,7 @@
         <v>28.2835546282796</v>
       </c>
     </row>
-    <row r="186" spans="22:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="186" spans="16:23" x14ac:dyDescent="0.55000000000000004">
       <c r="V186">
         <v>38900</v>
       </c>
@@ -16089,7 +16305,7 @@
         <v>28.181858917892502</v>
       </c>
     </row>
-    <row r="187" spans="22:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="187" spans="16:23" x14ac:dyDescent="0.55000000000000004">
       <c r="V187">
         <v>39000</v>
       </c>
@@ -16097,7 +16313,7 @@
         <v>28.1724087975131</v>
       </c>
     </row>
-    <row r="188" spans="22:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="188" spans="16:23" x14ac:dyDescent="0.55000000000000004">
       <c r="V188">
         <v>39100</v>
       </c>
@@ -16105,7 +16321,7 @@
         <v>28.141508186689201</v>
       </c>
     </row>
-    <row r="189" spans="22:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="189" spans="16:23" x14ac:dyDescent="0.55000000000000004">
       <c r="V189">
         <v>39200</v>
       </c>
@@ -16113,7 +16329,7 @@
         <v>28.080751368128901</v>
       </c>
     </row>
-    <row r="190" spans="22:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="190" spans="16:23" x14ac:dyDescent="0.55000000000000004">
       <c r="V190">
         <v>39300</v>
       </c>
@@ -16121,7 +16337,7 @@
         <v>28.036541788891999</v>
       </c>
     </row>
-    <row r="191" spans="22:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="191" spans="16:23" x14ac:dyDescent="0.55000000000000004">
       <c r="V191">
         <v>39400</v>
       </c>
@@ -16129,7 +16345,7 @@
         <v>27.527228748652</v>
       </c>
     </row>
-    <row r="192" spans="22:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="192" spans="16:23" x14ac:dyDescent="0.55000000000000004">
       <c r="V192">
         <v>39500</v>
       </c>
@@ -20587,6 +20803,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A117:D117"/>
+    <mergeCell ref="E117:H117"/>
+    <mergeCell ref="I117:L117"/>
+    <mergeCell ref="M117:N117"/>
+    <mergeCell ref="A79:D79"/>
+    <mergeCell ref="E79:H79"/>
+    <mergeCell ref="I79:L79"/>
+    <mergeCell ref="M79:N79"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="E3:H3"/>
     <mergeCell ref="I3:L3"/>
@@ -20595,14 +20819,6 @@
     <mergeCell ref="E41:H41"/>
     <mergeCell ref="I41:L41"/>
     <mergeCell ref="M41:N41"/>
-    <mergeCell ref="A117:D117"/>
-    <mergeCell ref="E117:H117"/>
-    <mergeCell ref="I117:L117"/>
-    <mergeCell ref="M117:N117"/>
-    <mergeCell ref="A79:D79"/>
-    <mergeCell ref="E79:H79"/>
-    <mergeCell ref="I79:L79"/>
-    <mergeCell ref="M79:N79"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>